<commit_message>
add CAS, UNII, PubChem identifiers
</commit_message>
<xml_diff>
--- a/datasets/analysis_dataset.xlsx
+++ b/datasets/analysis_dataset.xlsx
@@ -4375,7 +4375,7 @@
         <v>0</v>
       </c>
       <c r="BY14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ14" s="2">
         <v>1</v>
@@ -5839,7 +5839,7 @@
         <v>0</v>
       </c>
       <c r="BY20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ20" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
add UNII, CAS, PubChem to lab detail
</commit_message>
<xml_diff>
--- a/datasets/analysis_dataset.xlsx
+++ b/datasets/analysis_dataset.xlsx
@@ -51,24 +51,24 @@
     <t>193</t>
   </si>
   <si>
+    <t>299</t>
+  </si>
+  <si>
     <t>253</t>
   </si>
   <si>
-    <t>299</t>
-  </si>
-  <si>
     <t>644</t>
   </si>
   <si>
     <t>340</t>
   </si>
   <si>
+    <t>836</t>
+  </si>
+  <si>
     <t>555</t>
   </si>
   <si>
-    <t>836</t>
-  </si>
-  <si>
     <t>408</t>
   </si>
   <si>
@@ -381,12 +381,12 @@
     <t>powder; chunky; shiny</t>
   </si>
   <si>
+    <t>fake pill</t>
+  </si>
+  <si>
     <t>crystals</t>
   </si>
   <si>
-    <t>fake pill</t>
-  </si>
-  <si>
     <t>tar</t>
   </si>
   <si>
@@ -483,10 +483,10 @@
     <t>fast acting</t>
   </si>
   <si>
+    <t>strong blues</t>
+  </si>
+  <si>
     <t>FTS = negative</t>
-  </si>
-  <si>
-    <t>strong blues</t>
   </si>
   <si>
     <t>overdose</t>
@@ -1070,7 +1070,7 @@
         <v>125</v>
       </c>
       <c r="AA1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="AB1" t="s">
         <v>126</v>
@@ -3958,28 +3958,28 @@
         <v>72</v>
       </c>
       <c r="G13" s="1">
-        <v>44707</v>
+        <v>44695</v>
       </c>
       <c r="H13" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I13" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J13" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="K13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M13" s="2">
         <v>0</v>
       </c>
       <c r="N13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O13" s="2">
         <v>0</v>
@@ -3988,7 +3988,7 @@
         <v>0</v>
       </c>
       <c r="Q13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R13" s="2">
         <v>0</v>
@@ -3997,7 +3997,7 @@
         <v>0</v>
       </c>
       <c r="T13" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="U13" s="2">
         <v>0</v>
@@ -4048,7 +4048,7 @@
         <v>0</v>
       </c>
       <c r="AU13" s="1">
-        <v>44714</v>
+        <v>44707</v>
       </c>
       <c r="AV13" s="2">
         <v>1</v>
@@ -4058,22 +4058,22 @@
       </c>
       <c r="AX13" s="2"/>
       <c r="AY13" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AZ13" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="BA13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE13" s="2">
         <v>0</v>
@@ -4085,10 +4085,10 @@
         <v>0</v>
       </c>
       <c r="BH13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ13" s="2">
         <v>0</v>
@@ -4097,7 +4097,7 @@
         <v>0</v>
       </c>
       <c r="BL13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM13" s="2">
         <v>0</v>
@@ -4121,7 +4121,7 @@
         <v>0</v>
       </c>
       <c r="BT13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BU13" s="2">
         <v>0</v>
@@ -4133,19 +4133,19 @@
         <v>0</v>
       </c>
       <c r="BX13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CA13" s="2">
         <v>0</v>
       </c>
       <c r="CB13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CC13" s="2">
         <v>0</v>
@@ -4197,28 +4197,28 @@
         <v>72</v>
       </c>
       <c r="G14" s="1">
-        <v>44695</v>
+        <v>44707</v>
       </c>
       <c r="H14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I14" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J14" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="K14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14" s="2">
         <v>0</v>
       </c>
       <c r="N14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O14" s="2">
         <v>0</v>
@@ -4227,7 +4227,7 @@
         <v>0</v>
       </c>
       <c r="Q14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R14" s="2">
         <v>0</v>
@@ -4236,7 +4236,7 @@
         <v>0</v>
       </c>
       <c r="T14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="U14" s="2">
         <v>0</v>
@@ -4287,7 +4287,7 @@
         <v>0</v>
       </c>
       <c r="AU14" s="1">
-        <v>44707</v>
+        <v>44714</v>
       </c>
       <c r="AV14" s="2">
         <v>1</v>
@@ -4297,22 +4297,22 @@
       </c>
       <c r="AX14" s="2"/>
       <c r="AY14" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AZ14" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BA14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE14" s="2">
         <v>0</v>
@@ -4324,10 +4324,10 @@
         <v>0</v>
       </c>
       <c r="BH14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ14" s="2">
         <v>0</v>
@@ -4336,7 +4336,7 @@
         <v>0</v>
       </c>
       <c r="BL14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BM14" s="2">
         <v>0</v>
@@ -4360,7 +4360,7 @@
         <v>0</v>
       </c>
       <c r="BT14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU14" s="2">
         <v>0</v>
@@ -4372,19 +4372,19 @@
         <v>0</v>
       </c>
       <c r="BX14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BY14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BZ14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA14" s="2">
         <v>0</v>
       </c>
       <c r="CB14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC14" s="2">
         <v>0</v>
@@ -4924,34 +4924,34 @@
         <v>73</v>
       </c>
       <c r="G17" s="1">
-        <v>44797</v>
+        <v>44871</v>
       </c>
       <c r="H17" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I17" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="J17" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="K17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17" s="2">
         <v>0</v>
       </c>
       <c r="N17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O17" s="2">
         <v>0</v>
       </c>
       <c r="P17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q17" s="2">
         <v>0</v>
@@ -4963,24 +4963,24 @@
         <v>0</v>
       </c>
       <c r="T17" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="U17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V17" t="s">
         <v>122</v>
       </c>
       <c r="W17" s="2"/>
-      <c r="X17" s="2"/>
+      <c r="X17" s="2">
+        <v>1</v>
+      </c>
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
-      <c r="AA17" s="2">
-        <v>1</v>
-      </c>
+      <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
       <c r="AC17" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AD17" s="2">
         <v>1</v>
@@ -4989,13 +4989,17 @@
       <c r="AF17" s="2"/>
       <c r="AG17" s="2"/>
       <c r="AH17" s="2"/>
-      <c r="AI17" s="2"/>
-      <c r="AJ17" s="2"/>
+      <c r="AI17" s="2">
+        <v>1</v>
+      </c>
+      <c r="AJ17" s="2">
+        <v>1</v>
+      </c>
       <c r="AK17" s="2"/>
       <c r="AL17" s="2"/>
       <c r="AM17" s="2"/>
       <c r="AN17" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
       <c r="AO17" t="s">
         <v>156</v>
@@ -5014,26 +5018,26 @@
         <v>1</v>
       </c>
       <c r="AU17" s="1">
-        <v>44803</v>
+        <v>44879</v>
       </c>
       <c r="AV17" s="2">
         <v>1</v>
       </c>
       <c r="AW17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX17" s="2"/>
       <c r="AY17" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="AZ17" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BA17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC17" s="2">
         <v>0</v>
@@ -5045,7 +5049,7 @@
         <v>0</v>
       </c>
       <c r="BF17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG17" s="2">
         <v>1</v>
@@ -5069,7 +5073,7 @@
         <v>0</v>
       </c>
       <c r="BN17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BO17" s="2">
         <v>0</v>
@@ -5087,7 +5091,7 @@
         <v>0</v>
       </c>
       <c r="BT17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BU17" s="2">
         <v>0</v>
@@ -5111,7 +5115,7 @@
         <v>0</v>
       </c>
       <c r="CB17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CC17" s="2">
         <v>0</v>
@@ -5167,34 +5171,34 @@
         <v>73</v>
       </c>
       <c r="G18" s="1">
-        <v>44871</v>
+        <v>44797</v>
       </c>
       <c r="H18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M18" s="2">
         <v>0</v>
       </c>
       <c r="N18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O18" s="2">
         <v>0</v>
       </c>
       <c r="P18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q18" s="2">
         <v>0</v>
@@ -5206,24 +5210,24 @@
         <v>0</v>
       </c>
       <c r="T18" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="U18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V18" t="s">
         <v>123</v>
       </c>
       <c r="W18" s="2"/>
-      <c r="X18" s="2">
-        <v>1</v>
-      </c>
+      <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
-      <c r="AA18" s="2"/>
+      <c r="AA18" s="2">
+        <v>1</v>
+      </c>
       <c r="AB18" s="2"/>
       <c r="AC18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AD18" s="2">
         <v>1</v>
@@ -5232,17 +5236,13 @@
       <c r="AF18" s="2"/>
       <c r="AG18" s="2"/>
       <c r="AH18" s="2"/>
-      <c r="AI18" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ18" s="2">
-        <v>1</v>
-      </c>
+      <c r="AI18" s="2"/>
+      <c r="AJ18" s="2"/>
       <c r="AK18" s="2"/>
       <c r="AL18" s="2"/>
       <c r="AM18" s="2"/>
       <c r="AN18" t="s">
-        <v>107</v>
+        <v>149</v>
       </c>
       <c r="AO18" t="s">
         <v>157</v>
@@ -5261,26 +5261,26 @@
         <v>1</v>
       </c>
       <c r="AU18" s="1">
-        <v>44879</v>
+        <v>44803</v>
       </c>
       <c r="AV18" s="2">
         <v>1</v>
       </c>
       <c r="AW18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX18" s="2"/>
       <c r="AY18" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="AZ18" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="BA18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC18" s="2">
         <v>0</v>
@@ -5292,7 +5292,7 @@
         <v>0</v>
       </c>
       <c r="BF18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG18" s="2">
         <v>1</v>
@@ -5316,7 +5316,7 @@
         <v>0</v>
       </c>
       <c r="BN18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO18" s="2">
         <v>0</v>
@@ -5334,7 +5334,7 @@
         <v>0</v>
       </c>
       <c r="BT18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU18" s="2">
         <v>0</v>
@@ -5358,7 +5358,7 @@
         <v>0</v>
       </c>
       <c r="CB18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC18" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
updated UNII CAS PubChem
</commit_message>
<xml_diff>
--- a/datasets/analysis_dataset.xlsx
+++ b/datasets/analysis_dataset.xlsx
@@ -51,10 +51,10 @@
     <t>193</t>
   </si>
   <si>
+    <t>253</t>
+  </si>
+  <si>
     <t>299</t>
-  </si>
-  <si>
-    <t>253</t>
   </si>
   <si>
     <t>644</t>
@@ -3958,28 +3958,28 @@
         <v>72</v>
       </c>
       <c r="G13" s="1">
-        <v>44695</v>
+        <v>44707</v>
       </c>
       <c r="H13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J13" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="K13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13" s="2">
         <v>0</v>
       </c>
       <c r="N13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O13" s="2">
         <v>0</v>
@@ -3988,7 +3988,7 @@
         <v>0</v>
       </c>
       <c r="Q13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R13" s="2">
         <v>0</v>
@@ -3997,7 +3997,7 @@
         <v>0</v>
       </c>
       <c r="T13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="U13" s="2">
         <v>0</v>
@@ -4048,7 +4048,7 @@
         <v>0</v>
       </c>
       <c r="AU13" s="1">
-        <v>44707</v>
+        <v>44714</v>
       </c>
       <c r="AV13" s="2">
         <v>1</v>
@@ -4058,22 +4058,22 @@
       </c>
       <c r="AX13" s="2"/>
       <c r="AY13" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AZ13" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BA13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE13" s="2">
         <v>0</v>
@@ -4085,10 +4085,10 @@
         <v>0</v>
       </c>
       <c r="BH13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ13" s="2">
         <v>0</v>
@@ -4097,7 +4097,7 @@
         <v>0</v>
       </c>
       <c r="BL13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BM13" s="2">
         <v>0</v>
@@ -4121,7 +4121,7 @@
         <v>0</v>
       </c>
       <c r="BT13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU13" s="2">
         <v>0</v>
@@ -4133,19 +4133,19 @@
         <v>0</v>
       </c>
       <c r="BX13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BY13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BZ13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA13" s="2">
         <v>0</v>
       </c>
       <c r="CB13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC13" s="2">
         <v>0</v>
@@ -4197,28 +4197,28 @@
         <v>72</v>
       </c>
       <c r="G14" s="1">
-        <v>44707</v>
+        <v>44695</v>
       </c>
       <c r="H14" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J14" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="K14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14" s="2">
         <v>0</v>
       </c>
       <c r="N14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O14" s="2">
         <v>0</v>
@@ -4227,7 +4227,7 @@
         <v>0</v>
       </c>
       <c r="Q14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R14" s="2">
         <v>0</v>
@@ -4236,7 +4236,7 @@
         <v>0</v>
       </c>
       <c r="T14" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="U14" s="2">
         <v>0</v>
@@ -4287,7 +4287,7 @@
         <v>0</v>
       </c>
       <c r="AU14" s="1">
-        <v>44714</v>
+        <v>44707</v>
       </c>
       <c r="AV14" s="2">
         <v>1</v>
@@ -4297,22 +4297,22 @@
       </c>
       <c r="AX14" s="2"/>
       <c r="AY14" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AZ14" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="BA14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE14" s="2">
         <v>0</v>
@@ -4324,10 +4324,10 @@
         <v>0</v>
       </c>
       <c r="BH14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ14" s="2">
         <v>0</v>
@@ -4336,7 +4336,7 @@
         <v>0</v>
       </c>
       <c r="BL14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM14" s="2">
         <v>0</v>
@@ -4360,7 +4360,7 @@
         <v>0</v>
       </c>
       <c r="BT14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BU14" s="2">
         <v>0</v>
@@ -4372,19 +4372,19 @@
         <v>0</v>
       </c>
       <c r="BX14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY14" s="2">
         <v>1</v>
       </c>
       <c r="BZ14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CA14" s="2">
         <v>0</v>
       </c>
       <c r="CB14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CC14" s="2">
         <v>0</v>
@@ -5839,7 +5839,7 @@
         <v>0</v>
       </c>
       <c r="BY20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BZ20" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
evening results and pending update
</commit_message>
<xml_diff>
--- a/datasets/analysis_dataset.xlsx
+++ b/datasets/analysis_dataset.xlsx
@@ -33,12 +33,12 @@
     <t>368</t>
   </si>
   <si>
+    <t>280</t>
+  </si>
+  <si>
     <t>424</t>
   </si>
   <si>
-    <t>280</t>
-  </si>
-  <si>
     <t>437</t>
   </si>
   <si>
@@ -51,12 +51,12 @@
     <t>193</t>
   </si>
   <si>
+    <t>253</t>
+  </si>
+  <si>
     <t>299</t>
   </si>
   <si>
-    <t>253</t>
-  </si>
-  <si>
     <t>644</t>
   </si>
   <si>
@@ -258,12 +258,12 @@
     <t>syringe</t>
   </si>
   <si>
+    <t>pill</t>
+  </si>
+  <si>
     <t>spatula</t>
   </si>
   <si>
-    <t>pill</t>
-  </si>
-  <si>
     <t>swab</t>
   </si>
   <si>
@@ -348,10 +348,10 @@
     <t>tan</t>
   </si>
   <si>
+    <t>blue</t>
+  </si>
+  <si>
     <t>white</t>
-  </si>
-  <si>
-    <t>blue</t>
   </si>
   <si>
     <t>brown</t>
@@ -1073,7 +1073,7 @@
         <v>125</v>
       </c>
       <c r="Y1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z1" t="s">
         <v>120</v>
@@ -2563,7 +2563,7 @@
         <v>70</v>
       </c>
       <c r="G7" s="1">
-        <v>44484</v>
+        <v>44701</v>
       </c>
       <c r="H7" t="s">
         <v>81</v>
@@ -2575,13 +2575,13 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="L7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7" s="2">
         <v>0</v>
@@ -2602,22 +2602,22 @@
         <v>0</v>
       </c>
       <c r="T7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U7" t="s">
         <v>111</v>
       </c>
       <c r="V7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W7" t="s">
-        <v>120</v>
+        <v>81</v>
       </c>
       <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="2">
-        <v>1</v>
-      </c>
+      <c r="Y7" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
@@ -2638,12 +2638,14 @@
         <v>108</v>
       </c>
       <c r="AP7" t="s">
-        <v>108</v>
+        <v>155</v>
       </c>
       <c r="AQ7" t="s">
-        <v>79</v>
-      </c>
-      <c r="AR7" s="2"/>
+        <v>160</v>
+      </c>
+      <c r="AR7" s="2">
+        <v>0</v>
+      </c>
       <c r="AS7" t="s">
         <v>108</v>
       </c>
@@ -2652,32 +2654,32 @@
         <v>0</v>
       </c>
       <c r="AV7" s="1">
-        <v>44603</v>
+        <v>44721</v>
       </c>
       <c r="AW7" s="2">
         <v>1</v>
       </c>
       <c r="AX7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY7" s="2"/>
       <c r="AZ7" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="BA7" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="BB7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF7" s="2">
         <v>0</v>
@@ -2686,7 +2688,7 @@
         <v>0</v>
       </c>
       <c r="BH7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI7" s="2">
         <v>0</v>
@@ -2695,7 +2697,7 @@
         <v>0</v>
       </c>
       <c r="BK7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL7" s="2">
         <v>0</v>
@@ -2731,7 +2733,7 @@
         <v>0</v>
       </c>
       <c r="BW7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX7" s="2">
         <v>0</v>
@@ -2746,7 +2748,7 @@
         <v>0</v>
       </c>
       <c r="CB7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CC7" s="2">
         <v>0</v>
@@ -2755,13 +2757,13 @@
         <v>0</v>
       </c>
       <c r="CE7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CH7" t="s">
         <v>47</v>
@@ -2811,7 +2813,7 @@
         <v>70</v>
       </c>
       <c r="G8" s="1">
-        <v>44701</v>
+        <v>44484</v>
       </c>
       <c r="H8" t="s">
         <v>82</v>
@@ -2823,13 +2825,13 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="L8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8" s="2">
         <v>0</v>
@@ -2850,22 +2852,22 @@
         <v>0</v>
       </c>
       <c r="T8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U8" t="s">
         <v>112</v>
       </c>
       <c r="V8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W8" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
       <c r="X8" s="2"/>
-      <c r="Y8" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2">
+        <v>1</v>
+      </c>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
@@ -2886,14 +2888,12 @@
         <v>108</v>
       </c>
       <c r="AP8" t="s">
-        <v>155</v>
+        <v>108</v>
       </c>
       <c r="AQ8" t="s">
-        <v>160</v>
-      </c>
-      <c r="AR8" s="2">
-        <v>0</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="AR8" s="2"/>
       <c r="AS8" t="s">
         <v>108</v>
       </c>
@@ -2902,32 +2902,32 @@
         <v>0</v>
       </c>
       <c r="AV8" s="1">
-        <v>44721</v>
+        <v>44603</v>
       </c>
       <c r="AW8" s="2">
         <v>1</v>
       </c>
       <c r="AX8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY8" s="2"/>
       <c r="AZ8" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="BA8" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="BB8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF8" s="2">
         <v>0</v>
@@ -2936,7 +2936,7 @@
         <v>0</v>
       </c>
       <c r="BH8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI8" s="2">
         <v>0</v>
@@ -2945,7 +2945,7 @@
         <v>0</v>
       </c>
       <c r="BK8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL8" s="2">
         <v>0</v>
@@ -2981,7 +2981,7 @@
         <v>0</v>
       </c>
       <c r="BW8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX8" s="2">
         <v>0</v>
@@ -2996,7 +2996,7 @@
         <v>0</v>
       </c>
       <c r="CB8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC8" s="2">
         <v>0</v>
@@ -3005,13 +3005,13 @@
         <v>0</v>
       </c>
       <c r="CE8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CG8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH8" t="s">
         <v>47</v>
@@ -3353,7 +3353,7 @@
         <v>0</v>
       </c>
       <c r="U10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V10" s="2">
         <v>0</v>
@@ -3818,10 +3818,10 @@
         <v>44883</v>
       </c>
       <c r="H12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J12" s="2">
         <v>1</v>
@@ -3857,7 +3857,7 @@
         <v>0</v>
       </c>
       <c r="U12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V12" s="2">
         <v>0</v>
@@ -4075,31 +4075,31 @@
         <v>72</v>
       </c>
       <c r="G13" s="1">
-        <v>44695</v>
+        <v>44707</v>
       </c>
       <c r="H13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J13" s="2">
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="L13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N13" s="2">
         <v>0</v>
       </c>
       <c r="O13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P13" s="2">
         <v>0</v>
@@ -4108,7 +4108,7 @@
         <v>0</v>
       </c>
       <c r="R13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S13" s="2">
         <v>0</v>
@@ -4117,7 +4117,7 @@
         <v>0</v>
       </c>
       <c r="U13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="V13" s="2">
         <v>0</v>
@@ -4168,7 +4168,7 @@
         <v>0</v>
       </c>
       <c r="AV13" s="1">
-        <v>44707</v>
+        <v>44714</v>
       </c>
       <c r="AW13" s="2">
         <v>1</v>
@@ -4178,22 +4178,22 @@
       </c>
       <c r="AY13" s="2"/>
       <c r="AZ13" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="BA13" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BB13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF13" s="2">
         <v>0</v>
@@ -4205,10 +4205,10 @@
         <v>0</v>
       </c>
       <c r="BI13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK13" s="2">
         <v>0</v>
@@ -4217,7 +4217,7 @@
         <v>0</v>
       </c>
       <c r="BM13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN13" s="2">
         <v>0</v>
@@ -4247,7 +4247,7 @@
         <v>0</v>
       </c>
       <c r="BW13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX13" s="2">
         <v>0</v>
@@ -4259,19 +4259,19 @@
         <v>0</v>
       </c>
       <c r="CA13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CB13" s="2">
         <v>1</v>
       </c>
       <c r="CC13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD13" s="2">
         <v>0</v>
       </c>
       <c r="CE13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF13" s="2">
         <v>0</v>
@@ -4323,31 +4323,31 @@
         <v>72</v>
       </c>
       <c r="G14" s="1">
-        <v>44707</v>
+        <v>44695</v>
       </c>
       <c r="H14" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J14" s="2">
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="L14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14" s="2">
         <v>0</v>
       </c>
       <c r="O14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P14" s="2">
         <v>0</v>
@@ -4356,7 +4356,7 @@
         <v>0</v>
       </c>
       <c r="R14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S14" s="2">
         <v>0</v>
@@ -4365,7 +4365,7 @@
         <v>0</v>
       </c>
       <c r="U14" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="V14" s="2">
         <v>0</v>
@@ -4416,7 +4416,7 @@
         <v>0</v>
       </c>
       <c r="AV14" s="1">
-        <v>44714</v>
+        <v>44707</v>
       </c>
       <c r="AW14" s="2">
         <v>1</v>
@@ -4426,22 +4426,22 @@
       </c>
       <c r="AY14" s="2"/>
       <c r="AZ14" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="BA14" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="BB14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF14" s="2">
         <v>0</v>
@@ -4453,10 +4453,10 @@
         <v>0</v>
       </c>
       <c r="BI14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK14" s="2">
         <v>0</v>
@@ -4465,7 +4465,7 @@
         <v>0</v>
       </c>
       <c r="BM14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN14" s="2">
         <v>0</v>
@@ -4495,7 +4495,7 @@
         <v>0</v>
       </c>
       <c r="BW14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX14" s="2">
         <v>0</v>
@@ -4507,19 +4507,19 @@
         <v>0</v>
       </c>
       <c r="CA14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB14" s="2">
         <v>1</v>
       </c>
       <c r="CC14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CD14" s="2">
         <v>0</v>
       </c>
       <c r="CE14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF14" s="2">
         <v>0</v>
@@ -4613,7 +4613,7 @@
         <v>0</v>
       </c>
       <c r="U15" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V15" s="2">
         <v>0</v>
@@ -5080,10 +5080,10 @@
         <v>44871</v>
       </c>
       <c r="H17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J17" s="2">
         <v>1</v>
@@ -5119,7 +5119,7 @@
         <v>0</v>
       </c>
       <c r="U17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V17" s="2">
         <v>1</v>
@@ -5844,10 +5844,10 @@
         <v>44727</v>
       </c>
       <c r="H20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J20" s="2">
         <v>1</v>
@@ -5883,7 +5883,7 @@
         <v>0</v>
       </c>
       <c r="U20" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V20" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Automatic post-commit hook for streamlit
</commit_message>
<xml_diff>
--- a/datasets/analysis_dataset.xlsx
+++ b/datasets/analysis_dataset.xlsx
@@ -33,12 +33,12 @@
     <t>368</t>
   </si>
   <si>
+    <t>280</t>
+  </si>
+  <si>
     <t>424</t>
   </si>
   <si>
-    <t>280</t>
-  </si>
-  <si>
     <t>437</t>
   </si>
   <si>
@@ -51,24 +51,24 @@
     <t>193</t>
   </si>
   <si>
+    <t>299</t>
+  </si>
+  <si>
     <t>253</t>
   </si>
   <si>
-    <t>299</t>
-  </si>
-  <si>
     <t>644</t>
   </si>
   <si>
     <t>340</t>
   </si>
   <si>
+    <t>555</t>
+  </si>
+  <si>
     <t>836</t>
   </si>
   <si>
-    <t>555</t>
-  </si>
-  <si>
     <t>408</t>
   </si>
   <si>
@@ -258,12 +258,12 @@
     <t>syringe</t>
   </si>
   <si>
+    <t>pill</t>
+  </si>
+  <si>
     <t>spatula</t>
   </si>
   <si>
-    <t>pill</t>
-  </si>
-  <si>
     <t>swab</t>
   </si>
   <si>
@@ -348,12 +348,12 @@
     <t>tan</t>
   </si>
   <si>
+    <t>blue</t>
+  </si>
+  <si>
     <t>white</t>
   </si>
   <si>
-    <t>blue</t>
-  </si>
-  <si>
     <t>brown</t>
   </si>
   <si>
@@ -384,12 +384,12 @@
     <t>powder; chunky; shiny</t>
   </si>
   <si>
+    <t>crystals</t>
+  </si>
+  <si>
     <t>fake pill</t>
   </si>
   <si>
-    <t>crystals</t>
-  </si>
-  <si>
     <t>tar</t>
   </si>
   <si>
@@ -486,10 +486,10 @@
     <t>fast acting</t>
   </si>
   <si>
+    <t>FTS = negative</t>
+  </si>
+  <si>
     <t>strong blues</t>
-  </si>
-  <si>
-    <t>FTS = negative</t>
   </si>
   <si>
     <t>overdose</t>
@@ -1073,7 +1073,7 @@
         <v>125</v>
       </c>
       <c r="Y1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z1" t="s">
         <v>120</v>
@@ -1082,7 +1082,7 @@
         <v>126</v>
       </c>
       <c r="AB1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AC1" t="s">
         <v>127</v>
@@ -2563,7 +2563,7 @@
         <v>70</v>
       </c>
       <c r="G7" s="1">
-        <v>44484</v>
+        <v>44701</v>
       </c>
       <c r="H7" t="s">
         <v>81</v>
@@ -2575,13 +2575,13 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="L7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7" s="2">
         <v>0</v>
@@ -2602,22 +2602,22 @@
         <v>0</v>
       </c>
       <c r="T7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U7" t="s">
         <v>111</v>
       </c>
       <c r="V7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W7" t="s">
-        <v>120</v>
+        <v>81</v>
       </c>
       <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="2">
-        <v>1</v>
-      </c>
+      <c r="Y7" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
@@ -2638,12 +2638,14 @@
         <v>108</v>
       </c>
       <c r="AP7" t="s">
-        <v>108</v>
+        <v>155</v>
       </c>
       <c r="AQ7" t="s">
-        <v>79</v>
-      </c>
-      <c r="AR7" s="2"/>
+        <v>160</v>
+      </c>
+      <c r="AR7" s="2">
+        <v>0</v>
+      </c>
       <c r="AS7" t="s">
         <v>108</v>
       </c>
@@ -2652,32 +2654,32 @@
         <v>0</v>
       </c>
       <c r="AV7" s="1">
-        <v>44603</v>
+        <v>44721</v>
       </c>
       <c r="AW7" s="2">
         <v>1</v>
       </c>
       <c r="AX7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY7" s="2"/>
       <c r="AZ7" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="BA7" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="BB7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF7" s="2">
         <v>0</v>
@@ -2686,7 +2688,7 @@
         <v>0</v>
       </c>
       <c r="BH7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI7" s="2">
         <v>0</v>
@@ -2695,7 +2697,7 @@
         <v>0</v>
       </c>
       <c r="BK7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL7" s="2">
         <v>0</v>
@@ -2731,7 +2733,7 @@
         <v>0</v>
       </c>
       <c r="BW7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX7" s="2">
         <v>0</v>
@@ -2746,7 +2748,7 @@
         <v>0</v>
       </c>
       <c r="CB7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CC7" s="2">
         <v>0</v>
@@ -2755,13 +2757,13 @@
         <v>0</v>
       </c>
       <c r="CE7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CH7" t="s">
         <v>47</v>
@@ -2811,7 +2813,7 @@
         <v>70</v>
       </c>
       <c r="G8" s="1">
-        <v>44701</v>
+        <v>44484</v>
       </c>
       <c r="H8" t="s">
         <v>82</v>
@@ -2823,13 +2825,13 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="L8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8" s="2">
         <v>0</v>
@@ -2850,22 +2852,22 @@
         <v>0</v>
       </c>
       <c r="T8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U8" t="s">
         <v>112</v>
       </c>
       <c r="V8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W8" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
       <c r="X8" s="2"/>
-      <c r="Y8" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2">
+        <v>1</v>
+      </c>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
@@ -2886,14 +2888,12 @@
         <v>108</v>
       </c>
       <c r="AP8" t="s">
-        <v>155</v>
+        <v>108</v>
       </c>
       <c r="AQ8" t="s">
-        <v>160</v>
-      </c>
-      <c r="AR8" s="2">
-        <v>0</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="AR8" s="2"/>
       <c r="AS8" t="s">
         <v>108</v>
       </c>
@@ -2902,32 +2902,32 @@
         <v>0</v>
       </c>
       <c r="AV8" s="1">
-        <v>44721</v>
+        <v>44603</v>
       </c>
       <c r="AW8" s="2">
         <v>1</v>
       </c>
       <c r="AX8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY8" s="2"/>
       <c r="AZ8" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="BA8" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="BB8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF8" s="2">
         <v>0</v>
@@ -2936,7 +2936,7 @@
         <v>0</v>
       </c>
       <c r="BH8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI8" s="2">
         <v>0</v>
@@ -2945,7 +2945,7 @@
         <v>0</v>
       </c>
       <c r="BK8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL8" s="2">
         <v>0</v>
@@ -2981,7 +2981,7 @@
         <v>0</v>
       </c>
       <c r="BW8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX8" s="2">
         <v>0</v>
@@ -2996,7 +2996,7 @@
         <v>0</v>
       </c>
       <c r="CB8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC8" s="2">
         <v>0</v>
@@ -3005,13 +3005,13 @@
         <v>0</v>
       </c>
       <c r="CE8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CG8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH8" t="s">
         <v>47</v>
@@ -3353,7 +3353,7 @@
         <v>0</v>
       </c>
       <c r="U10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V10" s="2">
         <v>0</v>
@@ -3818,10 +3818,10 @@
         <v>44883</v>
       </c>
       <c r="H12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J12" s="2">
         <v>1</v>
@@ -3857,7 +3857,7 @@
         <v>0</v>
       </c>
       <c r="U12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V12" s="2">
         <v>0</v>
@@ -4075,31 +4075,31 @@
         <v>72</v>
       </c>
       <c r="G13" s="1">
-        <v>44707</v>
+        <v>44695</v>
       </c>
       <c r="H13" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I13" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J13" s="2">
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="L13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13" s="2">
         <v>0</v>
       </c>
       <c r="O13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P13" s="2">
         <v>0</v>
@@ -4108,7 +4108,7 @@
         <v>0</v>
       </c>
       <c r="R13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S13" s="2">
         <v>0</v>
@@ -4117,7 +4117,7 @@
         <v>0</v>
       </c>
       <c r="U13" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="V13" s="2">
         <v>0</v>
@@ -4168,7 +4168,7 @@
         <v>0</v>
       </c>
       <c r="AV13" s="1">
-        <v>44714</v>
+        <v>44707</v>
       </c>
       <c r="AW13" s="2">
         <v>1</v>
@@ -4178,22 +4178,22 @@
       </c>
       <c r="AY13" s="2"/>
       <c r="AZ13" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="BA13" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="BB13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF13" s="2">
         <v>0</v>
@@ -4205,10 +4205,10 @@
         <v>0</v>
       </c>
       <c r="BI13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK13" s="2">
         <v>0</v>
@@ -4217,7 +4217,7 @@
         <v>0</v>
       </c>
       <c r="BM13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN13" s="2">
         <v>0</v>
@@ -4247,7 +4247,7 @@
         <v>0</v>
       </c>
       <c r="BW13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX13" s="2">
         <v>0</v>
@@ -4259,19 +4259,19 @@
         <v>0</v>
       </c>
       <c r="CA13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB13" s="2">
         <v>1</v>
       </c>
       <c r="CC13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CD13" s="2">
         <v>0</v>
       </c>
       <c r="CE13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF13" s="2">
         <v>0</v>
@@ -4323,31 +4323,31 @@
         <v>72</v>
       </c>
       <c r="G14" s="1">
-        <v>44695</v>
+        <v>44707</v>
       </c>
       <c r="H14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I14" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J14" s="2">
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="L14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N14" s="2">
         <v>0</v>
       </c>
       <c r="O14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P14" s="2">
         <v>0</v>
@@ -4356,7 +4356,7 @@
         <v>0</v>
       </c>
       <c r="R14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S14" s="2">
         <v>0</v>
@@ -4365,7 +4365,7 @@
         <v>0</v>
       </c>
       <c r="U14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="V14" s="2">
         <v>0</v>
@@ -4416,7 +4416,7 @@
         <v>0</v>
       </c>
       <c r="AV14" s="1">
-        <v>44707</v>
+        <v>44714</v>
       </c>
       <c r="AW14" s="2">
         <v>1</v>
@@ -4426,22 +4426,22 @@
       </c>
       <c r="AY14" s="2"/>
       <c r="AZ14" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="BA14" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BB14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF14" s="2">
         <v>0</v>
@@ -4453,10 +4453,10 @@
         <v>0</v>
       </c>
       <c r="BI14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK14" s="2">
         <v>0</v>
@@ -4465,7 +4465,7 @@
         <v>0</v>
       </c>
       <c r="BM14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN14" s="2">
         <v>0</v>
@@ -4495,7 +4495,7 @@
         <v>0</v>
       </c>
       <c r="BW14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX14" s="2">
         <v>0</v>
@@ -4507,19 +4507,19 @@
         <v>0</v>
       </c>
       <c r="CA14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CB14" s="2">
         <v>1</v>
       </c>
       <c r="CC14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD14" s="2">
         <v>0</v>
       </c>
       <c r="CE14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF14" s="2">
         <v>0</v>
@@ -4613,7 +4613,7 @@
         <v>0</v>
       </c>
       <c r="U15" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V15" s="2">
         <v>0</v>
@@ -5077,37 +5077,37 @@
         <v>73</v>
       </c>
       <c r="G17" s="1">
-        <v>44871</v>
+        <v>44797</v>
       </c>
       <c r="H17" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I17" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J17" s="2">
         <v>1</v>
       </c>
       <c r="K17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N17" s="2">
         <v>0</v>
       </c>
       <c r="O17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P17" s="2">
         <v>0</v>
       </c>
       <c r="Q17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R17" s="2">
         <v>0</v>
@@ -5119,24 +5119,24 @@
         <v>0</v>
       </c>
       <c r="U17" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="V17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W17" t="s">
         <v>123</v>
       </c>
       <c r="X17" s="2"/>
-      <c r="Y17" s="2">
-        <v>1</v>
-      </c>
+      <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
-      <c r="AB17" s="2"/>
+      <c r="AB17" s="2">
+        <v>1</v>
+      </c>
       <c r="AC17" s="2"/>
       <c r="AD17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AE17" s="2">
         <v>1</v>
@@ -5145,17 +5145,13 @@
       <c r="AG17" s="2"/>
       <c r="AH17" s="2"/>
       <c r="AI17" s="2"/>
-      <c r="AJ17" s="2">
-        <v>1</v>
-      </c>
-      <c r="AK17" s="2">
-        <v>1</v>
-      </c>
+      <c r="AJ17" s="2"/>
+      <c r="AK17" s="2"/>
       <c r="AL17" s="2"/>
       <c r="AM17" s="2"/>
       <c r="AN17" s="2"/>
       <c r="AO17" t="s">
-        <v>108</v>
+        <v>150</v>
       </c>
       <c r="AP17" t="s">
         <v>157</v>
@@ -5174,26 +5170,26 @@
         <v>1</v>
       </c>
       <c r="AV17" s="1">
-        <v>44879</v>
+        <v>44803</v>
       </c>
       <c r="AW17" s="2">
         <v>1</v>
       </c>
       <c r="AX17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY17" s="2"/>
       <c r="AZ17" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="BA17" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="BB17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD17" s="2">
         <v>0</v>
@@ -5205,7 +5201,7 @@
         <v>0</v>
       </c>
       <c r="BG17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BH17" s="2">
         <v>1</v>
@@ -5229,7 +5225,7 @@
         <v>0</v>
       </c>
       <c r="BO17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP17" s="2">
         <v>0</v>
@@ -5253,7 +5249,7 @@
         <v>0</v>
       </c>
       <c r="BW17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX17" s="2">
         <v>0</v>
@@ -5277,7 +5273,7 @@
         <v>0</v>
       </c>
       <c r="CE17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF17" s="2">
         <v>0</v>
@@ -5333,37 +5329,37 @@
         <v>73</v>
       </c>
       <c r="G18" s="1">
-        <v>44797</v>
+        <v>44871</v>
       </c>
       <c r="H18" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I18" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="J18" s="2">
         <v>1</v>
       </c>
       <c r="K18" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N18" s="2">
         <v>0</v>
       </c>
       <c r="O18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P18" s="2">
         <v>0</v>
       </c>
       <c r="Q18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R18" s="2">
         <v>0</v>
@@ -5375,24 +5371,24 @@
         <v>0</v>
       </c>
       <c r="U18" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="V18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W18" t="s">
         <v>124</v>
       </c>
       <c r="X18" s="2"/>
-      <c r="Y18" s="2"/>
+      <c r="Y18" s="2">
+        <v>1</v>
+      </c>
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
-      <c r="AB18" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB18" s="2"/>
       <c r="AC18" s="2"/>
       <c r="AD18" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="AE18" s="2">
         <v>1</v>
@@ -5401,13 +5397,17 @@
       <c r="AG18" s="2"/>
       <c r="AH18" s="2"/>
       <c r="AI18" s="2"/>
-      <c r="AJ18" s="2"/>
-      <c r="AK18" s="2"/>
+      <c r="AJ18" s="2">
+        <v>1</v>
+      </c>
+      <c r="AK18" s="2">
+        <v>1</v>
+      </c>
       <c r="AL18" s="2"/>
       <c r="AM18" s="2"/>
       <c r="AN18" s="2"/>
       <c r="AO18" t="s">
-        <v>150</v>
+        <v>108</v>
       </c>
       <c r="AP18" t="s">
         <v>158</v>
@@ -5426,26 +5426,26 @@
         <v>1</v>
       </c>
       <c r="AV18" s="1">
-        <v>44803</v>
+        <v>44879</v>
       </c>
       <c r="AW18" s="2">
         <v>1</v>
       </c>
       <c r="AX18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY18" s="2"/>
       <c r="AZ18" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="BA18" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BB18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD18" s="2">
         <v>0</v>
@@ -5457,7 +5457,7 @@
         <v>0</v>
       </c>
       <c r="BG18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH18" s="2">
         <v>1</v>
@@ -5481,7 +5481,7 @@
         <v>0</v>
       </c>
       <c r="BO18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BP18" s="2">
         <v>0</v>
@@ -5505,7 +5505,7 @@
         <v>0</v>
       </c>
       <c r="BW18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX18" s="2">
         <v>0</v>
@@ -5529,7 +5529,7 @@
         <v>0</v>
       </c>
       <c r="CE18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF18" s="2">
         <v>0</v>
@@ -5844,10 +5844,10 @@
         <v>44727</v>
       </c>
       <c r="H20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J20" s="2">
         <v>1</v>
@@ -5883,7 +5883,7 @@
         <v>0</v>
       </c>
       <c r="U20" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V20" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Tuesday update batch 2
</commit_message>
<xml_diff>
--- a/datasets/analysis_dataset.xlsx
+++ b/datasets/analysis_dataset.xlsx
@@ -51,24 +51,24 @@
     <t>193</t>
   </si>
   <si>
+    <t>299</t>
+  </si>
+  <si>
     <t>253</t>
   </si>
   <si>
-    <t>299</t>
-  </si>
-  <si>
     <t>644</t>
   </si>
   <si>
     <t>340</t>
   </si>
   <si>
+    <t>555</t>
+  </si>
+  <si>
     <t>836</t>
   </si>
   <si>
-    <t>555</t>
-  </si>
-  <si>
     <t>408</t>
   </si>
   <si>
@@ -384,12 +384,12 @@
     <t>powder; chunky; shiny</t>
   </si>
   <si>
+    <t>crystals</t>
+  </si>
+  <si>
     <t>fake pill</t>
   </si>
   <si>
-    <t>crystals</t>
-  </si>
-  <si>
     <t>tar</t>
   </si>
   <si>
@@ -486,10 +486,10 @@
     <t>fast acting</t>
   </si>
   <si>
+    <t>FTS = negative</t>
+  </si>
+  <si>
     <t>strong blues</t>
-  </si>
-  <si>
-    <t>FTS = negative</t>
   </si>
   <si>
     <t>overdose</t>
@@ -1082,7 +1082,7 @@
         <v>126</v>
       </c>
       <c r="AB1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AC1" t="s">
         <v>127</v>
@@ -4075,31 +4075,31 @@
         <v>72</v>
       </c>
       <c r="G13" s="1">
-        <v>44707</v>
+        <v>44695</v>
       </c>
       <c r="H13" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I13" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J13" s="2">
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="L13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13" s="2">
         <v>0</v>
       </c>
       <c r="O13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P13" s="2">
         <v>0</v>
@@ -4108,7 +4108,7 @@
         <v>0</v>
       </c>
       <c r="R13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S13" s="2">
         <v>0</v>
@@ -4117,7 +4117,7 @@
         <v>0</v>
       </c>
       <c r="U13" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="V13" s="2">
         <v>0</v>
@@ -4168,7 +4168,7 @@
         <v>0</v>
       </c>
       <c r="AV13" s="1">
-        <v>44714</v>
+        <v>44707</v>
       </c>
       <c r="AW13" s="2">
         <v>1</v>
@@ -4178,22 +4178,22 @@
       </c>
       <c r="AY13" s="2"/>
       <c r="AZ13" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="BA13" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="BB13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF13" s="2">
         <v>0</v>
@@ -4205,10 +4205,10 @@
         <v>0</v>
       </c>
       <c r="BI13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK13" s="2">
         <v>0</v>
@@ -4217,7 +4217,7 @@
         <v>0</v>
       </c>
       <c r="BM13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN13" s="2">
         <v>0</v>
@@ -4247,7 +4247,7 @@
         <v>0</v>
       </c>
       <c r="BW13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX13" s="2">
         <v>0</v>
@@ -4259,19 +4259,19 @@
         <v>0</v>
       </c>
       <c r="CA13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB13" s="2">
         <v>1</v>
       </c>
       <c r="CC13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CD13" s="2">
         <v>0</v>
       </c>
       <c r="CE13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF13" s="2">
         <v>0</v>
@@ -4323,31 +4323,31 @@
         <v>72</v>
       </c>
       <c r="G14" s="1">
-        <v>44695</v>
+        <v>44707</v>
       </c>
       <c r="H14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I14" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J14" s="2">
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="L14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N14" s="2">
         <v>0</v>
       </c>
       <c r="O14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P14" s="2">
         <v>0</v>
@@ -4356,7 +4356,7 @@
         <v>0</v>
       </c>
       <c r="R14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S14" s="2">
         <v>0</v>
@@ -4365,7 +4365,7 @@
         <v>0</v>
       </c>
       <c r="U14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="V14" s="2">
         <v>0</v>
@@ -4416,7 +4416,7 @@
         <v>0</v>
       </c>
       <c r="AV14" s="1">
-        <v>44707</v>
+        <v>44714</v>
       </c>
       <c r="AW14" s="2">
         <v>1</v>
@@ -4426,22 +4426,22 @@
       </c>
       <c r="AY14" s="2"/>
       <c r="AZ14" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="BA14" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BB14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF14" s="2">
         <v>0</v>
@@ -4453,10 +4453,10 @@
         <v>0</v>
       </c>
       <c r="BI14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK14" s="2">
         <v>0</v>
@@ -4465,7 +4465,7 @@
         <v>0</v>
       </c>
       <c r="BM14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN14" s="2">
         <v>0</v>
@@ -4495,7 +4495,7 @@
         <v>0</v>
       </c>
       <c r="BW14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX14" s="2">
         <v>0</v>
@@ -4507,19 +4507,19 @@
         <v>0</v>
       </c>
       <c r="CA14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CB14" s="2">
         <v>1</v>
       </c>
       <c r="CC14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD14" s="2">
         <v>0</v>
       </c>
       <c r="CE14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF14" s="2">
         <v>0</v>
@@ -5077,37 +5077,37 @@
         <v>73</v>
       </c>
       <c r="G17" s="1">
-        <v>44871</v>
+        <v>44797</v>
       </c>
       <c r="H17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J17" s="2">
         <v>1</v>
       </c>
       <c r="K17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N17" s="2">
         <v>0</v>
       </c>
       <c r="O17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P17" s="2">
         <v>0</v>
       </c>
       <c r="Q17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R17" s="2">
         <v>0</v>
@@ -5119,24 +5119,24 @@
         <v>0</v>
       </c>
       <c r="U17" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="V17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W17" t="s">
         <v>123</v>
       </c>
       <c r="X17" s="2"/>
-      <c r="Y17" s="2">
-        <v>1</v>
-      </c>
+      <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
-      <c r="AB17" s="2"/>
+      <c r="AB17" s="2">
+        <v>1</v>
+      </c>
       <c r="AC17" s="2"/>
       <c r="AD17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AE17" s="2">
         <v>1</v>
@@ -5145,17 +5145,13 @@
       <c r="AG17" s="2"/>
       <c r="AH17" s="2"/>
       <c r="AI17" s="2"/>
-      <c r="AJ17" s="2">
-        <v>1</v>
-      </c>
-      <c r="AK17" s="2">
-        <v>1</v>
-      </c>
+      <c r="AJ17" s="2"/>
+      <c r="AK17" s="2"/>
       <c r="AL17" s="2"/>
       <c r="AM17" s="2"/>
       <c r="AN17" s="2"/>
       <c r="AO17" t="s">
-        <v>108</v>
+        <v>150</v>
       </c>
       <c r="AP17" t="s">
         <v>157</v>
@@ -5174,26 +5170,26 @@
         <v>1</v>
       </c>
       <c r="AV17" s="1">
-        <v>44879</v>
+        <v>44803</v>
       </c>
       <c r="AW17" s="2">
         <v>1</v>
       </c>
       <c r="AX17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY17" s="2"/>
       <c r="AZ17" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="BA17" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="BB17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD17" s="2">
         <v>0</v>
@@ -5205,7 +5201,7 @@
         <v>0</v>
       </c>
       <c r="BG17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BH17" s="2">
         <v>1</v>
@@ -5229,7 +5225,7 @@
         <v>0</v>
       </c>
       <c r="BO17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP17" s="2">
         <v>0</v>
@@ -5253,7 +5249,7 @@
         <v>0</v>
       </c>
       <c r="BW17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX17" s="2">
         <v>0</v>
@@ -5277,7 +5273,7 @@
         <v>0</v>
       </c>
       <c r="CE17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF17" s="2">
         <v>0</v>
@@ -5333,37 +5329,37 @@
         <v>73</v>
       </c>
       <c r="G18" s="1">
-        <v>44797</v>
+        <v>44871</v>
       </c>
       <c r="H18" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I18" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="J18" s="2">
         <v>1</v>
       </c>
       <c r="K18" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N18" s="2">
         <v>0</v>
       </c>
       <c r="O18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P18" s="2">
         <v>0</v>
       </c>
       <c r="Q18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R18" s="2">
         <v>0</v>
@@ -5375,24 +5371,24 @@
         <v>0</v>
       </c>
       <c r="U18" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="V18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W18" t="s">
         <v>124</v>
       </c>
       <c r="X18" s="2"/>
-      <c r="Y18" s="2"/>
+      <c r="Y18" s="2">
+        <v>1</v>
+      </c>
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
-      <c r="AB18" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB18" s="2"/>
       <c r="AC18" s="2"/>
       <c r="AD18" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="AE18" s="2">
         <v>1</v>
@@ -5401,13 +5397,17 @@
       <c r="AG18" s="2"/>
       <c r="AH18" s="2"/>
       <c r="AI18" s="2"/>
-      <c r="AJ18" s="2"/>
-      <c r="AK18" s="2"/>
+      <c r="AJ18" s="2">
+        <v>1</v>
+      </c>
+      <c r="AK18" s="2">
+        <v>1</v>
+      </c>
       <c r="AL18" s="2"/>
       <c r="AM18" s="2"/>
       <c r="AN18" s="2"/>
       <c r="AO18" t="s">
-        <v>150</v>
+        <v>108</v>
       </c>
       <c r="AP18" t="s">
         <v>158</v>
@@ -5426,26 +5426,26 @@
         <v>1</v>
       </c>
       <c r="AV18" s="1">
-        <v>44803</v>
+        <v>44879</v>
       </c>
       <c r="AW18" s="2">
         <v>1</v>
       </c>
       <c r="AX18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY18" s="2"/>
       <c r="AZ18" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="BA18" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BB18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD18" s="2">
         <v>0</v>
@@ -5457,7 +5457,7 @@
         <v>0</v>
       </c>
       <c r="BG18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH18" s="2">
         <v>1</v>
@@ -5481,7 +5481,7 @@
         <v>0</v>
       </c>
       <c r="BO18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BP18" s="2">
         <v>0</v>
@@ -5505,7 +5505,7 @@
         <v>0</v>
       </c>
       <c r="BW18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX18" s="2">
         <v>0</v>
@@ -5529,7 +5529,7 @@
         <v>0</v>
       </c>
       <c r="CE18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF18" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Wed and Thurs results
</commit_message>
<xml_diff>
--- a/datasets/analysis_dataset.xlsx
+++ b/datasets/analysis_dataset.xlsx
@@ -33,12 +33,12 @@
     <t>368</t>
   </si>
   <si>
+    <t>280</t>
+  </si>
+  <si>
     <t>424</t>
   </si>
   <si>
-    <t>280</t>
-  </si>
-  <si>
     <t>437</t>
   </si>
   <si>
@@ -51,24 +51,24 @@
     <t>193</t>
   </si>
   <si>
+    <t>253</t>
+  </si>
+  <si>
     <t>299</t>
   </si>
   <si>
-    <t>253</t>
-  </si>
-  <si>
     <t>644</t>
   </si>
   <si>
     <t>340</t>
   </si>
   <si>
+    <t>836</t>
+  </si>
+  <si>
     <t>555</t>
   </si>
   <si>
-    <t>836</t>
-  </si>
-  <si>
     <t>408</t>
   </si>
   <si>
@@ -258,12 +258,12 @@
     <t>syringe</t>
   </si>
   <si>
+    <t>pill</t>
+  </si>
+  <si>
     <t>spatula</t>
   </si>
   <si>
-    <t>pill</t>
-  </si>
-  <si>
     <t>swab</t>
   </si>
   <si>
@@ -348,12 +348,12 @@
     <t>tan</t>
   </si>
   <si>
+    <t>blue</t>
+  </si>
+  <si>
     <t>white</t>
   </si>
   <si>
-    <t>blue</t>
-  </si>
-  <si>
     <t>brown</t>
   </si>
   <si>
@@ -384,12 +384,12 @@
     <t>powder; chunky; shiny</t>
   </si>
   <si>
+    <t>fake pill</t>
+  </si>
+  <si>
     <t>crystals</t>
   </si>
   <si>
-    <t>fake pill</t>
-  </si>
-  <si>
     <t>tar</t>
   </si>
   <si>
@@ -486,10 +486,10 @@
     <t>fast acting</t>
   </si>
   <si>
+    <t>strong blues</t>
+  </si>
+  <si>
     <t>FTS = negative</t>
-  </si>
-  <si>
-    <t>strong blues</t>
   </si>
   <si>
     <t>overdose</t>
@@ -1073,7 +1073,7 @@
         <v>125</v>
       </c>
       <c r="Y1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z1" t="s">
         <v>120</v>
@@ -1082,7 +1082,7 @@
         <v>126</v>
       </c>
       <c r="AB1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AC1" t="s">
         <v>127</v>
@@ -2563,7 +2563,7 @@
         <v>70</v>
       </c>
       <c r="G7" s="1">
-        <v>44484</v>
+        <v>44701</v>
       </c>
       <c r="H7" t="s">
         <v>81</v>
@@ -2575,13 +2575,13 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="L7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7" s="2">
         <v>0</v>
@@ -2602,22 +2602,22 @@
         <v>0</v>
       </c>
       <c r="T7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U7" t="s">
         <v>111</v>
       </c>
       <c r="V7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W7" t="s">
-        <v>120</v>
+        <v>81</v>
       </c>
       <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="2">
-        <v>1</v>
-      </c>
+      <c r="Y7" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
@@ -2638,12 +2638,14 @@
         <v>108</v>
       </c>
       <c r="AP7" t="s">
-        <v>108</v>
+        <v>155</v>
       </c>
       <c r="AQ7" t="s">
-        <v>79</v>
-      </c>
-      <c r="AR7" s="2"/>
+        <v>160</v>
+      </c>
+      <c r="AR7" s="2">
+        <v>0</v>
+      </c>
       <c r="AS7" t="s">
         <v>108</v>
       </c>
@@ -2652,32 +2654,32 @@
         <v>0</v>
       </c>
       <c r="AV7" s="1">
-        <v>44603</v>
+        <v>44721</v>
       </c>
       <c r="AW7" s="2">
         <v>1</v>
       </c>
       <c r="AX7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY7" s="2"/>
       <c r="AZ7" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="BA7" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="BB7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF7" s="2">
         <v>0</v>
@@ -2686,7 +2688,7 @@
         <v>0</v>
       </c>
       <c r="BH7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI7" s="2">
         <v>0</v>
@@ -2695,7 +2697,7 @@
         <v>0</v>
       </c>
       <c r="BK7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL7" s="2">
         <v>0</v>
@@ -2731,7 +2733,7 @@
         <v>0</v>
       </c>
       <c r="BW7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX7" s="2">
         <v>0</v>
@@ -2746,7 +2748,7 @@
         <v>0</v>
       </c>
       <c r="CB7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CC7" s="2">
         <v>0</v>
@@ -2755,13 +2757,13 @@
         <v>0</v>
       </c>
       <c r="CE7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CH7" t="s">
         <v>47</v>
@@ -2811,7 +2813,7 @@
         <v>70</v>
       </c>
       <c r="G8" s="1">
-        <v>44701</v>
+        <v>44484</v>
       </c>
       <c r="H8" t="s">
         <v>82</v>
@@ -2823,13 +2825,13 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="L8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8" s="2">
         <v>0</v>
@@ -2850,22 +2852,22 @@
         <v>0</v>
       </c>
       <c r="T8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U8" t="s">
         <v>112</v>
       </c>
       <c r="V8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W8" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
       <c r="X8" s="2"/>
-      <c r="Y8" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2">
+        <v>1</v>
+      </c>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
@@ -2886,14 +2888,12 @@
         <v>108</v>
       </c>
       <c r="AP8" t="s">
-        <v>155</v>
+        <v>108</v>
       </c>
       <c r="AQ8" t="s">
-        <v>160</v>
-      </c>
-      <c r="AR8" s="2">
-        <v>0</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="AR8" s="2"/>
       <c r="AS8" t="s">
         <v>108</v>
       </c>
@@ -2902,32 +2902,32 @@
         <v>0</v>
       </c>
       <c r="AV8" s="1">
-        <v>44721</v>
+        <v>44603</v>
       </c>
       <c r="AW8" s="2">
         <v>1</v>
       </c>
       <c r="AX8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY8" s="2"/>
       <c r="AZ8" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="BA8" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="BB8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF8" s="2">
         <v>0</v>
@@ -2936,7 +2936,7 @@
         <v>0</v>
       </c>
       <c r="BH8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI8" s="2">
         <v>0</v>
@@ -2945,7 +2945,7 @@
         <v>0</v>
       </c>
       <c r="BK8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL8" s="2">
         <v>0</v>
@@ -2981,7 +2981,7 @@
         <v>0</v>
       </c>
       <c r="BW8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX8" s="2">
         <v>0</v>
@@ -2996,7 +2996,7 @@
         <v>0</v>
       </c>
       <c r="CB8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC8" s="2">
         <v>0</v>
@@ -3005,13 +3005,13 @@
         <v>0</v>
       </c>
       <c r="CE8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CG8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH8" t="s">
         <v>47</v>
@@ -3353,7 +3353,7 @@
         <v>0</v>
       </c>
       <c r="U10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V10" s="2">
         <v>0</v>
@@ -3818,10 +3818,10 @@
         <v>44883</v>
       </c>
       <c r="H12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J12" s="2">
         <v>1</v>
@@ -3857,7 +3857,7 @@
         <v>0</v>
       </c>
       <c r="U12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V12" s="2">
         <v>0</v>
@@ -4075,31 +4075,31 @@
         <v>72</v>
       </c>
       <c r="G13" s="1">
-        <v>44695</v>
+        <v>44707</v>
       </c>
       <c r="H13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J13" s="2">
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="L13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N13" s="2">
         <v>0</v>
       </c>
       <c r="O13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P13" s="2">
         <v>0</v>
@@ -4108,7 +4108,7 @@
         <v>0</v>
       </c>
       <c r="R13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S13" s="2">
         <v>0</v>
@@ -4117,7 +4117,7 @@
         <v>0</v>
       </c>
       <c r="U13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="V13" s="2">
         <v>0</v>
@@ -4168,7 +4168,7 @@
         <v>0</v>
       </c>
       <c r="AV13" s="1">
-        <v>44707</v>
+        <v>44714</v>
       </c>
       <c r="AW13" s="2">
         <v>1</v>
@@ -4178,22 +4178,22 @@
       </c>
       <c r="AY13" s="2"/>
       <c r="AZ13" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="BA13" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BB13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF13" s="2">
         <v>0</v>
@@ -4205,10 +4205,10 @@
         <v>0</v>
       </c>
       <c r="BI13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK13" s="2">
         <v>0</v>
@@ -4217,7 +4217,7 @@
         <v>0</v>
       </c>
       <c r="BM13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN13" s="2">
         <v>0</v>
@@ -4247,7 +4247,7 @@
         <v>0</v>
       </c>
       <c r="BW13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX13" s="2">
         <v>0</v>
@@ -4259,19 +4259,19 @@
         <v>0</v>
       </c>
       <c r="CA13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CB13" s="2">
         <v>1</v>
       </c>
       <c r="CC13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD13" s="2">
         <v>0</v>
       </c>
       <c r="CE13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF13" s="2">
         <v>0</v>
@@ -4323,31 +4323,31 @@
         <v>72</v>
       </c>
       <c r="G14" s="1">
-        <v>44707</v>
+        <v>44695</v>
       </c>
       <c r="H14" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J14" s="2">
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="L14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14" s="2">
         <v>0</v>
       </c>
       <c r="O14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P14" s="2">
         <v>0</v>
@@ -4356,7 +4356,7 @@
         <v>0</v>
       </c>
       <c r="R14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S14" s="2">
         <v>0</v>
@@ -4365,7 +4365,7 @@
         <v>0</v>
       </c>
       <c r="U14" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="V14" s="2">
         <v>0</v>
@@ -4416,7 +4416,7 @@
         <v>0</v>
       </c>
       <c r="AV14" s="1">
-        <v>44714</v>
+        <v>44707</v>
       </c>
       <c r="AW14" s="2">
         <v>1</v>
@@ -4426,22 +4426,22 @@
       </c>
       <c r="AY14" s="2"/>
       <c r="AZ14" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="BA14" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="BB14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF14" s="2">
         <v>0</v>
@@ -4453,10 +4453,10 @@
         <v>0</v>
       </c>
       <c r="BI14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK14" s="2">
         <v>0</v>
@@ -4465,7 +4465,7 @@
         <v>0</v>
       </c>
       <c r="BM14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN14" s="2">
         <v>0</v>
@@ -4495,7 +4495,7 @@
         <v>0</v>
       </c>
       <c r="BW14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX14" s="2">
         <v>0</v>
@@ -4507,19 +4507,19 @@
         <v>0</v>
       </c>
       <c r="CA14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB14" s="2">
         <v>1</v>
       </c>
       <c r="CC14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CD14" s="2">
         <v>0</v>
       </c>
       <c r="CE14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF14" s="2">
         <v>0</v>
@@ -4613,7 +4613,7 @@
         <v>0</v>
       </c>
       <c r="U15" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V15" s="2">
         <v>0</v>
@@ -5077,37 +5077,37 @@
         <v>73</v>
       </c>
       <c r="G17" s="1">
-        <v>44797</v>
+        <v>44871</v>
       </c>
       <c r="H17" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I17" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="J17" s="2">
         <v>1</v>
       </c>
       <c r="K17" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N17" s="2">
         <v>0</v>
       </c>
       <c r="O17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P17" s="2">
         <v>0</v>
       </c>
       <c r="Q17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R17" s="2">
         <v>0</v>
@@ -5119,24 +5119,24 @@
         <v>0</v>
       </c>
       <c r="U17" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="V17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W17" t="s">
         <v>123</v>
       </c>
       <c r="X17" s="2"/>
-      <c r="Y17" s="2"/>
+      <c r="Y17" s="2">
+        <v>1</v>
+      </c>
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
-      <c r="AB17" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB17" s="2"/>
       <c r="AC17" s="2"/>
       <c r="AD17" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="AE17" s="2">
         <v>1</v>
@@ -5145,13 +5145,17 @@
       <c r="AG17" s="2"/>
       <c r="AH17" s="2"/>
       <c r="AI17" s="2"/>
-      <c r="AJ17" s="2"/>
-      <c r="AK17" s="2"/>
+      <c r="AJ17" s="2">
+        <v>1</v>
+      </c>
+      <c r="AK17" s="2">
+        <v>1</v>
+      </c>
       <c r="AL17" s="2"/>
       <c r="AM17" s="2"/>
       <c r="AN17" s="2"/>
       <c r="AO17" t="s">
-        <v>150</v>
+        <v>108</v>
       </c>
       <c r="AP17" t="s">
         <v>157</v>
@@ -5170,26 +5174,26 @@
         <v>1</v>
       </c>
       <c r="AV17" s="1">
-        <v>44803</v>
+        <v>44879</v>
       </c>
       <c r="AW17" s="2">
         <v>1</v>
       </c>
       <c r="AX17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY17" s="2"/>
       <c r="AZ17" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="BA17" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BB17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD17" s="2">
         <v>0</v>
@@ -5201,7 +5205,7 @@
         <v>0</v>
       </c>
       <c r="BG17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH17" s="2">
         <v>1</v>
@@ -5225,7 +5229,7 @@
         <v>0</v>
       </c>
       <c r="BO17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BP17" s="2">
         <v>0</v>
@@ -5249,7 +5253,7 @@
         <v>0</v>
       </c>
       <c r="BW17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX17" s="2">
         <v>0</v>
@@ -5273,7 +5277,7 @@
         <v>0</v>
       </c>
       <c r="CE17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF17" s="2">
         <v>0</v>
@@ -5329,37 +5333,37 @@
         <v>73</v>
       </c>
       <c r="G18" s="1">
-        <v>44871</v>
+        <v>44797</v>
       </c>
       <c r="H18" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I18" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J18" s="2">
         <v>1</v>
       </c>
       <c r="K18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N18" s="2">
         <v>0</v>
       </c>
       <c r="O18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P18" s="2">
         <v>0</v>
       </c>
       <c r="Q18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R18" s="2">
         <v>0</v>
@@ -5371,24 +5375,24 @@
         <v>0</v>
       </c>
       <c r="U18" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="V18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W18" t="s">
         <v>124</v>
       </c>
       <c r="X18" s="2"/>
-      <c r="Y18" s="2">
-        <v>1</v>
-      </c>
+      <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
-      <c r="AB18" s="2"/>
+      <c r="AB18" s="2">
+        <v>1</v>
+      </c>
       <c r="AC18" s="2"/>
       <c r="AD18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AE18" s="2">
         <v>1</v>
@@ -5397,17 +5401,13 @@
       <c r="AG18" s="2"/>
       <c r="AH18" s="2"/>
       <c r="AI18" s="2"/>
-      <c r="AJ18" s="2">
-        <v>1</v>
-      </c>
-      <c r="AK18" s="2">
-        <v>1</v>
-      </c>
+      <c r="AJ18" s="2"/>
+      <c r="AK18" s="2"/>
       <c r="AL18" s="2"/>
       <c r="AM18" s="2"/>
       <c r="AN18" s="2"/>
       <c r="AO18" t="s">
-        <v>108</v>
+        <v>150</v>
       </c>
       <c r="AP18" t="s">
         <v>158</v>
@@ -5426,26 +5426,26 @@
         <v>1</v>
       </c>
       <c r="AV18" s="1">
-        <v>44879</v>
+        <v>44803</v>
       </c>
       <c r="AW18" s="2">
         <v>1</v>
       </c>
       <c r="AX18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY18" s="2"/>
       <c r="AZ18" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="BA18" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="BB18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD18" s="2">
         <v>0</v>
@@ -5457,7 +5457,7 @@
         <v>0</v>
       </c>
       <c r="BG18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BH18" s="2">
         <v>1</v>
@@ -5481,7 +5481,7 @@
         <v>0</v>
       </c>
       <c r="BO18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP18" s="2">
         <v>0</v>
@@ -5505,7 +5505,7 @@
         <v>0</v>
       </c>
       <c r="BW18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX18" s="2">
         <v>0</v>
@@ -5529,7 +5529,7 @@
         <v>0</v>
       </c>
       <c r="CE18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF18" s="2">
         <v>0</v>
@@ -5844,10 +5844,10 @@
         <v>44727</v>
       </c>
       <c r="H20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J20" s="2">
         <v>1</v>
@@ -5883,7 +5883,7 @@
         <v>0</v>
       </c>
       <c r="U20" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V20" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Thursday pending and counts update
Code fixes for blank rows
</commit_message>
<xml_diff>
--- a/datasets/analysis_dataset.xlsx
+++ b/datasets/analysis_dataset.xlsx
@@ -33,12 +33,12 @@
     <t>368</t>
   </si>
   <si>
+    <t>424</t>
+  </si>
+  <si>
     <t>280</t>
   </si>
   <si>
-    <t>424</t>
-  </si>
-  <si>
     <t>437</t>
   </si>
   <si>
@@ -51,12 +51,12 @@
     <t>193</t>
   </si>
   <si>
+    <t>253</t>
+  </si>
+  <si>
     <t>299</t>
   </si>
   <si>
-    <t>253</t>
-  </si>
-  <si>
     <t>644</t>
   </si>
   <si>
@@ -258,12 +258,12 @@
     <t>syringe</t>
   </si>
   <si>
+    <t>spatula</t>
+  </si>
+  <si>
     <t>pill</t>
   </si>
   <si>
-    <t>spatula</t>
-  </si>
-  <si>
     <t>swab</t>
   </si>
   <si>
@@ -348,10 +348,10 @@
     <t>tan</t>
   </si>
   <si>
+    <t>white</t>
+  </si>
+  <si>
     <t>blue</t>
-  </si>
-  <si>
-    <t>white</t>
   </si>
   <si>
     <t>brown</t>
@@ -1073,7 +1073,7 @@
         <v>125</v>
       </c>
       <c r="Y1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="Z1" t="s">
         <v>120</v>
@@ -2563,7 +2563,7 @@
         <v>70</v>
       </c>
       <c r="G7" s="1">
-        <v>44701</v>
+        <v>44484</v>
       </c>
       <c r="H7" t="s">
         <v>81</v>
@@ -2575,13 +2575,13 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="L7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7" s="2">
         <v>0</v>
@@ -2602,22 +2602,22 @@
         <v>0</v>
       </c>
       <c r="T7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U7" t="s">
         <v>111</v>
       </c>
       <c r="V7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W7" t="s">
-        <v>81</v>
+        <v>120</v>
       </c>
       <c r="X7" s="2"/>
-      <c r="Y7" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2">
+        <v>1</v>
+      </c>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
@@ -2638,14 +2638,12 @@
         <v>108</v>
       </c>
       <c r="AP7" t="s">
-        <v>155</v>
+        <v>108</v>
       </c>
       <c r="AQ7" t="s">
-        <v>160</v>
-      </c>
-      <c r="AR7" s="2">
-        <v>0</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="AR7" s="2"/>
       <c r="AS7" t="s">
         <v>108</v>
       </c>
@@ -2654,32 +2652,32 @@
         <v>0</v>
       </c>
       <c r="AV7" s="1">
-        <v>44721</v>
+        <v>44603</v>
       </c>
       <c r="AW7" s="2">
         <v>1</v>
       </c>
       <c r="AX7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY7" s="2"/>
       <c r="AZ7" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="BA7" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="BB7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF7" s="2">
         <v>0</v>
@@ -2688,7 +2686,7 @@
         <v>0</v>
       </c>
       <c r="BH7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI7" s="2">
         <v>0</v>
@@ -2697,7 +2695,7 @@
         <v>0</v>
       </c>
       <c r="BK7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL7" s="2">
         <v>0</v>
@@ -2733,7 +2731,7 @@
         <v>0</v>
       </c>
       <c r="BW7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX7" s="2">
         <v>0</v>
@@ -2748,7 +2746,7 @@
         <v>0</v>
       </c>
       <c r="CB7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC7" s="2">
         <v>0</v>
@@ -2757,13 +2755,13 @@
         <v>0</v>
       </c>
       <c r="CE7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CG7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH7" t="s">
         <v>47</v>
@@ -2813,7 +2811,7 @@
         <v>70</v>
       </c>
       <c r="G8" s="1">
-        <v>44484</v>
+        <v>44701</v>
       </c>
       <c r="H8" t="s">
         <v>82</v>
@@ -2825,13 +2823,13 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="L8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8" s="2">
         <v>0</v>
@@ -2852,22 +2850,22 @@
         <v>0</v>
       </c>
       <c r="T8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8" t="s">
         <v>112</v>
       </c>
       <c r="V8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W8" t="s">
-        <v>120</v>
+        <v>82</v>
       </c>
       <c r="X8" s="2"/>
-      <c r="Y8" s="2"/>
-      <c r="Z8" s="2">
-        <v>1</v>
-      </c>
+      <c r="Y8" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
@@ -2888,12 +2886,14 @@
         <v>108</v>
       </c>
       <c r="AP8" t="s">
-        <v>108</v>
+        <v>155</v>
       </c>
       <c r="AQ8" t="s">
-        <v>79</v>
-      </c>
-      <c r="AR8" s="2"/>
+        <v>160</v>
+      </c>
+      <c r="AR8" s="2">
+        <v>0</v>
+      </c>
       <c r="AS8" t="s">
         <v>108</v>
       </c>
@@ -2902,32 +2902,32 @@
         <v>0</v>
       </c>
       <c r="AV8" s="1">
-        <v>44603</v>
+        <v>44721</v>
       </c>
       <c r="AW8" s="2">
         <v>1</v>
       </c>
       <c r="AX8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY8" s="2"/>
       <c r="AZ8" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="BA8" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="BB8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF8" s="2">
         <v>0</v>
@@ -2936,7 +2936,7 @@
         <v>0</v>
       </c>
       <c r="BH8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI8" s="2">
         <v>0</v>
@@ -2945,7 +2945,7 @@
         <v>0</v>
       </c>
       <c r="BK8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL8" s="2">
         <v>0</v>
@@ -2981,7 +2981,7 @@
         <v>0</v>
       </c>
       <c r="BW8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX8" s="2">
         <v>0</v>
@@ -2996,7 +2996,7 @@
         <v>0</v>
       </c>
       <c r="CB8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CC8" s="2">
         <v>0</v>
@@ -3005,13 +3005,13 @@
         <v>0</v>
       </c>
       <c r="CE8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CH8" t="s">
         <v>47</v>
@@ -3353,7 +3353,7 @@
         <v>0</v>
       </c>
       <c r="U10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V10" s="2">
         <v>0</v>
@@ -3818,10 +3818,10 @@
         <v>44883</v>
       </c>
       <c r="H12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J12" s="2">
         <v>1</v>
@@ -3857,7 +3857,7 @@
         <v>0</v>
       </c>
       <c r="U12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V12" s="2">
         <v>0</v>
@@ -4075,31 +4075,31 @@
         <v>72</v>
       </c>
       <c r="G13" s="1">
-        <v>44695</v>
+        <v>44707</v>
       </c>
       <c r="H13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J13" s="2">
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="L13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N13" s="2">
         <v>0</v>
       </c>
       <c r="O13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P13" s="2">
         <v>0</v>
@@ -4108,7 +4108,7 @@
         <v>0</v>
       </c>
       <c r="R13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S13" s="2">
         <v>0</v>
@@ -4117,7 +4117,7 @@
         <v>0</v>
       </c>
       <c r="U13" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="V13" s="2">
         <v>0</v>
@@ -4168,7 +4168,7 @@
         <v>0</v>
       </c>
       <c r="AV13" s="1">
-        <v>44707</v>
+        <v>44714</v>
       </c>
       <c r="AW13" s="2">
         <v>1</v>
@@ -4178,22 +4178,22 @@
       </c>
       <c r="AY13" s="2"/>
       <c r="AZ13" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="BA13" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BB13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF13" s="2">
         <v>0</v>
@@ -4205,10 +4205,10 @@
         <v>0</v>
       </c>
       <c r="BI13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK13" s="2">
         <v>0</v>
@@ -4217,7 +4217,7 @@
         <v>0</v>
       </c>
       <c r="BM13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN13" s="2">
         <v>0</v>
@@ -4247,7 +4247,7 @@
         <v>0</v>
       </c>
       <c r="BW13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX13" s="2">
         <v>0</v>
@@ -4259,19 +4259,19 @@
         <v>0</v>
       </c>
       <c r="CA13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CB13" s="2">
         <v>1</v>
       </c>
       <c r="CC13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD13" s="2">
         <v>0</v>
       </c>
       <c r="CE13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF13" s="2">
         <v>0</v>
@@ -4323,31 +4323,31 @@
         <v>72</v>
       </c>
       <c r="G14" s="1">
-        <v>44707</v>
+        <v>44695</v>
       </c>
       <c r="H14" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J14" s="2">
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="L14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14" s="2">
         <v>0</v>
       </c>
       <c r="O14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P14" s="2">
         <v>0</v>
@@ -4356,7 +4356,7 @@
         <v>0</v>
       </c>
       <c r="R14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S14" s="2">
         <v>0</v>
@@ -4365,7 +4365,7 @@
         <v>0</v>
       </c>
       <c r="U14" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="V14" s="2">
         <v>0</v>
@@ -4416,7 +4416,7 @@
         <v>0</v>
       </c>
       <c r="AV14" s="1">
-        <v>44714</v>
+        <v>44707</v>
       </c>
       <c r="AW14" s="2">
         <v>1</v>
@@ -4426,22 +4426,22 @@
       </c>
       <c r="AY14" s="2"/>
       <c r="AZ14" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="BA14" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="BB14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF14" s="2">
         <v>0</v>
@@ -4453,10 +4453,10 @@
         <v>0</v>
       </c>
       <c r="BI14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK14" s="2">
         <v>0</v>
@@ -4465,7 +4465,7 @@
         <v>0</v>
       </c>
       <c r="BM14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN14" s="2">
         <v>0</v>
@@ -4495,7 +4495,7 @@
         <v>0</v>
       </c>
       <c r="BW14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX14" s="2">
         <v>0</v>
@@ -4507,19 +4507,19 @@
         <v>0</v>
       </c>
       <c r="CA14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB14" s="2">
         <v>1</v>
       </c>
       <c r="CC14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CD14" s="2">
         <v>0</v>
       </c>
       <c r="CE14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF14" s="2">
         <v>0</v>
@@ -4613,7 +4613,7 @@
         <v>0</v>
       </c>
       <c r="U15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V15" s="2">
         <v>0</v>
@@ -5332,10 +5332,10 @@
         <v>44871</v>
       </c>
       <c r="H18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J18" s="2">
         <v>1</v>
@@ -5371,7 +5371,7 @@
         <v>0</v>
       </c>
       <c r="U18" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V18" s="2">
         <v>1</v>
@@ -5844,10 +5844,10 @@
         <v>44727</v>
       </c>
       <c r="H20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J20" s="2">
         <v>1</v>
@@ -5883,7 +5883,7 @@
         <v>0</v>
       </c>
       <c r="U20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V20" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Tuesday and Wednesday results
</commit_message>
<xml_diff>
--- a/datasets/analysis_dataset.xlsx
+++ b/datasets/analysis_dataset.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0"/>
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="554" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="454">
   <si>
     <t>sampleid</t>
   </si>
@@ -33,12 +33,12 @@
     <t>368</t>
   </si>
   <si>
+    <t>424</t>
+  </si>
+  <si>
     <t>280</t>
   </si>
   <si>
-    <t>424</t>
-  </si>
-  <si>
     <t>437</t>
   </si>
   <si>
@@ -51,12 +51,12 @@
     <t>193</t>
   </si>
   <si>
+    <t>299</t>
+  </si>
+  <si>
     <t>253</t>
   </si>
   <si>
-    <t>299</t>
-  </si>
-  <si>
     <t>644</t>
   </si>
   <si>
@@ -159,6 +159,9 @@
     <t>Guilford County</t>
   </si>
   <si>
+    <t>Pitt County</t>
+  </si>
+  <si>
     <t>Randolph County</t>
   </si>
   <si>
@@ -255,27 +258,111 @@
     <t>unknown</t>
   </si>
   <si>
+    <t>cotton</t>
+  </si>
+  <si>
     <t>syringe</t>
   </si>
   <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>spatula</t>
+  </si>
+  <si>
     <t>pill</t>
   </si>
   <si>
+    <t>swab</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
     <t>spatula</t>
   </si>
   <si>
+    <t>swab; spatula</t>
+  </si>
+  <si>
     <t>swab</t>
   </si>
   <si>
-    <t>swab; spatula</t>
+    <t>cotton</t>
+  </si>
+  <si>
+    <t>pill</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>cotton</t>
+  </si>
+  <si>
+    <t>spatula</t>
+  </si>
+  <si>
+    <t>unknown</t>
   </si>
   <si>
     <t>collection</t>
   </si>
   <si>
+    <t>cotton</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>cotton</t>
+  </si>
+  <si>
+    <t>syringe</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>spatula</t>
+  </si>
+  <si>
+    <t>pill</t>
+  </si>
+  <si>
+    <t>swab</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>spatula</t>
+  </si>
+  <si>
     <t>multiple methods</t>
   </si>
   <si>
+    <t>swab</t>
+  </si>
+  <si>
+    <t>cotton</t>
+  </si>
+  <si>
+    <t>pill</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>cotton</t>
+  </si>
+  <si>
+    <t>spatula</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
     <t>consumed</t>
   </si>
   <si>
@@ -288,21 +375,54 @@
     <t>methamphetamine</t>
   </si>
   <si>
+    <t>heroin; fentanyl</t>
+  </si>
+  <si>
     <t>fentanyl</t>
   </si>
   <si>
+    <t>heroin; fentanyl</t>
+  </si>
+  <si>
     <t>MDMA</t>
   </si>
   <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>heroin; fentanyl</t>
+  </si>
+  <si>
+    <t>MDMA</t>
+  </si>
+  <si>
     <t>cocaine</t>
   </si>
   <si>
+    <t>heroin; fentanyl</t>
+  </si>
+  <si>
     <t>crack</t>
   </si>
   <si>
+    <t>heroin; fentanyl</t>
+  </si>
+  <si>
     <t>heroin</t>
   </si>
   <si>
+    <t>fentanyl</t>
+  </si>
+  <si>
+    <t>methamphetamine</t>
+  </si>
+  <si>
+    <t>fentanyl</t>
+  </si>
+  <si>
+    <t>heroin</t>
+  </si>
+  <si>
     <t>expect_opioid</t>
   </si>
   <si>
@@ -348,21 +468,45 @@
     <t>tan</t>
   </si>
   <si>
+    <t>white</t>
+  </si>
+  <si>
     <t>blue</t>
   </si>
   <si>
+    <t>unknown</t>
+  </si>
+  <si>
     <t>white</t>
   </si>
   <si>
     <t>brown</t>
   </si>
   <si>
+    <t>white</t>
+  </si>
+  <si>
     <t>light gray</t>
   </si>
   <si>
+    <t>white</t>
+  </si>
+  <si>
     <t>gray; brown</t>
   </si>
   <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>clear</t>
+  </si>
+  <si>
+    <t>brown</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
     <t>light brown</t>
   </si>
   <si>
@@ -372,30 +516,69 @@
     <t>texture</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>crystals; powder; chunky</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>powder</t>
   </si>
   <si>
     <t>powder; chunky</t>
   </si>
   <si>
+    <t>powder</t>
+  </si>
+  <si>
+    <t>pill</t>
+  </si>
+  <si>
+    <t>powder</t>
+  </si>
+  <si>
+    <t>powder; chunky</t>
+  </si>
+  <si>
     <t>powder; chunky; shiny</t>
   </si>
   <si>
+    <t>powder</t>
+  </si>
+  <si>
+    <t>powder; chunky</t>
+  </si>
+  <si>
+    <t>powder</t>
+  </si>
+  <si>
     <t>fake pill</t>
   </si>
   <si>
     <t>crystals</t>
   </si>
   <si>
+    <t>powder</t>
+  </si>
+  <si>
     <t>tar</t>
   </si>
   <si>
+    <t>pill</t>
+  </si>
+  <si>
+    <t>powder</t>
+  </si>
+  <si>
     <t>plant</t>
   </si>
   <si>
+    <t>crystals</t>
+  </si>
+  <si>
     <t>lustre</t>
   </si>
   <si>
@@ -411,21 +594,54 @@
     <t>normal</t>
   </si>
   <si>
+    <t>weird</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>normal; stronger</t>
   </si>
   <si>
+    <t>weird</t>
+  </si>
+  <si>
     <t>stronger; more up; unpleasant</t>
   </si>
   <si>
+    <t>normal</t>
+  </si>
+  <si>
     <t>stronger</t>
   </si>
   <si>
+    <t>weird</t>
+  </si>
+  <si>
     <t>nice; stronger; long</t>
   </si>
   <si>
+    <t>stronger</t>
+  </si>
+  <si>
     <t>weird; weaker; unpleasant</t>
   </si>
   <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>weird</t>
+  </si>
+  <si>
     <t>sen_strength</t>
   </si>
   <si>
@@ -462,60 +678,228 @@
     <t>cotton appears black</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>heroin from powder</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>brittle, opaque, crumbly</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>sensation_notes</t>
   </si>
   <si>
     <t>bad abscesses</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>Ostensibly fentanyl. Thinks not but very weird</t>
   </si>
   <si>
     <t>different color than usual</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>?</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>fast acting</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>strong blues</t>
   </si>
   <si>
     <t>FTS = negative</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>overdose</t>
   </si>
   <si>
     <t>not overdose related</t>
   </si>
   <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>not overdose related</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>not overdose related</t>
+  </si>
+  <si>
     <t>involved in OD</t>
   </si>
   <si>
+    <t>not overdose related</t>
+  </si>
+  <si>
+    <t>involved in OD</t>
+  </si>
+  <si>
+    <t>not overdose related</t>
+  </si>
+  <si>
+    <t>involved in OD</t>
+  </si>
+  <si>
+    <t>not overdose related</t>
+  </si>
+  <si>
     <t>od</t>
   </si>
   <si>
     <t>overdose_notes</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>seizures</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>fall out v quickly ear ringing after reversal 80% who used OD'd</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>rapid fall out person sober for 3+ years. 2 doses naloxone</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>fatal_od</t>
   </si>
   <si>
@@ -642,7 +1026,52 @@
     <t>Grand Traverse County</t>
   </si>
   <si>
+    <t>Missoula County</t>
+  </si>
+  <si>
+    <t>Buncombe County</t>
+  </si>
+  <si>
+    <t>Catawba County</t>
+  </si>
+  <si>
+    <t>Guilford County</t>
+  </si>
+  <si>
+    <t>Pitt County</t>
+  </si>
+  <si>
+    <t>Randolph County</t>
+  </si>
+  <si>
+    <t>Guilford County</t>
+  </si>
+  <si>
+    <t>Santa Fe County</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>Albany County</t>
+  </si>
+  <si>
+    <t>Suffolk County</t>
+  </si>
+  <si>
+    <t>Multnomah County</t>
+  </si>
+  <si>
+    <t>Madison County</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>lat_program</t>
@@ -951,7 +1380,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -992,11 +1421,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:CP21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -1013,274 +1439,274 @@
         <v>41</v>
       </c>
       <c r="E1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I1" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="J1" t="s">
-        <v>87</v>
+        <v>116</v>
       </c>
       <c r="K1" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
       <c r="L1" t="s">
-        <v>96</v>
+        <v>136</v>
       </c>
       <c r="M1" t="s">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="N1" t="s">
-        <v>98</v>
+        <v>138</v>
       </c>
       <c r="O1" t="s">
-        <v>99</v>
+        <v>139</v>
       </c>
       <c r="P1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="Q1" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="R1" t="s">
-        <v>102</v>
+        <v>142</v>
       </c>
       <c r="S1" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="T1" t="s">
-        <v>104</v>
+        <v>144</v>
       </c>
       <c r="U1" t="s">
-        <v>105</v>
+        <v>145</v>
       </c>
       <c r="V1" t="s">
-        <v>117</v>
+        <v>165</v>
       </c>
       <c r="W1" t="s">
-        <v>118</v>
+        <v>166</v>
       </c>
       <c r="X1" t="s">
-        <v>125</v>
+        <v>183</v>
       </c>
       <c r="Y1" t="s">
-        <v>81</v>
+        <v>184</v>
       </c>
       <c r="Z1" t="s">
-        <v>120</v>
+        <v>185</v>
       </c>
       <c r="AA1" t="s">
-        <v>126</v>
+        <v>186</v>
       </c>
       <c r="AB1" t="s">
-        <v>124</v>
+        <v>187</v>
       </c>
       <c r="AC1" t="s">
-        <v>127</v>
+        <v>188</v>
       </c>
       <c r="AD1" t="s">
-        <v>128</v>
+        <v>189</v>
       </c>
       <c r="AE1" t="s">
-        <v>137</v>
+        <v>209</v>
       </c>
       <c r="AF1" t="s">
-        <v>138</v>
+        <v>210</v>
       </c>
       <c r="AG1" t="s">
-        <v>139</v>
+        <v>211</v>
       </c>
       <c r="AH1" t="s">
-        <v>140</v>
+        <v>212</v>
       </c>
       <c r="AI1" t="s">
-        <v>141</v>
+        <v>213</v>
       </c>
       <c r="AJ1" t="s">
-        <v>142</v>
+        <v>214</v>
       </c>
       <c r="AK1" t="s">
-        <v>143</v>
+        <v>215</v>
       </c>
       <c r="AL1" t="s">
-        <v>144</v>
+        <v>216</v>
       </c>
       <c r="AM1" t="s">
-        <v>145</v>
+        <v>217</v>
       </c>
       <c r="AN1" t="s">
-        <v>146</v>
+        <v>218</v>
       </c>
       <c r="AO1" t="s">
-        <v>147</v>
+        <v>219</v>
       </c>
       <c r="AP1" t="s">
-        <v>151</v>
+        <v>240</v>
       </c>
       <c r="AQ1" t="s">
-        <v>159</v>
+        <v>261</v>
       </c>
       <c r="AR1" t="s">
-        <v>162</v>
+        <v>273</v>
       </c>
       <c r="AS1" t="s">
-        <v>163</v>
+        <v>274</v>
       </c>
       <c r="AT1" t="s">
-        <v>167</v>
+        <v>295</v>
       </c>
       <c r="AU1" t="s">
-        <v>168</v>
+        <v>296</v>
       </c>
       <c r="AV1" t="s">
-        <v>169</v>
+        <v>297</v>
       </c>
       <c r="AW1" t="s">
-        <v>170</v>
+        <v>298</v>
       </c>
       <c r="AX1" t="s">
-        <v>171</v>
+        <v>299</v>
       </c>
       <c r="AY1" t="s">
-        <v>172</v>
+        <v>300</v>
       </c>
       <c r="AZ1" t="s">
-        <v>173</v>
+        <v>301</v>
       </c>
       <c r="BA1" t="s">
-        <v>174</v>
+        <v>302</v>
       </c>
       <c r="BB1" t="s">
-        <v>175</v>
+        <v>303</v>
       </c>
       <c r="BC1" t="s">
-        <v>176</v>
+        <v>304</v>
       </c>
       <c r="BD1" t="s">
-        <v>177</v>
+        <v>305</v>
       </c>
       <c r="BE1" t="s">
-        <v>178</v>
+        <v>306</v>
       </c>
       <c r="BF1" t="s">
-        <v>179</v>
+        <v>307</v>
       </c>
       <c r="BG1" t="s">
-        <v>180</v>
+        <v>308</v>
       </c>
       <c r="BH1" t="s">
-        <v>181</v>
+        <v>309</v>
       </c>
       <c r="BI1" t="s">
-        <v>182</v>
+        <v>310</v>
       </c>
       <c r="BJ1" t="s">
-        <v>183</v>
+        <v>311</v>
       </c>
       <c r="BK1" t="s">
-        <v>184</v>
+        <v>312</v>
       </c>
       <c r="BL1" t="s">
-        <v>185</v>
+        <v>313</v>
       </c>
       <c r="BM1" t="s">
-        <v>186</v>
+        <v>314</v>
       </c>
       <c r="BN1" t="s">
-        <v>187</v>
+        <v>315</v>
       </c>
       <c r="BO1" t="s">
-        <v>188</v>
+        <v>316</v>
       </c>
       <c r="BP1" t="s">
-        <v>189</v>
+        <v>317</v>
       </c>
       <c r="BQ1" t="s">
-        <v>190</v>
+        <v>318</v>
       </c>
       <c r="BR1" t="s">
-        <v>191</v>
+        <v>319</v>
       </c>
       <c r="BS1" t="s">
-        <v>192</v>
+        <v>320</v>
       </c>
       <c r="BT1" t="s">
-        <v>193</v>
+        <v>321</v>
       </c>
       <c r="BU1" t="s">
-        <v>194</v>
+        <v>322</v>
       </c>
       <c r="BV1" t="s">
-        <v>195</v>
+        <v>323</v>
       </c>
       <c r="BW1" t="s">
-        <v>196</v>
+        <v>324</v>
       </c>
       <c r="BX1" t="s">
-        <v>197</v>
+        <v>325</v>
       </c>
       <c r="BY1" t="s">
-        <v>198</v>
+        <v>326</v>
       </c>
       <c r="BZ1" t="s">
-        <v>199</v>
+        <v>327</v>
       </c>
       <c r="CA1" t="s">
-        <v>200</v>
+        <v>328</v>
       </c>
       <c r="CB1" t="s">
-        <v>201</v>
+        <v>329</v>
       </c>
       <c r="CC1" t="s">
-        <v>202</v>
+        <v>330</v>
       </c>
       <c r="CD1" t="s">
-        <v>203</v>
+        <v>331</v>
       </c>
       <c r="CE1" t="s">
-        <v>204</v>
+        <v>332</v>
       </c>
       <c r="CF1" t="s">
-        <v>205</v>
+        <v>333</v>
       </c>
       <c r="CG1" t="s">
-        <v>206</v>
+        <v>334</v>
       </c>
       <c r="CH1" t="s">
-        <v>207</v>
+        <v>335</v>
       </c>
       <c r="CI1" t="s">
-        <v>210</v>
+        <v>353</v>
       </c>
       <c r="CJ1" t="s">
-        <v>211</v>
+        <v>354</v>
       </c>
       <c r="CK1" t="s">
-        <v>212</v>
+        <v>355</v>
       </c>
       <c r="CL1" t="s">
-        <v>230</v>
+        <v>373</v>
       </c>
       <c r="CM1" t="s">
-        <v>248</v>
+        <v>391</v>
       </c>
       <c r="CN1" t="s">
-        <v>266</v>
+        <v>409</v>
       </c>
       <c r="CO1" t="s">
-        <v>275</v>
+        <v>418</v>
       </c>
       <c r="CP1" t="s">
-        <v>293</v>
+        <v>436</v>
       </c>
     </row>
     <row r="2">
@@ -1297,25 +1723,25 @@
         <v>42</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G2" s="1">
         <v>44854</v>
       </c>
       <c r="H2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I2" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="J2" s="2">
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>89</v>
+        <v>118</v>
       </c>
       <c r="L2" s="2">
         <v>1</v>
@@ -1345,13 +1771,13 @@
         <v>0</v>
       </c>
       <c r="U2" t="s">
-        <v>106</v>
+        <v>146</v>
       </c>
       <c r="V2" s="2">
         <v>0</v>
       </c>
       <c r="W2" t="s">
-        <v>108</v>
+        <v>167</v>
       </c>
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
@@ -1360,7 +1786,7 @@
       <c r="AB2" s="2"/>
       <c r="AC2" s="2"/>
       <c r="AD2" t="s">
-        <v>129</v>
+        <v>190</v>
       </c>
       <c r="AE2" s="2"/>
       <c r="AF2" s="2">
@@ -1377,19 +1803,19 @@
       </c>
       <c r="AN2" s="2"/>
       <c r="AO2" t="s">
-        <v>148</v>
+        <v>220</v>
       </c>
       <c r="AP2" t="s">
-        <v>152</v>
+        <v>241</v>
       </c>
       <c r="AQ2" t="s">
-        <v>160</v>
+        <v>262</v>
       </c>
       <c r="AR2" s="2">
         <v>0</v>
       </c>
       <c r="AS2" t="s">
-        <v>108</v>
+        <v>275</v>
       </c>
       <c r="AT2" s="2"/>
       <c r="AU2" s="2">
@@ -1508,7 +1934,7 @@
         <v>0</v>
       </c>
       <c r="CH2" t="s">
-        <v>208</v>
+        <v>336</v>
       </c>
       <c r="CI2" s="2">
         <v>44.7606441</v>
@@ -1517,22 +1943,22 @@
         <v>-85.616530100000006</v>
       </c>
       <c r="CK2" t="s">
-        <v>213</v>
+        <v>356</v>
       </c>
       <c r="CL2" t="s">
-        <v>231</v>
+        <v>374</v>
       </c>
       <c r="CM2" t="s">
-        <v>249</v>
+        <v>392</v>
       </c>
       <c r="CN2" t="s">
-        <v>267</v>
+        <v>410</v>
       </c>
       <c r="CO2" t="s">
-        <v>276</v>
+        <v>419</v>
       </c>
       <c r="CP2" t="s">
-        <v>294</v>
+        <v>437</v>
       </c>
     </row>
     <row r="3">
@@ -1549,25 +1975,25 @@
         <v>43</v>
       </c>
       <c r="E3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G3" s="1">
         <v>44875</v>
       </c>
       <c r="H3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I3" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="J3" s="2">
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="L3" s="2">
         <v>0</v>
@@ -1597,13 +2023,13 @@
         <v>0</v>
       </c>
       <c r="U3" t="s">
-        <v>107</v>
+        <v>147</v>
       </c>
       <c r="V3" s="2">
         <v>0</v>
       </c>
       <c r="W3" t="s">
-        <v>119</v>
+        <v>168</v>
       </c>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
@@ -1616,7 +2042,7 @@
       </c>
       <c r="AC3" s="2"/>
       <c r="AD3" t="s">
-        <v>130</v>
+        <v>191</v>
       </c>
       <c r="AE3" s="2">
         <v>-1</v>
@@ -1631,19 +2057,19 @@
       <c r="AM3" s="2"/>
       <c r="AN3" s="2"/>
       <c r="AO3" t="s">
-        <v>108</v>
+        <v>221</v>
       </c>
       <c r="AP3" t="s">
-        <v>108</v>
+        <v>242</v>
       </c>
       <c r="AQ3" t="s">
-        <v>160</v>
+        <v>262</v>
       </c>
       <c r="AR3" s="2">
         <v>0</v>
       </c>
       <c r="AS3" t="s">
-        <v>108</v>
+        <v>276</v>
       </c>
       <c r="AT3" s="2"/>
       <c r="AU3" s="2">
@@ -1762,7 +2188,7 @@
         <v>0</v>
       </c>
       <c r="CH3" t="s">
-        <v>43</v>
+        <v>337</v>
       </c>
       <c r="CI3" s="2">
         <v>46.870104900000001</v>
@@ -1771,22 +2197,22 @@
         <v>-113.995267</v>
       </c>
       <c r="CK3" t="s">
-        <v>214</v>
+        <v>357</v>
       </c>
       <c r="CL3" t="s">
-        <v>232</v>
+        <v>375</v>
       </c>
       <c r="CM3" t="s">
-        <v>250</v>
+        <v>393</v>
       </c>
       <c r="CN3" t="s">
-        <v>268</v>
+        <v>411</v>
       </c>
       <c r="CO3" t="s">
-        <v>277</v>
+        <v>420</v>
       </c>
       <c r="CP3" t="s">
-        <v>295</v>
+        <v>438</v>
       </c>
     </row>
     <row r="4">
@@ -1803,25 +2229,25 @@
         <v>44</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G4" s="1">
         <v>44888</v>
       </c>
       <c r="H4" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I4" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="J4" s="2">
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="L4" s="2">
         <v>0</v>
@@ -1851,13 +2277,13 @@
         <v>0</v>
       </c>
       <c r="U4" t="s">
-        <v>108</v>
+        <v>148</v>
       </c>
       <c r="V4" s="2">
         <v>0</v>
       </c>
       <c r="W4" t="s">
-        <v>108</v>
+        <v>169</v>
       </c>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
@@ -1866,7 +2292,7 @@
       <c r="AB4" s="2"/>
       <c r="AC4" s="2"/>
       <c r="AD4" t="s">
-        <v>131</v>
+        <v>192</v>
       </c>
       <c r="AE4" s="2">
         <v>0</v>
@@ -1881,19 +2307,19 @@
       <c r="AM4" s="2"/>
       <c r="AN4" s="2"/>
       <c r="AO4" t="s">
-        <v>108</v>
+        <v>222</v>
       </c>
       <c r="AP4" t="s">
-        <v>108</v>
+        <v>243</v>
       </c>
       <c r="AQ4" t="s">
-        <v>160</v>
+        <v>262</v>
       </c>
       <c r="AR4" s="2">
         <v>0</v>
       </c>
       <c r="AS4" t="s">
-        <v>108</v>
+        <v>277</v>
       </c>
       <c r="AT4" s="2"/>
       <c r="AU4" s="2">
@@ -2012,7 +2438,7 @@
         <v>0</v>
       </c>
       <c r="CH4" t="s">
-        <v>44</v>
+        <v>338</v>
       </c>
       <c r="CI4" s="2">
         <v>35.600949800000002</v>
@@ -2021,22 +2447,22 @@
         <v>-82.554016099999998</v>
       </c>
       <c r="CK4" t="s">
-        <v>215</v>
+        <v>358</v>
       </c>
       <c r="CL4" t="s">
-        <v>233</v>
+        <v>376</v>
       </c>
       <c r="CM4" t="s">
-        <v>251</v>
+        <v>394</v>
       </c>
       <c r="CN4" t="s">
-        <v>269</v>
+        <v>412</v>
       </c>
       <c r="CO4" t="s">
-        <v>278</v>
+        <v>421</v>
       </c>
       <c r="CP4" t="s">
-        <v>296</v>
+        <v>439</v>
       </c>
     </row>
     <row r="5">
@@ -2053,25 +2479,25 @@
         <v>45</v>
       </c>
       <c r="E5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G5" s="1">
         <v>44682</v>
       </c>
       <c r="H5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I5" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="J5" s="2">
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>89</v>
+        <v>120</v>
       </c>
       <c r="L5" s="2">
         <v>1</v>
@@ -2101,13 +2527,13 @@
         <v>0</v>
       </c>
       <c r="U5" t="s">
-        <v>109</v>
+        <v>149</v>
       </c>
       <c r="V5" s="2">
         <v>0</v>
       </c>
       <c r="W5" t="s">
-        <v>120</v>
+        <v>170</v>
       </c>
       <c r="X5" s="2"/>
       <c r="Y5" s="2"/>
@@ -2118,7 +2544,7 @@
       <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
       <c r="AD5" t="s">
-        <v>129</v>
+        <v>193</v>
       </c>
       <c r="AE5" s="2"/>
       <c r="AF5" s="2">
@@ -2133,17 +2559,17 @@
       <c r="AM5" s="2"/>
       <c r="AN5" s="2"/>
       <c r="AO5" t="s">
-        <v>149</v>
+        <v>223</v>
       </c>
       <c r="AP5" t="s">
-        <v>153</v>
+        <v>244</v>
       </c>
       <c r="AQ5" t="s">
-        <v>79</v>
+        <v>263</v>
       </c>
       <c r="AR5" s="2"/>
       <c r="AS5" t="s">
-        <v>108</v>
+        <v>278</v>
       </c>
       <c r="AT5" s="2"/>
       <c r="AU5" s="2">
@@ -2264,7 +2690,7 @@
         <v>0</v>
       </c>
       <c r="CH5" t="s">
-        <v>45</v>
+        <v>339</v>
       </c>
       <c r="CI5" s="2">
         <v>35.733331200000002</v>
@@ -2273,22 +2699,22 @@
         <v>-81.344291499999997</v>
       </c>
       <c r="CK5" t="s">
-        <v>216</v>
+        <v>359</v>
       </c>
       <c r="CL5" t="s">
-        <v>234</v>
+        <v>377</v>
       </c>
       <c r="CM5" t="s">
-        <v>252</v>
+        <v>395</v>
       </c>
       <c r="CN5" t="s">
-        <v>269</v>
+        <v>412</v>
       </c>
       <c r="CO5" t="s">
-        <v>279</v>
+        <v>422</v>
       </c>
       <c r="CP5" t="s">
-        <v>297</v>
+        <v>440</v>
       </c>
     </row>
     <row r="6">
@@ -2305,25 +2731,25 @@
         <v>46</v>
       </c>
       <c r="E6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G6" s="1">
         <v>44774</v>
       </c>
       <c r="H6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="I6" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="J6" s="2">
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>91</v>
+        <v>121</v>
       </c>
       <c r="L6" s="2">
         <v>1</v>
@@ -2353,13 +2779,13 @@
         <v>0</v>
       </c>
       <c r="U6" t="s">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="V6" s="2">
         <v>0</v>
       </c>
       <c r="W6" t="s">
-        <v>121</v>
+        <v>171</v>
       </c>
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
@@ -2370,7 +2796,7 @@
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
       <c r="AD6" t="s">
-        <v>131</v>
+        <v>194</v>
       </c>
       <c r="AE6" s="2">
         <v>0</v>
@@ -2385,19 +2811,19 @@
       <c r="AM6" s="2"/>
       <c r="AN6" s="2"/>
       <c r="AO6" t="s">
-        <v>108</v>
+        <v>224</v>
       </c>
       <c r="AP6" t="s">
-        <v>154</v>
+        <v>245</v>
       </c>
       <c r="AQ6" t="s">
-        <v>160</v>
+        <v>264</v>
       </c>
       <c r="AR6" s="2">
         <v>0</v>
       </c>
       <c r="AS6" t="s">
-        <v>108</v>
+        <v>279</v>
       </c>
       <c r="AT6" s="2"/>
       <c r="AU6" s="2">
@@ -2516,7 +2942,7 @@
         <v>0</v>
       </c>
       <c r="CH6" t="s">
-        <v>45</v>
+        <v>339</v>
       </c>
       <c r="CI6" s="2">
         <v>35.733331200000002</v>
@@ -2525,22 +2951,22 @@
         <v>-81.344291499999997</v>
       </c>
       <c r="CK6" t="s">
-        <v>217</v>
+        <v>360</v>
       </c>
       <c r="CL6" t="s">
-        <v>235</v>
+        <v>378</v>
       </c>
       <c r="CM6" t="s">
-        <v>253</v>
+        <v>396</v>
       </c>
       <c r="CN6" t="s">
-        <v>269</v>
+        <v>412</v>
       </c>
       <c r="CO6" t="s">
-        <v>280</v>
+        <v>423</v>
       </c>
       <c r="CP6" t="s">
-        <v>298</v>
+        <v>441</v>
       </c>
     </row>
     <row r="7">
@@ -2557,31 +2983,31 @@
         <v>47</v>
       </c>
       <c r="E7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G7" s="1">
-        <v>44701</v>
+        <v>44484</v>
       </c>
       <c r="H7" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I7" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="J7" s="2">
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>92</v>
+        <v>122</v>
       </c>
       <c r="L7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7" s="2">
         <v>0</v>
@@ -2602,27 +3028,27 @@
         <v>0</v>
       </c>
       <c r="T7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U7" t="s">
-        <v>111</v>
+        <v>151</v>
       </c>
       <c r="V7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W7" t="s">
-        <v>81</v>
+        <v>172</v>
       </c>
       <c r="X7" s="2"/>
-      <c r="Y7" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2">
+        <v>1</v>
+      </c>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
       <c r="AD7" t="s">
-        <v>108</v>
+        <v>195</v>
       </c>
       <c r="AE7" s="2"/>
       <c r="AF7" s="2"/>
@@ -2635,51 +3061,49 @@
       <c r="AM7" s="2"/>
       <c r="AN7" s="2"/>
       <c r="AO7" t="s">
-        <v>108</v>
+        <v>225</v>
       </c>
       <c r="AP7" t="s">
-        <v>155</v>
+        <v>246</v>
       </c>
       <c r="AQ7" t="s">
-        <v>160</v>
-      </c>
-      <c r="AR7" s="2">
-        <v>0</v>
-      </c>
+        <v>265</v>
+      </c>
+      <c r="AR7" s="2"/>
       <c r="AS7" t="s">
-        <v>108</v>
+        <v>280</v>
       </c>
       <c r="AT7" s="2"/>
       <c r="AU7" s="2">
         <v>0</v>
       </c>
       <c r="AV7" s="1">
-        <v>44721</v>
+        <v>44603</v>
       </c>
       <c r="AW7" s="2">
         <v>1</v>
       </c>
       <c r="AX7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY7" s="2"/>
       <c r="AZ7" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="BA7" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="BB7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF7" s="2">
         <v>0</v>
@@ -2688,7 +3112,7 @@
         <v>0</v>
       </c>
       <c r="BH7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI7" s="2">
         <v>0</v>
@@ -2697,7 +3121,7 @@
         <v>0</v>
       </c>
       <c r="BK7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL7" s="2">
         <v>0</v>
@@ -2733,7 +3157,7 @@
         <v>0</v>
       </c>
       <c r="BW7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX7" s="2">
         <v>0</v>
@@ -2748,7 +3172,7 @@
         <v>0</v>
       </c>
       <c r="CB7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC7" s="2">
         <v>0</v>
@@ -2757,16 +3181,16 @@
         <v>0</v>
       </c>
       <c r="CE7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CG7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH7" t="s">
-        <v>47</v>
+        <v>340</v>
       </c>
       <c r="CI7" s="2">
         <v>36.072635499999997</v>
@@ -2775,22 +3199,22 @@
         <v>-79.791975399999998</v>
       </c>
       <c r="CK7" t="s">
-        <v>218</v>
+        <v>361</v>
       </c>
       <c r="CL7" t="s">
-        <v>236</v>
+        <v>379</v>
       </c>
       <c r="CM7" t="s">
-        <v>254</v>
+        <v>397</v>
       </c>
       <c r="CN7" t="s">
-        <v>269</v>
+        <v>412</v>
       </c>
       <c r="CO7" t="s">
-        <v>281</v>
+        <v>424</v>
       </c>
       <c r="CP7" t="s">
-        <v>299</v>
+        <v>442</v>
       </c>
     </row>
     <row r="8">
@@ -2807,31 +3231,31 @@
         <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G8" s="1">
-        <v>44484</v>
+        <v>44701</v>
       </c>
       <c r="H8" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="I8" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="J8" s="2">
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="L8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8" s="2">
         <v>0</v>
@@ -2852,27 +3276,27 @@
         <v>0</v>
       </c>
       <c r="T8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8" t="s">
-        <v>112</v>
+        <v>152</v>
       </c>
       <c r="V8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W8" t="s">
-        <v>120</v>
+        <v>173</v>
       </c>
       <c r="X8" s="2"/>
-      <c r="Y8" s="2"/>
-      <c r="Z8" s="2">
-        <v>1</v>
-      </c>
+      <c r="Y8" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
       <c r="AD8" t="s">
-        <v>108</v>
+        <v>196</v>
       </c>
       <c r="AE8" s="2"/>
       <c r="AF8" s="2"/>
@@ -2885,49 +3309,51 @@
       <c r="AM8" s="2"/>
       <c r="AN8" s="2"/>
       <c r="AO8" t="s">
-        <v>108</v>
+        <v>226</v>
       </c>
       <c r="AP8" t="s">
-        <v>108</v>
+        <v>247</v>
       </c>
       <c r="AQ8" t="s">
-        <v>79</v>
-      </c>
-      <c r="AR8" s="2"/>
+        <v>266</v>
+      </c>
+      <c r="AR8" s="2">
+        <v>0</v>
+      </c>
       <c r="AS8" t="s">
-        <v>108</v>
+        <v>281</v>
       </c>
       <c r="AT8" s="2"/>
       <c r="AU8" s="2">
         <v>0</v>
       </c>
       <c r="AV8" s="1">
-        <v>44603</v>
+        <v>44721</v>
       </c>
       <c r="AW8" s="2">
         <v>1</v>
       </c>
       <c r="AX8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY8" s="2"/>
       <c r="AZ8" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="BA8" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="BB8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF8" s="2">
         <v>0</v>
@@ -2936,7 +3362,7 @@
         <v>0</v>
       </c>
       <c r="BH8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI8" s="2">
         <v>0</v>
@@ -2945,7 +3371,7 @@
         <v>0</v>
       </c>
       <c r="BK8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL8" s="2">
         <v>0</v>
@@ -2981,7 +3407,7 @@
         <v>0</v>
       </c>
       <c r="BW8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX8" s="2">
         <v>0</v>
@@ -2996,7 +3422,7 @@
         <v>0</v>
       </c>
       <c r="CB8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CC8" s="2">
         <v>0</v>
@@ -3005,16 +3431,16 @@
         <v>0</v>
       </c>
       <c r="CE8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CH8" t="s">
-        <v>47</v>
+        <v>340</v>
       </c>
       <c r="CI8" s="2">
         <v>36.072635499999997</v>
@@ -3023,22 +3449,22 @@
         <v>-79.791975399999998</v>
       </c>
       <c r="CK8" t="s">
-        <v>218</v>
+        <v>361</v>
       </c>
       <c r="CL8" t="s">
-        <v>236</v>
+        <v>379</v>
       </c>
       <c r="CM8" t="s">
-        <v>254</v>
+        <v>397</v>
       </c>
       <c r="CN8" t="s">
-        <v>269</v>
+        <v>412</v>
       </c>
       <c r="CO8" t="s">
-        <v>281</v>
+        <v>424</v>
       </c>
       <c r="CP8" t="s">
-        <v>299</v>
+        <v>442</v>
       </c>
     </row>
     <row r="9">
@@ -3052,28 +3478,28 @@
         <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="E9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G9" s="1">
         <v>44835</v>
       </c>
       <c r="H9" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I9" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="J9" s="2">
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>79</v>
+        <v>124</v>
       </c>
       <c r="L9" s="2">
         <v>0</v>
@@ -3103,13 +3529,13 @@
         <v>0</v>
       </c>
       <c r="U9" t="s">
-        <v>79</v>
+        <v>153</v>
       </c>
       <c r="V9" s="2">
         <v>1</v>
       </c>
       <c r="W9" t="s">
-        <v>120</v>
+        <v>174</v>
       </c>
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
@@ -3120,7 +3546,7 @@
       <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
       <c r="AD9" t="s">
-        <v>108</v>
+        <v>197</v>
       </c>
       <c r="AE9" s="2"/>
       <c r="AF9" s="2"/>
@@ -3133,19 +3559,19 @@
       <c r="AM9" s="2"/>
       <c r="AN9" s="2"/>
       <c r="AO9" t="s">
-        <v>108</v>
+        <v>227</v>
       </c>
       <c r="AP9" t="s">
-        <v>108</v>
+        <v>248</v>
       </c>
       <c r="AQ9" t="s">
-        <v>160</v>
+        <v>266</v>
       </c>
       <c r="AR9" s="2">
         <v>0</v>
       </c>
       <c r="AS9" t="s">
-        <v>108</v>
+        <v>282</v>
       </c>
       <c r="AT9" s="2"/>
       <c r="AU9" s="2">
@@ -3264,7 +3690,7 @@
         <v>0</v>
       </c>
       <c r="CH9" t="s">
-        <v>30</v>
+        <v>341</v>
       </c>
       <c r="CI9" s="2">
         <v>35.613224000000002</v>
@@ -3273,22 +3699,22 @@
         <v>-77.372459300000003</v>
       </c>
       <c r="CK9" t="s">
-        <v>219</v>
+        <v>362</v>
       </c>
       <c r="CL9" t="s">
-        <v>237</v>
+        <v>380</v>
       </c>
       <c r="CM9" t="s">
-        <v>255</v>
+        <v>398</v>
       </c>
       <c r="CN9" t="s">
-        <v>269</v>
+        <v>412</v>
       </c>
       <c r="CO9" t="s">
-        <v>282</v>
+        <v>425</v>
       </c>
       <c r="CP9" t="s">
-        <v>300</v>
+        <v>443</v>
       </c>
     </row>
     <row r="10">
@@ -3302,28 +3728,28 @@
         <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G10" s="1">
         <v>44867</v>
       </c>
       <c r="H10" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I10" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="J10" s="2">
         <v>1</v>
       </c>
       <c r="K10" t="s">
-        <v>89</v>
+        <v>125</v>
       </c>
       <c r="L10" s="2">
         <v>1</v>
@@ -3353,13 +3779,13 @@
         <v>0</v>
       </c>
       <c r="U10" t="s">
-        <v>112</v>
+        <v>154</v>
       </c>
       <c r="V10" s="2">
         <v>0</v>
       </c>
       <c r="W10" t="s">
-        <v>120</v>
+        <v>174</v>
       </c>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
@@ -3370,7 +3796,7 @@
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
       <c r="AD10" t="s">
-        <v>132</v>
+        <v>198</v>
       </c>
       <c r="AE10" s="2">
         <v>1</v>
@@ -3385,19 +3811,19 @@
       <c r="AM10" s="2"/>
       <c r="AN10" s="2"/>
       <c r="AO10" t="s">
-        <v>108</v>
+        <v>228</v>
       </c>
       <c r="AP10" t="s">
-        <v>108</v>
+        <v>249</v>
       </c>
       <c r="AQ10" t="s">
-        <v>160</v>
+        <v>266</v>
       </c>
       <c r="AR10" s="2">
         <v>0</v>
       </c>
       <c r="AS10" t="s">
-        <v>108</v>
+        <v>283</v>
       </c>
       <c r="AT10" s="2"/>
       <c r="AU10" s="2">
@@ -3516,7 +3942,7 @@
         <v>0</v>
       </c>
       <c r="CH10" t="s">
-        <v>48</v>
+        <v>342</v>
       </c>
       <c r="CI10" s="2">
         <v>35.707914600000002</v>
@@ -3525,22 +3951,22 @@
         <v>-79.813644600000003</v>
       </c>
       <c r="CK10" t="s">
-        <v>220</v>
+        <v>363</v>
       </c>
       <c r="CL10" t="s">
-        <v>238</v>
+        <v>381</v>
       </c>
       <c r="CM10" t="s">
-        <v>256</v>
+        <v>399</v>
       </c>
       <c r="CN10" t="s">
-        <v>269</v>
+        <v>412</v>
       </c>
       <c r="CO10" t="s">
-        <v>283</v>
+        <v>426</v>
       </c>
       <c r="CP10" t="s">
-        <v>301</v>
+        <v>444</v>
       </c>
     </row>
     <row r="11">
@@ -3554,28 +3980,28 @@
         <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G11" s="1">
         <v>44666</v>
       </c>
       <c r="H11" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="I11" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="J11" s="2">
         <v>1</v>
       </c>
       <c r="K11" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="L11" s="2">
         <v>0</v>
@@ -3605,13 +4031,13 @@
         <v>1</v>
       </c>
       <c r="U11" t="s">
-        <v>113</v>
+        <v>155</v>
       </c>
       <c r="V11" s="2">
         <v>0</v>
       </c>
       <c r="W11" t="s">
-        <v>121</v>
+        <v>175</v>
       </c>
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
@@ -3622,7 +4048,7 @@
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
       <c r="AD11" t="s">
-        <v>129</v>
+        <v>199</v>
       </c>
       <c r="AE11" s="2"/>
       <c r="AF11" s="2">
@@ -3637,19 +4063,19 @@
       <c r="AM11" s="2"/>
       <c r="AN11" s="2"/>
       <c r="AO11" t="s">
-        <v>108</v>
+        <v>229</v>
       </c>
       <c r="AP11" t="s">
-        <v>108</v>
+        <v>250</v>
       </c>
       <c r="AQ11" t="s">
-        <v>160</v>
+        <v>266</v>
       </c>
       <c r="AR11" s="2">
         <v>0</v>
       </c>
       <c r="AS11" t="s">
-        <v>108</v>
+        <v>284</v>
       </c>
       <c r="AT11" s="2"/>
       <c r="AU11" s="2">
@@ -3768,7 +4194,7 @@
         <v>0</v>
       </c>
       <c r="CH11" t="s">
-        <v>47</v>
+        <v>343</v>
       </c>
       <c r="CI11" s="2">
         <v>36.072635499999997</v>
@@ -3777,22 +4203,22 @@
         <v>-79.791975399999998</v>
       </c>
       <c r="CK11" t="s">
-        <v>221</v>
+        <v>364</v>
       </c>
       <c r="CL11" t="s">
-        <v>239</v>
+        <v>382</v>
       </c>
       <c r="CM11" t="s">
-        <v>257</v>
+        <v>400</v>
       </c>
       <c r="CN11" t="s">
-        <v>269</v>
+        <v>412</v>
       </c>
       <c r="CO11" t="s">
-        <v>284</v>
+        <v>427</v>
       </c>
       <c r="CP11" t="s">
-        <v>302</v>
+        <v>445</v>
       </c>
     </row>
     <row r="12">
@@ -3806,28 +4232,28 @@
         <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G12" s="1">
         <v>44883</v>
       </c>
       <c r="H12" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="I12" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="J12" s="2">
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>93</v>
+        <v>127</v>
       </c>
       <c r="L12" s="2">
         <v>0</v>
@@ -3857,13 +4283,13 @@
         <v>0</v>
       </c>
       <c r="U12" t="s">
-        <v>112</v>
+        <v>156</v>
       </c>
       <c r="V12" s="2">
         <v>0</v>
       </c>
       <c r="W12" t="s">
-        <v>122</v>
+        <v>176</v>
       </c>
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
@@ -3876,7 +4302,7 @@
         <v>1</v>
       </c>
       <c r="AD12" t="s">
-        <v>133</v>
+        <v>200</v>
       </c>
       <c r="AE12" s="2">
         <v>1</v>
@@ -3897,19 +4323,19 @@
         <v>1</v>
       </c>
       <c r="AO12" t="s">
-        <v>108</v>
+        <v>230</v>
       </c>
       <c r="AP12" t="s">
-        <v>108</v>
+        <v>251</v>
       </c>
       <c r="AQ12" t="s">
-        <v>161</v>
+        <v>267</v>
       </c>
       <c r="AR12" s="2">
         <v>1</v>
       </c>
       <c r="AS12" t="s">
-        <v>164</v>
+        <v>285</v>
       </c>
       <c r="AT12" s="2"/>
       <c r="AU12" s="2">
@@ -4028,7 +4454,7 @@
         <v>0</v>
       </c>
       <c r="CH12" t="s">
-        <v>50</v>
+        <v>344</v>
       </c>
       <c r="CI12" s="2">
         <v>35.762427199999998</v>
@@ -4037,22 +4463,22 @@
         <v>-105.9323157</v>
       </c>
       <c r="CK12" t="s">
-        <v>222</v>
+        <v>365</v>
       </c>
       <c r="CL12" t="s">
-        <v>240</v>
+        <v>383</v>
       </c>
       <c r="CM12" t="s">
-        <v>258</v>
+        <v>401</v>
       </c>
       <c r="CN12" t="s">
-        <v>270</v>
+        <v>413</v>
       </c>
       <c r="CO12" t="s">
-        <v>285</v>
+        <v>428</v>
       </c>
       <c r="CP12" t="s">
-        <v>303</v>
+        <v>446</v>
       </c>
     </row>
     <row r="13">
@@ -4066,40 +4492,40 @@
         <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G13" s="1">
-        <v>44707</v>
+        <v>44695</v>
       </c>
       <c r="H13" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="I13" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="J13" s="2">
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="L13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13" s="2">
         <v>0</v>
       </c>
       <c r="O13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P13" s="2">
         <v>0</v>
@@ -4108,7 +4534,7 @@
         <v>0</v>
       </c>
       <c r="R13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S13" s="2">
         <v>0</v>
@@ -4117,13 +4543,13 @@
         <v>0</v>
       </c>
       <c r="U13" t="s">
-        <v>112</v>
+        <v>157</v>
       </c>
       <c r="V13" s="2">
         <v>0</v>
       </c>
       <c r="W13" t="s">
-        <v>120</v>
+        <v>177</v>
       </c>
       <c r="X13" s="2"/>
       <c r="Y13" s="2"/>
@@ -4134,7 +4560,7 @@
       <c r="AB13" s="2"/>
       <c r="AC13" s="2"/>
       <c r="AD13" t="s">
-        <v>131</v>
+        <v>201</v>
       </c>
       <c r="AE13" s="2">
         <v>0</v>
@@ -4149,26 +4575,26 @@
       <c r="AM13" s="2"/>
       <c r="AN13" s="2"/>
       <c r="AO13" t="s">
-        <v>108</v>
+        <v>231</v>
       </c>
       <c r="AP13" t="s">
-        <v>108</v>
+        <v>252</v>
       </c>
       <c r="AQ13" t="s">
-        <v>160</v>
+        <v>268</v>
       </c>
       <c r="AR13" s="2">
         <v>0</v>
       </c>
       <c r="AS13" t="s">
-        <v>108</v>
+        <v>286</v>
       </c>
       <c r="AT13" s="2"/>
       <c r="AU13" s="2">
         <v>0</v>
       </c>
       <c r="AV13" s="1">
-        <v>44714</v>
+        <v>44707</v>
       </c>
       <c r="AW13" s="2">
         <v>1</v>
@@ -4178,22 +4604,22 @@
       </c>
       <c r="AY13" s="2"/>
       <c r="AZ13" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="BA13" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="BB13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF13" s="2">
         <v>0</v>
@@ -4205,10 +4631,10 @@
         <v>0</v>
       </c>
       <c r="BI13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK13" s="2">
         <v>0</v>
@@ -4217,7 +4643,7 @@
         <v>0</v>
       </c>
       <c r="BM13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN13" s="2">
         <v>0</v>
@@ -4247,7 +4673,7 @@
         <v>0</v>
       </c>
       <c r="BW13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX13" s="2">
         <v>0</v>
@@ -4259,19 +4685,19 @@
         <v>0</v>
       </c>
       <c r="CA13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB13" s="2">
         <v>1</v>
       </c>
       <c r="CC13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CD13" s="2">
         <v>0</v>
       </c>
       <c r="CE13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF13" s="2">
         <v>0</v>
@@ -4280,27 +4706,27 @@
         <v>0</v>
       </c>
       <c r="CH13" t="s">
-        <v>108</v>
+        <v>345</v>
       </c>
       <c r="CI13" s="2"/>
       <c r="CJ13" s="2"/>
       <c r="CK13" t="s">
-        <v>223</v>
+        <v>366</v>
       </c>
       <c r="CL13" t="s">
-        <v>241</v>
+        <v>384</v>
       </c>
       <c r="CM13" t="s">
-        <v>259</v>
+        <v>402</v>
       </c>
       <c r="CN13" t="s">
-        <v>271</v>
+        <v>414</v>
       </c>
       <c r="CO13" t="s">
-        <v>286</v>
+        <v>429</v>
       </c>
       <c r="CP13" t="s">
-        <v>304</v>
+        <v>447</v>
       </c>
     </row>
     <row r="14">
@@ -4314,40 +4740,40 @@
         <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E14" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G14" s="1">
-        <v>44695</v>
+        <v>44707</v>
       </c>
       <c r="H14" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="I14" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="J14" s="2">
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="L14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N14" s="2">
         <v>0</v>
       </c>
       <c r="O14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P14" s="2">
         <v>0</v>
@@ -4356,7 +4782,7 @@
         <v>0</v>
       </c>
       <c r="R14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S14" s="2">
         <v>0</v>
@@ -4365,13 +4791,13 @@
         <v>0</v>
       </c>
       <c r="U14" t="s">
-        <v>114</v>
+        <v>158</v>
       </c>
       <c r="V14" s="2">
         <v>0</v>
       </c>
       <c r="W14" t="s">
-        <v>120</v>
+        <v>177</v>
       </c>
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
@@ -4382,7 +4808,7 @@
       <c r="AB14" s="2"/>
       <c r="AC14" s="2"/>
       <c r="AD14" t="s">
-        <v>131</v>
+        <v>201</v>
       </c>
       <c r="AE14" s="2">
         <v>0</v>
@@ -4397,26 +4823,26 @@
       <c r="AM14" s="2"/>
       <c r="AN14" s="2"/>
       <c r="AO14" t="s">
-        <v>108</v>
+        <v>232</v>
       </c>
       <c r="AP14" t="s">
-        <v>108</v>
+        <v>253</v>
       </c>
       <c r="AQ14" t="s">
-        <v>160</v>
+        <v>268</v>
       </c>
       <c r="AR14" s="2">
         <v>0</v>
       </c>
       <c r="AS14" t="s">
-        <v>108</v>
+        <v>287</v>
       </c>
       <c r="AT14" s="2"/>
       <c r="AU14" s="2">
         <v>0</v>
       </c>
       <c r="AV14" s="1">
-        <v>44707</v>
+        <v>44714</v>
       </c>
       <c r="AW14" s="2">
         <v>1</v>
@@ -4426,22 +4852,22 @@
       </c>
       <c r="AY14" s="2"/>
       <c r="AZ14" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="BA14" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BB14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF14" s="2">
         <v>0</v>
@@ -4453,10 +4879,10 @@
         <v>0</v>
       </c>
       <c r="BI14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK14" s="2">
         <v>0</v>
@@ -4465,7 +4891,7 @@
         <v>0</v>
       </c>
       <c r="BM14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN14" s="2">
         <v>0</v>
@@ -4495,7 +4921,7 @@
         <v>0</v>
       </c>
       <c r="BW14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX14" s="2">
         <v>0</v>
@@ -4507,19 +4933,19 @@
         <v>0</v>
       </c>
       <c r="CA14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CB14" s="2">
         <v>1</v>
       </c>
       <c r="CC14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD14" s="2">
         <v>0</v>
       </c>
       <c r="CE14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF14" s="2">
         <v>0</v>
@@ -4528,27 +4954,27 @@
         <v>0</v>
       </c>
       <c r="CH14" t="s">
-        <v>108</v>
+        <v>346</v>
       </c>
       <c r="CI14" s="2"/>
       <c r="CJ14" s="2"/>
       <c r="CK14" t="s">
-        <v>223</v>
+        <v>366</v>
       </c>
       <c r="CL14" t="s">
-        <v>241</v>
+        <v>384</v>
       </c>
       <c r="CM14" t="s">
-        <v>259</v>
+        <v>402</v>
       </c>
       <c r="CN14" t="s">
-        <v>271</v>
+        <v>414</v>
       </c>
       <c r="CO14" t="s">
-        <v>286</v>
+        <v>429</v>
       </c>
       <c r="CP14" t="s">
-        <v>304</v>
+        <v>447</v>
       </c>
     </row>
     <row r="15">
@@ -4562,28 +4988,28 @@
         <v>35</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F15" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G15" s="1">
         <v>44834</v>
       </c>
       <c r="H15" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="I15" t="s">
-        <v>83</v>
+        <v>109</v>
       </c>
       <c r="J15" s="2">
         <v>1</v>
       </c>
       <c r="K15" t="s">
-        <v>89</v>
+        <v>130</v>
       </c>
       <c r="L15" s="2">
         <v>1</v>
@@ -4613,13 +5039,13 @@
         <v>0</v>
       </c>
       <c r="U15" t="s">
-        <v>112</v>
+        <v>158</v>
       </c>
       <c r="V15" s="2">
         <v>0</v>
       </c>
       <c r="W15" t="s">
-        <v>121</v>
+        <v>178</v>
       </c>
       <c r="X15" s="2"/>
       <c r="Y15" s="2"/>
@@ -4630,7 +5056,7 @@
       <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
       <c r="AD15" t="s">
-        <v>134</v>
+        <v>202</v>
       </c>
       <c r="AE15" s="2">
         <v>1</v>
@@ -4647,19 +5073,19 @@
       <c r="AM15" s="2"/>
       <c r="AN15" s="2"/>
       <c r="AO15" t="s">
-        <v>108</v>
+        <v>233</v>
       </c>
       <c r="AP15" t="s">
-        <v>156</v>
+        <v>254</v>
       </c>
       <c r="AQ15" t="s">
-        <v>161</v>
+        <v>269</v>
       </c>
       <c r="AR15" s="2">
         <v>1</v>
       </c>
       <c r="AS15" t="s">
-        <v>165</v>
+        <v>288</v>
       </c>
       <c r="AT15" s="2"/>
       <c r="AU15" s="2">
@@ -4778,7 +5204,7 @@
         <v>0</v>
       </c>
       <c r="CH15" t="s">
-        <v>209</v>
+        <v>347</v>
       </c>
       <c r="CI15" s="2">
         <v>42.651167399999999</v>
@@ -4787,22 +5213,22 @@
         <v>-73.754968000000005</v>
       </c>
       <c r="CK15" t="s">
-        <v>224</v>
+        <v>367</v>
       </c>
       <c r="CL15" t="s">
-        <v>242</v>
+        <v>385</v>
       </c>
       <c r="CM15" t="s">
-        <v>260</v>
+        <v>403</v>
       </c>
       <c r="CN15" t="s">
-        <v>271</v>
+        <v>414</v>
       </c>
       <c r="CO15" t="s">
-        <v>287</v>
+        <v>430</v>
       </c>
       <c r="CP15" t="s">
-        <v>305</v>
+        <v>448</v>
       </c>
     </row>
     <row r="16">
@@ -4816,28 +5242,28 @@
         <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G16" s="1">
         <v>44780</v>
       </c>
       <c r="H16" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="I16" t="s">
-        <v>78</v>
+        <v>110</v>
       </c>
       <c r="J16" s="2">
         <v>1</v>
       </c>
       <c r="K16" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="L16" s="2">
         <v>1</v>
@@ -4867,13 +5293,13 @@
         <v>0</v>
       </c>
       <c r="U16" t="s">
-        <v>115</v>
+        <v>159</v>
       </c>
       <c r="V16" s="2">
         <v>0</v>
       </c>
       <c r="W16" t="s">
-        <v>120</v>
+        <v>179</v>
       </c>
       <c r="X16" s="2"/>
       <c r="Y16" s="2"/>
@@ -4884,7 +5310,7 @@
       <c r="AB16" s="2"/>
       <c r="AC16" s="2"/>
       <c r="AD16" t="s">
-        <v>129</v>
+        <v>203</v>
       </c>
       <c r="AE16" s="2"/>
       <c r="AF16" s="2">
@@ -4899,19 +5325,19 @@
       <c r="AM16" s="2"/>
       <c r="AN16" s="2"/>
       <c r="AO16" t="s">
-        <v>108</v>
+        <v>234</v>
       </c>
       <c r="AP16" t="s">
-        <v>108</v>
+        <v>255</v>
       </c>
       <c r="AQ16" t="s">
-        <v>160</v>
+        <v>270</v>
       </c>
       <c r="AR16" s="2">
         <v>0</v>
       </c>
       <c r="AS16" t="s">
-        <v>108</v>
+        <v>289</v>
       </c>
       <c r="AT16" s="2"/>
       <c r="AU16" s="2">
@@ -5030,7 +5456,7 @@
         <v>0</v>
       </c>
       <c r="CH16" t="s">
-        <v>53</v>
+        <v>348</v>
       </c>
       <c r="CI16" s="2">
         <v>40.946511800000003</v>
@@ -5039,22 +5465,22 @@
         <v>-73.069125700000001</v>
       </c>
       <c r="CK16" t="s">
-        <v>225</v>
+        <v>368</v>
       </c>
       <c r="CL16" t="s">
-        <v>243</v>
+        <v>386</v>
       </c>
       <c r="CM16" t="s">
-        <v>261</v>
+        <v>404</v>
       </c>
       <c r="CN16" t="s">
-        <v>271</v>
+        <v>414</v>
       </c>
       <c r="CO16" t="s">
-        <v>288</v>
+        <v>431</v>
       </c>
       <c r="CP16" t="s">
-        <v>306</v>
+        <v>449</v>
       </c>
     </row>
     <row r="17">
@@ -5068,28 +5494,28 @@
         <v>37</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F17" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G17" s="1">
         <v>44871</v>
       </c>
       <c r="H17" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="I17" t="s">
-        <v>81</v>
+        <v>111</v>
       </c>
       <c r="J17" s="2">
         <v>1</v>
       </c>
       <c r="K17" t="s">
-        <v>91</v>
+        <v>132</v>
       </c>
       <c r="L17" s="2">
         <v>1</v>
@@ -5119,13 +5545,13 @@
         <v>0</v>
       </c>
       <c r="U17" t="s">
-        <v>111</v>
+        <v>160</v>
       </c>
       <c r="V17" s="2">
         <v>1</v>
       </c>
       <c r="W17" t="s">
-        <v>123</v>
+        <v>180</v>
       </c>
       <c r="X17" s="2"/>
       <c r="Y17" s="2">
@@ -5136,7 +5562,7 @@
       <c r="AB17" s="2"/>
       <c r="AC17" s="2"/>
       <c r="AD17" t="s">
-        <v>135</v>
+        <v>204</v>
       </c>
       <c r="AE17" s="2">
         <v>1</v>
@@ -5155,19 +5581,19 @@
       <c r="AM17" s="2"/>
       <c r="AN17" s="2"/>
       <c r="AO17" t="s">
-        <v>108</v>
+        <v>235</v>
       </c>
       <c r="AP17" t="s">
-        <v>157</v>
+        <v>256</v>
       </c>
       <c r="AQ17" t="s">
-        <v>160</v>
+        <v>270</v>
       </c>
       <c r="AR17" s="2">
         <v>0</v>
       </c>
       <c r="AS17" t="s">
-        <v>108</v>
+        <v>290</v>
       </c>
       <c r="AT17" s="2"/>
       <c r="AU17" s="2">
@@ -5286,7 +5712,7 @@
         <v>0</v>
       </c>
       <c r="CH17" t="s">
-        <v>54</v>
+        <v>349</v>
       </c>
       <c r="CI17" s="2">
         <v>45.520247099999999</v>
@@ -5295,22 +5721,22 @@
         <v>-122.674194</v>
       </c>
       <c r="CK17" t="s">
-        <v>226</v>
+        <v>369</v>
       </c>
       <c r="CL17" t="s">
-        <v>244</v>
+        <v>387</v>
       </c>
       <c r="CM17" t="s">
-        <v>262</v>
+        <v>405</v>
       </c>
       <c r="CN17" t="s">
-        <v>272</v>
+        <v>415</v>
       </c>
       <c r="CO17" t="s">
-        <v>289</v>
+        <v>432</v>
       </c>
       <c r="CP17" t="s">
-        <v>307</v>
+        <v>450</v>
       </c>
     </row>
     <row r="18">
@@ -5324,28 +5750,28 @@
         <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E18" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G18" s="1">
         <v>44797</v>
       </c>
       <c r="H18" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="I18" t="s">
-        <v>79</v>
+        <v>112</v>
       </c>
       <c r="J18" s="2">
         <v>1</v>
       </c>
       <c r="K18" t="s">
-        <v>90</v>
+        <v>133</v>
       </c>
       <c r="L18" s="2">
         <v>0</v>
@@ -5375,13 +5801,13 @@
         <v>0</v>
       </c>
       <c r="U18" t="s">
-        <v>109</v>
+        <v>161</v>
       </c>
       <c r="V18" s="2">
         <v>0</v>
       </c>
       <c r="W18" t="s">
-        <v>124</v>
+        <v>181</v>
       </c>
       <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
@@ -5392,7 +5818,7 @@
       </c>
       <c r="AC18" s="2"/>
       <c r="AD18" t="s">
-        <v>134</v>
+        <v>205</v>
       </c>
       <c r="AE18" s="2">
         <v>1</v>
@@ -5407,19 +5833,19 @@
       <c r="AM18" s="2"/>
       <c r="AN18" s="2"/>
       <c r="AO18" t="s">
-        <v>150</v>
+        <v>236</v>
       </c>
       <c r="AP18" t="s">
-        <v>158</v>
+        <v>257</v>
       </c>
       <c r="AQ18" t="s">
-        <v>160</v>
+        <v>270</v>
       </c>
       <c r="AR18" s="2">
         <v>0</v>
       </c>
       <c r="AS18" t="s">
-        <v>108</v>
+        <v>291</v>
       </c>
       <c r="AT18" s="2"/>
       <c r="AU18" s="2">
@@ -5538,7 +5964,7 @@
         <v>0</v>
       </c>
       <c r="CH18" t="s">
-        <v>54</v>
+        <v>349</v>
       </c>
       <c r="CI18" s="2">
         <v>45.520247099999999</v>
@@ -5547,22 +5973,22 @@
         <v>-122.674194</v>
       </c>
       <c r="CK18" t="s">
-        <v>226</v>
+        <v>369</v>
       </c>
       <c r="CL18" t="s">
-        <v>244</v>
+        <v>387</v>
       </c>
       <c r="CM18" t="s">
-        <v>262</v>
+        <v>405</v>
       </c>
       <c r="CN18" t="s">
-        <v>272</v>
+        <v>415</v>
       </c>
       <c r="CO18" t="s">
-        <v>289</v>
+        <v>432</v>
       </c>
       <c r="CP18" t="s">
-        <v>307</v>
+        <v>450</v>
       </c>
     </row>
     <row r="19">
@@ -5576,28 +6002,28 @@
         <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F19" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G19" s="1">
         <v>44751</v>
       </c>
       <c r="H19" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="I19" t="s">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="J19" s="2">
         <v>1</v>
       </c>
       <c r="K19" t="s">
-        <v>91</v>
+        <v>134</v>
       </c>
       <c r="L19" s="2">
         <v>1</v>
@@ -5627,13 +6053,13 @@
         <v>0</v>
       </c>
       <c r="U19" t="s">
-        <v>113</v>
+        <v>162</v>
       </c>
       <c r="V19" s="2">
         <v>0</v>
       </c>
       <c r="W19" t="s">
-        <v>120</v>
+        <v>182</v>
       </c>
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
@@ -5644,7 +6070,7 @@
       <c r="AB19" s="2"/>
       <c r="AC19" s="2"/>
       <c r="AD19" t="s">
-        <v>136</v>
+        <v>206</v>
       </c>
       <c r="AE19" s="2">
         <v>-1</v>
@@ -5663,19 +6089,19 @@
       <c r="AM19" s="2"/>
       <c r="AN19" s="2"/>
       <c r="AO19" t="s">
-        <v>108</v>
+        <v>237</v>
       </c>
       <c r="AP19" t="s">
-        <v>108</v>
+        <v>258</v>
       </c>
       <c r="AQ19" t="s">
-        <v>161</v>
+        <v>271</v>
       </c>
       <c r="AR19" s="2">
         <v>1</v>
       </c>
       <c r="AS19" t="s">
-        <v>166</v>
+        <v>292</v>
       </c>
       <c r="AT19" s="2"/>
       <c r="AU19" s="2">
@@ -5794,7 +6220,7 @@
         <v>0</v>
       </c>
       <c r="CH19" t="s">
-        <v>56</v>
+        <v>350</v>
       </c>
       <c r="CI19" s="2">
         <v>35.797480700000001</v>
@@ -5803,22 +6229,22 @@
         <v>-82.683931299999998</v>
       </c>
       <c r="CK19" t="s">
-        <v>227</v>
+        <v>370</v>
       </c>
       <c r="CL19" t="s">
-        <v>245</v>
+        <v>388</v>
       </c>
       <c r="CM19" t="s">
-        <v>263</v>
+        <v>406</v>
       </c>
       <c r="CN19" t="s">
-        <v>273</v>
+        <v>416</v>
       </c>
       <c r="CO19" t="s">
-        <v>290</v>
+        <v>433</v>
       </c>
       <c r="CP19" t="s">
-        <v>308</v>
+        <v>451</v>
       </c>
     </row>
     <row r="20">
@@ -5832,28 +6258,28 @@
         <v>39</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F20" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G20" s="1">
         <v>44727</v>
       </c>
       <c r="H20" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="I20" t="s">
-        <v>82</v>
+        <v>114</v>
       </c>
       <c r="J20" s="2">
         <v>1</v>
       </c>
       <c r="K20" t="s">
-        <v>91</v>
+        <v>134</v>
       </c>
       <c r="L20" s="2">
         <v>1</v>
@@ -5883,13 +6309,13 @@
         <v>0</v>
       </c>
       <c r="U20" t="s">
-        <v>112</v>
+        <v>163</v>
       </c>
       <c r="V20" s="2">
         <v>0</v>
       </c>
       <c r="W20" t="s">
-        <v>120</v>
+        <v>182</v>
       </c>
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
@@ -5900,7 +6326,7 @@
       <c r="AB20" s="2"/>
       <c r="AC20" s="2"/>
       <c r="AD20" t="s">
-        <v>131</v>
+        <v>207</v>
       </c>
       <c r="AE20" s="2">
         <v>0</v>
@@ -5915,19 +6341,19 @@
       <c r="AM20" s="2"/>
       <c r="AN20" s="2"/>
       <c r="AO20" t="s">
-        <v>108</v>
+        <v>238</v>
       </c>
       <c r="AP20" t="s">
-        <v>108</v>
+        <v>259</v>
       </c>
       <c r="AQ20" t="s">
-        <v>160</v>
+        <v>272</v>
       </c>
       <c r="AR20" s="2">
         <v>0</v>
       </c>
       <c r="AS20" t="s">
-        <v>108</v>
+        <v>293</v>
       </c>
       <c r="AT20" s="2"/>
       <c r="AU20" s="2">
@@ -6046,27 +6472,27 @@
         <v>0</v>
       </c>
       <c r="CH20" t="s">
-        <v>108</v>
+        <v>351</v>
       </c>
       <c r="CI20" s="2"/>
       <c r="CJ20" s="2"/>
       <c r="CK20" t="s">
-        <v>228</v>
+        <v>371</v>
       </c>
       <c r="CL20" t="s">
-        <v>246</v>
+        <v>389</v>
       </c>
       <c r="CM20" t="s">
-        <v>264</v>
+        <v>407</v>
       </c>
       <c r="CN20" t="s">
-        <v>273</v>
+        <v>416</v>
       </c>
       <c r="CO20" t="s">
-        <v>291</v>
+        <v>434</v>
       </c>
       <c r="CP20" t="s">
-        <v>309</v>
+        <v>452</v>
       </c>
     </row>
     <row r="21">
@@ -6080,28 +6506,28 @@
         <v>40</v>
       </c>
       <c r="D21" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E21" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G21" s="1">
         <v>44730</v>
       </c>
       <c r="H21" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="I21" t="s">
-        <v>79</v>
+        <v>115</v>
       </c>
       <c r="J21" s="2">
         <v>1</v>
       </c>
       <c r="K21" t="s">
-        <v>95</v>
+        <v>135</v>
       </c>
       <c r="L21" s="2">
         <v>1</v>
@@ -6131,13 +6557,13 @@
         <v>0</v>
       </c>
       <c r="U21" t="s">
-        <v>116</v>
+        <v>164</v>
       </c>
       <c r="V21" s="2">
         <v>0</v>
       </c>
       <c r="W21" t="s">
-        <v>125</v>
+        <v>183</v>
       </c>
       <c r="X21" s="2"/>
       <c r="Y21" s="2"/>
@@ -6146,7 +6572,7 @@
       <c r="AB21" s="2"/>
       <c r="AC21" s="2"/>
       <c r="AD21" t="s">
-        <v>129</v>
+        <v>208</v>
       </c>
       <c r="AE21" s="2"/>
       <c r="AF21" s="2">
@@ -6161,19 +6587,19 @@
       <c r="AM21" s="2"/>
       <c r="AN21" s="2"/>
       <c r="AO21" t="s">
-        <v>108</v>
+        <v>239</v>
       </c>
       <c r="AP21" t="s">
-        <v>108</v>
+        <v>260</v>
       </c>
       <c r="AQ21" t="s">
-        <v>160</v>
+        <v>272</v>
       </c>
       <c r="AR21" s="2">
         <v>0</v>
       </c>
       <c r="AS21" t="s">
-        <v>108</v>
+        <v>294</v>
       </c>
       <c r="AT21" s="2"/>
       <c r="AU21" s="2">
@@ -6292,27 +6718,27 @@
         <v>0</v>
       </c>
       <c r="CH21" t="s">
-        <v>108</v>
+        <v>352</v>
       </c>
       <c r="CI21" s="2"/>
       <c r="CJ21" s="2"/>
       <c r="CK21" t="s">
-        <v>229</v>
+        <v>372</v>
       </c>
       <c r="CL21" t="s">
-        <v>247</v>
+        <v>390</v>
       </c>
       <c r="CM21" t="s">
-        <v>265</v>
+        <v>408</v>
       </c>
       <c r="CN21" t="s">
-        <v>274</v>
+        <v>417</v>
       </c>
       <c r="CO21" t="s">
-        <v>292</v>
+        <v>435</v>
       </c>
       <c r="CP21" t="s">
-        <v>310</v>
+        <v>453</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix geolocation for Fairview, NC
Should be Buncombe Co not Dare Co (assigned by GeoCage API)
</commit_message>
<xml_diff>
--- a/datasets/analysis_dataset.xlsx
+++ b/datasets/analysis_dataset.xlsx
@@ -33,12 +33,12 @@
     <t>368</t>
   </si>
   <si>
+    <t>424</t>
+  </si>
+  <si>
     <t>280</t>
   </si>
   <si>
-    <t>424</t>
-  </si>
-  <si>
     <t>437</t>
   </si>
   <si>
@@ -63,12 +63,12 @@
     <t>340</t>
   </si>
   <si>
+    <t>555</t>
+  </si>
+  <si>
     <t>836</t>
   </si>
   <si>
-    <t>555</t>
-  </si>
-  <si>
     <t>408</t>
   </si>
   <si>
@@ -258,12 +258,12 @@
     <t>syringe</t>
   </si>
   <si>
+    <t>spatula</t>
+  </si>
+  <si>
     <t>pill</t>
   </si>
   <si>
-    <t>spatula</t>
-  </si>
-  <si>
     <t>swab</t>
   </si>
   <si>
@@ -348,12 +348,12 @@
     <t>tan</t>
   </si>
   <si>
+    <t>white</t>
+  </si>
+  <si>
     <t>blue</t>
   </si>
   <si>
-    <t>white</t>
-  </si>
-  <si>
     <t>brown</t>
   </si>
   <si>
@@ -384,12 +384,12 @@
     <t>powder; chunky; shiny</t>
   </si>
   <si>
+    <t>crystals</t>
+  </si>
+  <si>
     <t>fake pill</t>
   </si>
   <si>
-    <t>crystals</t>
-  </si>
-  <si>
     <t>tar</t>
   </si>
   <si>
@@ -486,10 +486,10 @@
     <t>fast acting</t>
   </si>
   <si>
+    <t>FTS = negative</t>
+  </si>
+  <si>
     <t>strong blues</t>
-  </si>
-  <si>
-    <t>FTS = negative</t>
   </si>
   <si>
     <t>overdose</t>
@@ -1082,7 +1082,7 @@
         <v>125</v>
       </c>
       <c r="Y1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="Z1" t="s">
         <v>120</v>
@@ -1091,7 +1091,7 @@
         <v>126</v>
       </c>
       <c r="AB1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AC1" t="s">
         <v>127</v>
@@ -2608,7 +2608,7 @@
         <v>70</v>
       </c>
       <c r="G7" s="1">
-        <v>44701</v>
+        <v>44484</v>
       </c>
       <c r="H7" t="s">
         <v>81</v>
@@ -2620,13 +2620,13 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="L7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7" s="2">
         <v>0</v>
@@ -2647,22 +2647,22 @@
         <v>0</v>
       </c>
       <c r="T7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U7" t="s">
         <v>111</v>
       </c>
       <c r="V7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W7" t="s">
-        <v>81</v>
+        <v>120</v>
       </c>
       <c r="X7" s="2"/>
-      <c r="Y7" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2">
+        <v>1</v>
+      </c>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
@@ -2683,14 +2683,12 @@
         <v>108</v>
       </c>
       <c r="AP7" t="s">
-        <v>155</v>
+        <v>108</v>
       </c>
       <c r="AQ7" t="s">
-        <v>160</v>
-      </c>
-      <c r="AR7" s="2">
-        <v>0</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="AR7" s="2"/>
       <c r="AS7" t="s">
         <v>108</v>
       </c>
@@ -2699,32 +2697,32 @@
         <v>0</v>
       </c>
       <c r="AV7" s="1">
-        <v>44721</v>
+        <v>44603</v>
       </c>
       <c r="AW7" s="2">
         <v>1</v>
       </c>
       <c r="AX7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY7" s="2"/>
       <c r="AZ7" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="BA7" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="BB7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF7" s="2">
         <v>0</v>
@@ -2733,7 +2731,7 @@
         <v>0</v>
       </c>
       <c r="BH7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI7" s="2">
         <v>0</v>
@@ -2742,7 +2740,7 @@
         <v>0</v>
       </c>
       <c r="BK7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL7" s="2">
         <v>0</v>
@@ -2784,7 +2782,7 @@
         <v>0</v>
       </c>
       <c r="BY7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BZ7" s="2">
         <v>0</v>
@@ -2799,7 +2797,7 @@
         <v>0</v>
       </c>
       <c r="CD7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE7" s="2">
         <v>0</v>
@@ -2808,13 +2806,13 @@
         <v>0</v>
       </c>
       <c r="CG7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CH7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CI7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ7" t="s">
         <v>47</v>
@@ -2864,7 +2862,7 @@
         <v>70</v>
       </c>
       <c r="G8" s="1">
-        <v>44484</v>
+        <v>44701</v>
       </c>
       <c r="H8" t="s">
         <v>82</v>
@@ -2876,13 +2874,13 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="L8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8" s="2">
         <v>0</v>
@@ -2903,22 +2901,22 @@
         <v>0</v>
       </c>
       <c r="T8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8" t="s">
         <v>112</v>
       </c>
       <c r="V8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W8" t="s">
-        <v>120</v>
+        <v>82</v>
       </c>
       <c r="X8" s="2"/>
-      <c r="Y8" s="2"/>
-      <c r="Z8" s="2">
-        <v>1</v>
-      </c>
+      <c r="Y8" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
@@ -2939,12 +2937,14 @@
         <v>108</v>
       </c>
       <c r="AP8" t="s">
-        <v>108</v>
+        <v>155</v>
       </c>
       <c r="AQ8" t="s">
-        <v>79</v>
-      </c>
-      <c r="AR8" s="2"/>
+        <v>160</v>
+      </c>
+      <c r="AR8" s="2">
+        <v>0</v>
+      </c>
       <c r="AS8" t="s">
         <v>108</v>
       </c>
@@ -2953,32 +2953,32 @@
         <v>0</v>
       </c>
       <c r="AV8" s="1">
-        <v>44603</v>
+        <v>44721</v>
       </c>
       <c r="AW8" s="2">
         <v>1</v>
       </c>
       <c r="AX8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY8" s="2"/>
       <c r="AZ8" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="BA8" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="BB8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF8" s="2">
         <v>0</v>
@@ -2987,7 +2987,7 @@
         <v>0</v>
       </c>
       <c r="BH8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI8" s="2">
         <v>0</v>
@@ -2996,7 +2996,7 @@
         <v>0</v>
       </c>
       <c r="BK8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL8" s="2">
         <v>0</v>
@@ -3038,7 +3038,7 @@
         <v>0</v>
       </c>
       <c r="BY8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ8" s="2">
         <v>0</v>
@@ -3053,7 +3053,7 @@
         <v>0</v>
       </c>
       <c r="CD8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CE8" s="2">
         <v>0</v>
@@ -3062,13 +3062,13 @@
         <v>0</v>
       </c>
       <c r="CG8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CJ8" t="s">
         <v>47</v>
@@ -3416,7 +3416,7 @@
         <v>0</v>
       </c>
       <c r="U10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V10" s="2">
         <v>0</v>
@@ -3893,10 +3893,10 @@
         <v>44883</v>
       </c>
       <c r="H12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J12" s="2">
         <v>1</v>
@@ -3932,7 +3932,7 @@
         <v>0</v>
       </c>
       <c r="U12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V12" s="2">
         <v>0</v>
@@ -4452,7 +4452,7 @@
         <v>0</v>
       </c>
       <c r="U14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V14" s="2">
         <v>0</v>
@@ -4706,7 +4706,7 @@
         <v>0</v>
       </c>
       <c r="U15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V15" s="2">
         <v>0</v>
@@ -5182,37 +5182,37 @@
         <v>73</v>
       </c>
       <c r="G17" s="1">
-        <v>44871</v>
+        <v>44797</v>
       </c>
       <c r="H17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J17" s="2">
         <v>1</v>
       </c>
       <c r="K17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N17" s="2">
         <v>0</v>
       </c>
       <c r="O17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P17" s="2">
         <v>0</v>
       </c>
       <c r="Q17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R17" s="2">
         <v>0</v>
@@ -5224,24 +5224,24 @@
         <v>0</v>
       </c>
       <c r="U17" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="V17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W17" t="s">
         <v>123</v>
       </c>
       <c r="X17" s="2"/>
-      <c r="Y17" s="2">
-        <v>1</v>
-      </c>
+      <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
-      <c r="AB17" s="2"/>
+      <c r="AB17" s="2">
+        <v>1</v>
+      </c>
       <c r="AC17" s="2"/>
       <c r="AD17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AE17" s="2">
         <v>1</v>
@@ -5250,17 +5250,13 @@
       <c r="AG17" s="2"/>
       <c r="AH17" s="2"/>
       <c r="AI17" s="2"/>
-      <c r="AJ17" s="2">
-        <v>1</v>
-      </c>
-      <c r="AK17" s="2">
-        <v>1</v>
-      </c>
+      <c r="AJ17" s="2"/>
+      <c r="AK17" s="2"/>
       <c r="AL17" s="2"/>
       <c r="AM17" s="2"/>
       <c r="AN17" s="2"/>
       <c r="AO17" t="s">
-        <v>108</v>
+        <v>150</v>
       </c>
       <c r="AP17" t="s">
         <v>157</v>
@@ -5279,26 +5275,26 @@
         <v>1</v>
       </c>
       <c r="AV17" s="1">
-        <v>44879</v>
+        <v>44803</v>
       </c>
       <c r="AW17" s="2">
         <v>1</v>
       </c>
       <c r="AX17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY17" s="2"/>
       <c r="AZ17" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="BA17" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="BB17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD17" s="2">
         <v>0</v>
@@ -5310,7 +5306,7 @@
         <v>0</v>
       </c>
       <c r="BG17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BH17" s="2">
         <v>1</v>
@@ -5334,7 +5330,7 @@
         <v>0</v>
       </c>
       <c r="BO17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP17" s="2">
         <v>0</v>
@@ -5364,7 +5360,7 @@
         <v>0</v>
       </c>
       <c r="BY17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ17" s="2">
         <v>0</v>
@@ -5388,7 +5384,7 @@
         <v>0</v>
       </c>
       <c r="CG17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH17" s="2">
         <v>0</v>
@@ -5444,37 +5440,37 @@
         <v>73</v>
       </c>
       <c r="G18" s="1">
-        <v>44797</v>
+        <v>44871</v>
       </c>
       <c r="H18" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="I18" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="J18" s="2">
         <v>1</v>
       </c>
       <c r="K18" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N18" s="2">
         <v>0</v>
       </c>
       <c r="O18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P18" s="2">
         <v>0</v>
       </c>
       <c r="Q18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R18" s="2">
         <v>0</v>
@@ -5486,24 +5482,24 @@
         <v>0</v>
       </c>
       <c r="U18" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="V18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W18" t="s">
         <v>124</v>
       </c>
       <c r="X18" s="2"/>
-      <c r="Y18" s="2"/>
+      <c r="Y18" s="2">
+        <v>1</v>
+      </c>
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
-      <c r="AB18" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB18" s="2"/>
       <c r="AC18" s="2"/>
       <c r="AD18" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="AE18" s="2">
         <v>1</v>
@@ -5512,13 +5508,17 @@
       <c r="AG18" s="2"/>
       <c r="AH18" s="2"/>
       <c r="AI18" s="2"/>
-      <c r="AJ18" s="2"/>
-      <c r="AK18" s="2"/>
+      <c r="AJ18" s="2">
+        <v>1</v>
+      </c>
+      <c r="AK18" s="2">
+        <v>1</v>
+      </c>
       <c r="AL18" s="2"/>
       <c r="AM18" s="2"/>
       <c r="AN18" s="2"/>
       <c r="AO18" t="s">
-        <v>150</v>
+        <v>108</v>
       </c>
       <c r="AP18" t="s">
         <v>158</v>
@@ -5537,26 +5537,26 @@
         <v>1</v>
       </c>
       <c r="AV18" s="1">
-        <v>44803</v>
+        <v>44879</v>
       </c>
       <c r="AW18" s="2">
         <v>1</v>
       </c>
       <c r="AX18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY18" s="2"/>
       <c r="AZ18" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="BA18" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BB18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD18" s="2">
         <v>0</v>
@@ -5568,7 +5568,7 @@
         <v>0</v>
       </c>
       <c r="BG18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH18" s="2">
         <v>1</v>
@@ -5592,7 +5592,7 @@
         <v>0</v>
       </c>
       <c r="BO18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BP18" s="2">
         <v>0</v>
@@ -5622,7 +5622,7 @@
         <v>0</v>
       </c>
       <c r="BY18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BZ18" s="2">
         <v>0</v>
@@ -5646,7 +5646,7 @@
         <v>0</v>
       </c>
       <c r="CG18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CH18" s="2">
         <v>0</v>
@@ -5967,10 +5967,10 @@
         <v>44727</v>
       </c>
       <c r="H20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J20" s="2">
         <v>1</v>
@@ -6006,7 +6006,7 @@
         <v>0</v>
       </c>
       <c r="U20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V20" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Wednesday and Thursday results
Sorry no results yesterday. I was sick and traveling. And Sharepoint was having a sync issue but pretending it was working.
</commit_message>
<xml_diff>
--- a/datasets/analysis_dataset.xlsx
+++ b/datasets/analysis_dataset.xlsx
@@ -33,12 +33,12 @@
     <t>368</t>
   </si>
   <si>
+    <t>280</t>
+  </si>
+  <si>
     <t>424</t>
   </si>
   <si>
-    <t>280</t>
-  </si>
-  <si>
     <t>437</t>
   </si>
   <si>
@@ -51,24 +51,24 @@
     <t>193</t>
   </si>
   <si>
+    <t>253</t>
+  </si>
+  <si>
     <t>299</t>
   </si>
   <si>
-    <t>253</t>
-  </si>
-  <si>
     <t>644</t>
   </si>
   <si>
     <t>340</t>
   </si>
   <si>
+    <t>555</t>
+  </si>
+  <si>
     <t>836</t>
   </si>
   <si>
-    <t>555</t>
-  </si>
-  <si>
     <t>408</t>
   </si>
   <si>
@@ -258,12 +258,12 @@
     <t>syringe</t>
   </si>
   <si>
+    <t>pill</t>
+  </si>
+  <si>
     <t>spatula</t>
   </si>
   <si>
-    <t>pill</t>
-  </si>
-  <si>
     <t>swab</t>
   </si>
   <si>
@@ -348,12 +348,12 @@
     <t>tan</t>
   </si>
   <si>
+    <t>blue</t>
+  </si>
+  <si>
     <t>white</t>
   </si>
   <si>
-    <t>blue</t>
-  </si>
-  <si>
     <t>brown</t>
   </si>
   <si>
@@ -384,12 +384,12 @@
     <t>powder; chunky; shiny</t>
   </si>
   <si>
+    <t>crystals</t>
+  </si>
+  <si>
     <t>fake pill</t>
   </si>
   <si>
-    <t>crystals</t>
-  </si>
-  <si>
     <t>tar</t>
   </si>
   <si>
@@ -486,10 +486,10 @@
     <t>fast acting</t>
   </si>
   <si>
+    <t>FTS = negative</t>
+  </si>
+  <si>
     <t>strong blues</t>
-  </si>
-  <si>
-    <t>FTS = negative</t>
   </si>
   <si>
     <t>overdose</t>
@@ -1097,7 +1097,7 @@
         <v>125</v>
       </c>
       <c r="Y1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z1" t="s">
         <v>120</v>
@@ -1106,7 +1106,7 @@
         <v>126</v>
       </c>
       <c r="AB1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AC1" t="s">
         <v>127</v>
@@ -2713,7 +2713,7 @@
         <v>70</v>
       </c>
       <c r="G7" s="1">
-        <v>44484</v>
+        <v>44701</v>
       </c>
       <c r="H7" t="s">
         <v>81</v>
@@ -2725,13 +2725,13 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="L7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7" s="2">
         <v>0</v>
@@ -2752,22 +2752,22 @@
         <v>0</v>
       </c>
       <c r="T7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U7" t="s">
         <v>111</v>
       </c>
       <c r="V7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W7" t="s">
-        <v>120</v>
+        <v>81</v>
       </c>
       <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="2">
-        <v>1</v>
-      </c>
+      <c r="Y7" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
@@ -2788,12 +2788,14 @@
         <v>108</v>
       </c>
       <c r="AP7" t="s">
-        <v>108</v>
+        <v>155</v>
       </c>
       <c r="AQ7" t="s">
-        <v>79</v>
-      </c>
-      <c r="AR7" s="2"/>
+        <v>160</v>
+      </c>
+      <c r="AR7" s="2">
+        <v>0</v>
+      </c>
       <c r="AS7" t="s">
         <v>108</v>
       </c>
@@ -2802,32 +2804,32 @@
         <v>0</v>
       </c>
       <c r="AV7" s="1">
-        <v>44603</v>
+        <v>44721</v>
       </c>
       <c r="AW7" s="2">
         <v>1</v>
       </c>
       <c r="AX7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY7" s="2"/>
       <c r="AZ7" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="BA7" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="BB7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF7" s="2">
         <v>0</v>
@@ -2836,7 +2838,7 @@
         <v>0</v>
       </c>
       <c r="BH7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI7" s="2">
         <v>0</v>
@@ -2845,7 +2847,7 @@
         <v>0</v>
       </c>
       <c r="BK7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL7" s="2">
         <v>0</v>
@@ -2878,10 +2880,10 @@
         <v>0</v>
       </c>
       <c r="BV7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX7" s="2">
         <v>0</v>
@@ -2917,7 +2919,7 @@
         <v>0</v>
       </c>
       <c r="CI7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CJ7" s="2">
         <v>0</v>
@@ -2926,13 +2928,13 @@
         <v>0</v>
       </c>
       <c r="CL7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CM7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CN7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CO7" t="s">
         <v>47</v>
@@ -2982,7 +2984,7 @@
         <v>70</v>
       </c>
       <c r="G8" s="1">
-        <v>44701</v>
+        <v>44484</v>
       </c>
       <c r="H8" t="s">
         <v>82</v>
@@ -2994,13 +2996,13 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="L8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8" s="2">
         <v>0</v>
@@ -3021,22 +3023,22 @@
         <v>0</v>
       </c>
       <c r="T8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U8" t="s">
         <v>112</v>
       </c>
       <c r="V8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W8" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
       <c r="X8" s="2"/>
-      <c r="Y8" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2">
+        <v>1</v>
+      </c>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
@@ -3057,14 +3059,12 @@
         <v>108</v>
       </c>
       <c r="AP8" t="s">
-        <v>155</v>
+        <v>108</v>
       </c>
       <c r="AQ8" t="s">
-        <v>160</v>
-      </c>
-      <c r="AR8" s="2">
-        <v>0</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="AR8" s="2"/>
       <c r="AS8" t="s">
         <v>108</v>
       </c>
@@ -3073,32 +3073,32 @@
         <v>0</v>
       </c>
       <c r="AV8" s="1">
-        <v>44721</v>
+        <v>44603</v>
       </c>
       <c r="AW8" s="2">
         <v>1</v>
       </c>
       <c r="AX8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY8" s="2"/>
       <c r="AZ8" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="BA8" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="BB8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF8" s="2">
         <v>0</v>
@@ -3107,7 +3107,7 @@
         <v>0</v>
       </c>
       <c r="BH8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI8" s="2">
         <v>0</v>
@@ -3116,7 +3116,7 @@
         <v>0</v>
       </c>
       <c r="BK8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL8" s="2">
         <v>0</v>
@@ -3149,10 +3149,10 @@
         <v>0</v>
       </c>
       <c r="BV8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BW8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX8" s="2">
         <v>0</v>
@@ -3188,7 +3188,7 @@
         <v>0</v>
       </c>
       <c r="CI8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ8" s="2">
         <v>0</v>
@@ -3197,13 +3197,13 @@
         <v>0</v>
       </c>
       <c r="CL8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CM8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CN8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CO8" t="s">
         <v>47</v>
@@ -3566,7 +3566,7 @@
         <v>0</v>
       </c>
       <c r="U10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V10" s="2">
         <v>0</v>
@@ -4073,10 +4073,10 @@
         <v>44883</v>
       </c>
       <c r="H12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J12" s="2">
         <v>1</v>
@@ -4112,7 +4112,7 @@
         <v>0</v>
       </c>
       <c r="U12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V12" s="2">
         <v>0</v>
@@ -4351,31 +4351,31 @@
         <v>72</v>
       </c>
       <c r="G13" s="1">
-        <v>44695</v>
+        <v>44707</v>
       </c>
       <c r="H13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J13" s="2">
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="L13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N13" s="2">
         <v>0</v>
       </c>
       <c r="O13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P13" s="2">
         <v>0</v>
@@ -4384,7 +4384,7 @@
         <v>0</v>
       </c>
       <c r="R13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S13" s="2">
         <v>0</v>
@@ -4393,7 +4393,7 @@
         <v>0</v>
       </c>
       <c r="U13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="V13" s="2">
         <v>0</v>
@@ -4444,7 +4444,7 @@
         <v>0</v>
       </c>
       <c r="AV13" s="1">
-        <v>44707</v>
+        <v>44714</v>
       </c>
       <c r="AW13" s="2">
         <v>1</v>
@@ -4454,22 +4454,22 @@
       </c>
       <c r="AY13" s="2"/>
       <c r="AZ13" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="BA13" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BB13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF13" s="2">
         <v>0</v>
@@ -4481,10 +4481,10 @@
         <v>0</v>
       </c>
       <c r="BI13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK13" s="2">
         <v>0</v>
@@ -4493,7 +4493,7 @@
         <v>0</v>
       </c>
       <c r="BM13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN13" s="2">
         <v>0</v>
@@ -4520,10 +4520,10 @@
         <v>0</v>
       </c>
       <c r="BV13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX13" s="2">
         <v>0</v>
@@ -4556,19 +4556,19 @@
         <v>0</v>
       </c>
       <c r="CH13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CI13" s="2">
         <v>1</v>
       </c>
       <c r="CJ13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CK13" s="2">
         <v>0</v>
       </c>
       <c r="CL13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CM13" s="2">
         <v>0</v>
@@ -4620,31 +4620,31 @@
         <v>72</v>
       </c>
       <c r="G14" s="1">
-        <v>44707</v>
+        <v>44695</v>
       </c>
       <c r="H14" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J14" s="2">
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="L14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14" s="2">
         <v>0</v>
       </c>
       <c r="O14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P14" s="2">
         <v>0</v>
@@ -4653,7 +4653,7 @@
         <v>0</v>
       </c>
       <c r="R14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S14" s="2">
         <v>0</v>
@@ -4662,7 +4662,7 @@
         <v>0</v>
       </c>
       <c r="U14" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="V14" s="2">
         <v>0</v>
@@ -4713,7 +4713,7 @@
         <v>0</v>
       </c>
       <c r="AV14" s="1">
-        <v>44714</v>
+        <v>44707</v>
       </c>
       <c r="AW14" s="2">
         <v>1</v>
@@ -4723,22 +4723,22 @@
       </c>
       <c r="AY14" s="2"/>
       <c r="AZ14" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="BA14" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="BB14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF14" s="2">
         <v>0</v>
@@ -4750,10 +4750,10 @@
         <v>0</v>
       </c>
       <c r="BI14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK14" s="2">
         <v>0</v>
@@ -4762,7 +4762,7 @@
         <v>0</v>
       </c>
       <c r="BM14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN14" s="2">
         <v>0</v>
@@ -4789,10 +4789,10 @@
         <v>0</v>
       </c>
       <c r="BV14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BW14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX14" s="2">
         <v>0</v>
@@ -4825,19 +4825,19 @@
         <v>0</v>
       </c>
       <c r="CH14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI14" s="2">
         <v>1</v>
       </c>
       <c r="CJ14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CK14" s="2">
         <v>0</v>
       </c>
       <c r="CL14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CM14" s="2">
         <v>0</v>
@@ -4931,7 +4931,7 @@
         <v>0</v>
       </c>
       <c r="U15" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V15" s="2">
         <v>0</v>
@@ -5437,37 +5437,37 @@
         <v>73</v>
       </c>
       <c r="G17" s="1">
-        <v>44871</v>
+        <v>44797</v>
       </c>
       <c r="H17" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I17" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J17" s="2">
         <v>1</v>
       </c>
       <c r="K17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N17" s="2">
         <v>0</v>
       </c>
       <c r="O17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P17" s="2">
         <v>0</v>
       </c>
       <c r="Q17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R17" s="2">
         <v>0</v>
@@ -5479,24 +5479,24 @@
         <v>0</v>
       </c>
       <c r="U17" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="V17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W17" t="s">
         <v>123</v>
       </c>
       <c r="X17" s="2"/>
-      <c r="Y17" s="2">
-        <v>1</v>
-      </c>
+      <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
-      <c r="AB17" s="2"/>
+      <c r="AB17" s="2">
+        <v>1</v>
+      </c>
       <c r="AC17" s="2"/>
       <c r="AD17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AE17" s="2">
         <v>1</v>
@@ -5505,17 +5505,13 @@
       <c r="AG17" s="2"/>
       <c r="AH17" s="2"/>
       <c r="AI17" s="2"/>
-      <c r="AJ17" s="2">
-        <v>1</v>
-      </c>
-      <c r="AK17" s="2">
-        <v>1</v>
-      </c>
+      <c r="AJ17" s="2"/>
+      <c r="AK17" s="2"/>
       <c r="AL17" s="2"/>
       <c r="AM17" s="2"/>
       <c r="AN17" s="2"/>
       <c r="AO17" t="s">
-        <v>108</v>
+        <v>150</v>
       </c>
       <c r="AP17" t="s">
         <v>157</v>
@@ -5534,26 +5530,26 @@
         <v>1</v>
       </c>
       <c r="AV17" s="1">
-        <v>44879</v>
+        <v>44803</v>
       </c>
       <c r="AW17" s="2">
         <v>1</v>
       </c>
       <c r="AX17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY17" s="2"/>
       <c r="AZ17" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="BA17" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="BB17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD17" s="2">
         <v>0</v>
@@ -5565,7 +5561,7 @@
         <v>0</v>
       </c>
       <c r="BG17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BH17" s="2">
         <v>1</v>
@@ -5589,7 +5585,7 @@
         <v>0</v>
       </c>
       <c r="BO17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP17" s="2">
         <v>0</v>
@@ -5610,10 +5606,10 @@
         <v>0</v>
       </c>
       <c r="BV17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX17" s="2">
         <v>0</v>
@@ -5658,7 +5654,7 @@
         <v>0</v>
       </c>
       <c r="CL17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CM17" s="2">
         <v>0</v>
@@ -5714,37 +5710,37 @@
         <v>73</v>
       </c>
       <c r="G18" s="1">
-        <v>44797</v>
+        <v>44871</v>
       </c>
       <c r="H18" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I18" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="J18" s="2">
         <v>1</v>
       </c>
       <c r="K18" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N18" s="2">
         <v>0</v>
       </c>
       <c r="O18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P18" s="2">
         <v>0</v>
       </c>
       <c r="Q18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R18" s="2">
         <v>0</v>
@@ -5756,24 +5752,24 @@
         <v>0</v>
       </c>
       <c r="U18" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="V18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W18" t="s">
         <v>124</v>
       </c>
       <c r="X18" s="2"/>
-      <c r="Y18" s="2"/>
+      <c r="Y18" s="2">
+        <v>1</v>
+      </c>
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
-      <c r="AB18" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB18" s="2"/>
       <c r="AC18" s="2"/>
       <c r="AD18" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="AE18" s="2">
         <v>1</v>
@@ -5782,13 +5778,17 @@
       <c r="AG18" s="2"/>
       <c r="AH18" s="2"/>
       <c r="AI18" s="2"/>
-      <c r="AJ18" s="2"/>
-      <c r="AK18" s="2"/>
+      <c r="AJ18" s="2">
+        <v>1</v>
+      </c>
+      <c r="AK18" s="2">
+        <v>1</v>
+      </c>
       <c r="AL18" s="2"/>
       <c r="AM18" s="2"/>
       <c r="AN18" s="2"/>
       <c r="AO18" t="s">
-        <v>150</v>
+        <v>108</v>
       </c>
       <c r="AP18" t="s">
         <v>158</v>
@@ -5807,26 +5807,26 @@
         <v>1</v>
       </c>
       <c r="AV18" s="1">
-        <v>44803</v>
+        <v>44879</v>
       </c>
       <c r="AW18" s="2">
         <v>1</v>
       </c>
       <c r="AX18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY18" s="2"/>
       <c r="AZ18" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="BA18" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BB18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD18" s="2">
         <v>0</v>
@@ -5838,7 +5838,7 @@
         <v>0</v>
       </c>
       <c r="BG18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH18" s="2">
         <v>1</v>
@@ -5862,7 +5862,7 @@
         <v>0</v>
       </c>
       <c r="BO18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BP18" s="2">
         <v>0</v>
@@ -5883,10 +5883,10 @@
         <v>0</v>
       </c>
       <c r="BV18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BW18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX18" s="2">
         <v>0</v>
@@ -5931,7 +5931,7 @@
         <v>0</v>
       </c>
       <c r="CL18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CM18" s="2">
         <v>0</v>
@@ -6267,10 +6267,10 @@
         <v>44727</v>
       </c>
       <c r="H20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J20" s="2">
         <v>1</v>
@@ -6306,7 +6306,7 @@
         <v>0</v>
       </c>
       <c r="U20" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V20" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Monday results - 10,000th sample!
10,000th sample upload!!! GO @ectracy you are a star! 💫
</commit_message>
<xml_diff>
--- a/datasets/analysis_dataset.xlsx
+++ b/datasets/analysis_dataset.xlsx
@@ -51,10 +51,10 @@
     <t>193</t>
   </si>
   <si>
+    <t>299</t>
+  </si>
+  <si>
     <t>253</t>
-  </si>
-  <si>
-    <t>299</t>
   </si>
   <si>
     <t>644</t>
@@ -4351,31 +4351,31 @@
         <v>72</v>
       </c>
       <c r="G13" s="1">
-        <v>44707</v>
+        <v>44695</v>
       </c>
       <c r="H13" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I13" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J13" s="2">
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="L13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13" s="2">
         <v>0</v>
       </c>
       <c r="O13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P13" s="2">
         <v>0</v>
@@ -4384,7 +4384,7 @@
         <v>0</v>
       </c>
       <c r="R13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S13" s="2">
         <v>0</v>
@@ -4393,7 +4393,7 @@
         <v>0</v>
       </c>
       <c r="U13" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="V13" s="2">
         <v>0</v>
@@ -4444,7 +4444,7 @@
         <v>0</v>
       </c>
       <c r="AV13" s="1">
-        <v>44714</v>
+        <v>44707</v>
       </c>
       <c r="AW13" s="2">
         <v>1</v>
@@ -4454,22 +4454,22 @@
       </c>
       <c r="AY13" s="2"/>
       <c r="AZ13" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="BA13" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="BB13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF13" s="2">
         <v>0</v>
@@ -4481,10 +4481,10 @@
         <v>0</v>
       </c>
       <c r="BI13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK13" s="2">
         <v>0</v>
@@ -4493,7 +4493,7 @@
         <v>0</v>
       </c>
       <c r="BM13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN13" s="2">
         <v>0</v>
@@ -4520,10 +4520,10 @@
         <v>0</v>
       </c>
       <c r="BV13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BW13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX13" s="2">
         <v>0</v>
@@ -4556,19 +4556,19 @@
         <v>0</v>
       </c>
       <c r="CH13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI13" s="2">
         <v>1</v>
       </c>
       <c r="CJ13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CK13" s="2">
         <v>0</v>
       </c>
       <c r="CL13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CM13" s="2">
         <v>0</v>
@@ -4620,31 +4620,31 @@
         <v>72</v>
       </c>
       <c r="G14" s="1">
-        <v>44695</v>
+        <v>44707</v>
       </c>
       <c r="H14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I14" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J14" s="2">
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="L14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N14" s="2">
         <v>0</v>
       </c>
       <c r="O14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P14" s="2">
         <v>0</v>
@@ -4653,7 +4653,7 @@
         <v>0</v>
       </c>
       <c r="R14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S14" s="2">
         <v>0</v>
@@ -4662,7 +4662,7 @@
         <v>0</v>
       </c>
       <c r="U14" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="V14" s="2">
         <v>0</v>
@@ -4713,7 +4713,7 @@
         <v>0</v>
       </c>
       <c r="AV14" s="1">
-        <v>44707</v>
+        <v>44714</v>
       </c>
       <c r="AW14" s="2">
         <v>1</v>
@@ -4723,22 +4723,22 @@
       </c>
       <c r="AY14" s="2"/>
       <c r="AZ14" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="BA14" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BB14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF14" s="2">
         <v>0</v>
@@ -4750,10 +4750,10 @@
         <v>0</v>
       </c>
       <c r="BI14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK14" s="2">
         <v>0</v>
@@ -4762,7 +4762,7 @@
         <v>0</v>
       </c>
       <c r="BM14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN14" s="2">
         <v>0</v>
@@ -4789,10 +4789,10 @@
         <v>0</v>
       </c>
       <c r="BV14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX14" s="2">
         <v>0</v>
@@ -4825,19 +4825,19 @@
         <v>0</v>
       </c>
       <c r="CH14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CI14" s="2">
         <v>1</v>
       </c>
       <c r="CJ14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CK14" s="2">
         <v>0</v>
       </c>
       <c r="CL14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CM14" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Friday results. Have a good weekend!
Sorry to miss yesterday -- was out sick.
</commit_message>
<xml_diff>
--- a/datasets/analysis_dataset.xlsx
+++ b/datasets/analysis_dataset.xlsx
@@ -33,12 +33,12 @@
     <t>368</t>
   </si>
   <si>
+    <t>280</t>
+  </si>
+  <si>
     <t>424</t>
   </si>
   <si>
-    <t>280</t>
-  </si>
-  <si>
     <t>437</t>
   </si>
   <si>
@@ -51,12 +51,12 @@
     <t>193</t>
   </si>
   <si>
+    <t>299</t>
+  </si>
+  <si>
     <t>253</t>
   </si>
   <si>
-    <t>299</t>
-  </si>
-  <si>
     <t>644</t>
   </si>
   <si>
@@ -258,12 +258,12 @@
     <t>syringe</t>
   </si>
   <si>
+    <t>pill</t>
+  </si>
+  <si>
     <t>spatula</t>
   </si>
   <si>
-    <t>pill</t>
-  </si>
-  <si>
     <t>swab</t>
   </si>
   <si>
@@ -348,10 +348,10 @@
     <t>tan</t>
   </si>
   <si>
+    <t>blue</t>
+  </si>
+  <si>
     <t>white</t>
-  </si>
-  <si>
-    <t>blue</t>
   </si>
   <si>
     <t>brown</t>
@@ -1100,7 +1100,7 @@
         <v>125</v>
       </c>
       <c r="Y1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z1" t="s">
         <v>120</v>
@@ -2732,7 +2732,7 @@
         <v>70</v>
       </c>
       <c r="G7" s="1">
-        <v>44484</v>
+        <v>44701</v>
       </c>
       <c r="H7" t="s">
         <v>81</v>
@@ -2744,13 +2744,13 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="L7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7" s="2">
         <v>0</v>
@@ -2771,22 +2771,22 @@
         <v>0</v>
       </c>
       <c r="T7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U7" t="s">
         <v>111</v>
       </c>
       <c r="V7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W7" t="s">
-        <v>120</v>
+        <v>81</v>
       </c>
       <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="2">
-        <v>1</v>
-      </c>
+      <c r="Y7" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
@@ -2807,12 +2807,14 @@
         <v>108</v>
       </c>
       <c r="AP7" t="s">
-        <v>108</v>
+        <v>155</v>
       </c>
       <c r="AQ7" t="s">
-        <v>79</v>
-      </c>
-      <c r="AR7" s="2"/>
+        <v>160</v>
+      </c>
+      <c r="AR7" s="2">
+        <v>0</v>
+      </c>
       <c r="AS7" t="s">
         <v>108</v>
       </c>
@@ -2821,35 +2823,35 @@
         <v>0</v>
       </c>
       <c r="AV7" s="1">
-        <v>44603</v>
+        <v>44721</v>
       </c>
       <c r="AW7" s="2">
         <v>1</v>
       </c>
       <c r="AX7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY7" s="2">
-        <v>11.399999618530273</v>
+        <v>6.3899998664855957</v>
       </c>
       <c r="AZ7" s="2"/>
       <c r="BA7" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="BB7" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="BC7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG7" s="2">
         <v>0</v>
@@ -2858,7 +2860,7 @@
         <v>0</v>
       </c>
       <c r="BI7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ7" s="2">
         <v>0</v>
@@ -2867,7 +2869,7 @@
         <v>0</v>
       </c>
       <c r="BL7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BM7" s="2">
         <v>0</v>
@@ -2900,10 +2902,10 @@
         <v>0</v>
       </c>
       <c r="BW7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY7" s="2">
         <v>0</v>
@@ -2939,7 +2941,7 @@
         <v>0</v>
       </c>
       <c r="CJ7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CK7" s="2">
         <v>0</v>
@@ -2948,13 +2950,13 @@
         <v>0</v>
       </c>
       <c r="CM7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CN7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CO7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CP7" t="s">
         <v>47</v>
@@ -3004,7 +3006,7 @@
         <v>70</v>
       </c>
       <c r="G8" s="1">
-        <v>44701</v>
+        <v>44484</v>
       </c>
       <c r="H8" t="s">
         <v>82</v>
@@ -3016,13 +3018,13 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="L8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8" s="2">
         <v>0</v>
@@ -3043,22 +3045,22 @@
         <v>0</v>
       </c>
       <c r="T8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U8" t="s">
         <v>112</v>
       </c>
       <c r="V8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W8" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
       <c r="X8" s="2"/>
-      <c r="Y8" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2">
+        <v>1</v>
+      </c>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
@@ -3079,14 +3081,12 @@
         <v>108</v>
       </c>
       <c r="AP8" t="s">
-        <v>155</v>
+        <v>108</v>
       </c>
       <c r="AQ8" t="s">
-        <v>160</v>
-      </c>
-      <c r="AR8" s="2">
-        <v>0</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="AR8" s="2"/>
       <c r="AS8" t="s">
         <v>108</v>
       </c>
@@ -3095,35 +3095,35 @@
         <v>0</v>
       </c>
       <c r="AV8" s="1">
-        <v>44721</v>
+        <v>44603</v>
       </c>
       <c r="AW8" s="2">
         <v>1</v>
       </c>
       <c r="AX8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY8" s="2">
-        <v>6.3899998664855957</v>
+        <v>11.399999618530273</v>
       </c>
       <c r="AZ8" s="2"/>
       <c r="BA8" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="BB8" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="BC8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG8" s="2">
         <v>0</v>
@@ -3132,7 +3132,7 @@
         <v>0</v>
       </c>
       <c r="BI8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ8" s="2">
         <v>0</v>
@@ -3141,7 +3141,7 @@
         <v>0</v>
       </c>
       <c r="BL8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM8" s="2">
         <v>0</v>
@@ -3174,10 +3174,10 @@
         <v>0</v>
       </c>
       <c r="BW8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BY8" s="2">
         <v>0</v>
@@ -3213,7 +3213,7 @@
         <v>0</v>
       </c>
       <c r="CJ8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CK8" s="2">
         <v>0</v>
@@ -3222,13 +3222,13 @@
         <v>0</v>
       </c>
       <c r="CM8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CN8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CO8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CP8" t="s">
         <v>47</v>
@@ -3594,7 +3594,7 @@
         <v>0</v>
       </c>
       <c r="U10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V10" s="2">
         <v>0</v>
@@ -4107,10 +4107,10 @@
         <v>44883</v>
       </c>
       <c r="H12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J12" s="2">
         <v>1</v>
@@ -4146,7 +4146,7 @@
         <v>0</v>
       </c>
       <c r="U12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V12" s="2">
         <v>0</v>
@@ -4388,31 +4388,31 @@
         <v>72</v>
       </c>
       <c r="G13" s="1">
-        <v>44707</v>
+        <v>44695</v>
       </c>
       <c r="H13" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I13" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J13" s="2">
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="L13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13" s="2">
         <v>0</v>
       </c>
       <c r="O13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P13" s="2">
         <v>0</v>
@@ -4421,7 +4421,7 @@
         <v>0</v>
       </c>
       <c r="R13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S13" s="2">
         <v>0</v>
@@ -4430,7 +4430,7 @@
         <v>0</v>
       </c>
       <c r="U13" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="V13" s="2">
         <v>0</v>
@@ -4481,7 +4481,7 @@
         <v>0</v>
       </c>
       <c r="AV13" s="1">
-        <v>44714</v>
+        <v>44707</v>
       </c>
       <c r="AW13" s="2">
         <v>1</v>
@@ -4490,26 +4490,26 @@
         <v>1</v>
       </c>
       <c r="AY13" s="2">
-        <v>7.630000114440918</v>
+        <v>9.2399997711181641</v>
       </c>
       <c r="AZ13" s="2"/>
       <c r="BA13" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="BB13" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="BC13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG13" s="2">
         <v>0</v>
@@ -4521,10 +4521,10 @@
         <v>0</v>
       </c>
       <c r="BJ13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL13" s="2">
         <v>0</v>
@@ -4533,7 +4533,7 @@
         <v>0</v>
       </c>
       <c r="BN13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO13" s="2">
         <v>0</v>
@@ -4560,10 +4560,10 @@
         <v>0</v>
       </c>
       <c r="BW13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BY13" s="2">
         <v>0</v>
@@ -4596,19 +4596,19 @@
         <v>0</v>
       </c>
       <c r="CI13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ13" s="2">
         <v>1</v>
       </c>
       <c r="CK13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CL13" s="2">
         <v>0</v>
       </c>
       <c r="CM13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CN13" s="2">
         <v>0</v>
@@ -4660,31 +4660,31 @@
         <v>72</v>
       </c>
       <c r="G14" s="1">
-        <v>44695</v>
+        <v>44707</v>
       </c>
       <c r="H14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I14" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J14" s="2">
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="L14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N14" s="2">
         <v>0</v>
       </c>
       <c r="O14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P14" s="2">
         <v>0</v>
@@ -4693,7 +4693,7 @@
         <v>0</v>
       </c>
       <c r="R14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S14" s="2">
         <v>0</v>
@@ -4702,7 +4702,7 @@
         <v>0</v>
       </c>
       <c r="U14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="V14" s="2">
         <v>0</v>
@@ -4753,7 +4753,7 @@
         <v>0</v>
       </c>
       <c r="AV14" s="1">
-        <v>44707</v>
+        <v>44714</v>
       </c>
       <c r="AW14" s="2">
         <v>1</v>
@@ -4762,26 +4762,26 @@
         <v>1</v>
       </c>
       <c r="AY14" s="2">
-        <v>9.2399997711181641</v>
+        <v>7.630000114440918</v>
       </c>
       <c r="AZ14" s="2"/>
       <c r="BA14" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="BB14" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BC14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG14" s="2">
         <v>0</v>
@@ -4793,10 +4793,10 @@
         <v>0</v>
       </c>
       <c r="BJ14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL14" s="2">
         <v>0</v>
@@ -4805,7 +4805,7 @@
         <v>0</v>
       </c>
       <c r="BN14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BO14" s="2">
         <v>0</v>
@@ -4832,10 +4832,10 @@
         <v>0</v>
       </c>
       <c r="BW14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY14" s="2">
         <v>0</v>
@@ -4868,19 +4868,19 @@
         <v>0</v>
       </c>
       <c r="CI14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CJ14" s="2">
         <v>1</v>
       </c>
       <c r="CK14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CL14" s="2">
         <v>0</v>
       </c>
       <c r="CM14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CN14" s="2">
         <v>0</v>
@@ -4974,7 +4974,7 @@
         <v>0</v>
       </c>
       <c r="U15" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V15" s="2">
         <v>0</v>
@@ -5489,10 +5489,10 @@
         <v>44871</v>
       </c>
       <c r="H17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J17" s="2">
         <v>1</v>
@@ -5528,7 +5528,7 @@
         <v>0</v>
       </c>
       <c r="U17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V17" s="2">
         <v>1</v>
@@ -6325,10 +6325,10 @@
         <v>44727</v>
       </c>
       <c r="H20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J20" s="2">
         <v>1</v>
@@ -6364,7 +6364,7 @@
         <v>0</v>
       </c>
       <c r="U20" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V20" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Monday results (sorry for the delay)
Sorry for the delay during the Int'l Harm Reduction Conference
</commit_message>
<xml_diff>
--- a/datasets/analysis_dataset.xlsx
+++ b/datasets/analysis_dataset.xlsx
@@ -51,10 +51,10 @@
     <t>193</t>
   </si>
   <si>
+    <t>253</t>
+  </si>
+  <si>
     <t>299</t>
-  </si>
-  <si>
-    <t>253</t>
   </si>
   <si>
     <t>644</t>
@@ -4388,31 +4388,31 @@
         <v>72</v>
       </c>
       <c r="G13" s="1">
-        <v>44695</v>
+        <v>44707</v>
       </c>
       <c r="H13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J13" s="2">
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="L13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N13" s="2">
         <v>0</v>
       </c>
       <c r="O13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P13" s="2">
         <v>0</v>
@@ -4421,7 +4421,7 @@
         <v>0</v>
       </c>
       <c r="R13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S13" s="2">
         <v>0</v>
@@ -4430,7 +4430,7 @@
         <v>0</v>
       </c>
       <c r="U13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="V13" s="2">
         <v>0</v>
@@ -4481,7 +4481,7 @@
         <v>0</v>
       </c>
       <c r="AV13" s="1">
-        <v>44707</v>
+        <v>44714</v>
       </c>
       <c r="AW13" s="2">
         <v>1</v>
@@ -4490,26 +4490,26 @@
         <v>1</v>
       </c>
       <c r="AY13" s="2">
-        <v>9.2399997711181641</v>
+        <v>7.630000114440918</v>
       </c>
       <c r="AZ13" s="2"/>
       <c r="BA13" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="BB13" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BC13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG13" s="2">
         <v>0</v>
@@ -4521,10 +4521,10 @@
         <v>0</v>
       </c>
       <c r="BJ13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL13" s="2">
         <v>0</v>
@@ -4533,7 +4533,7 @@
         <v>0</v>
       </c>
       <c r="BN13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BO13" s="2">
         <v>0</v>
@@ -4560,10 +4560,10 @@
         <v>0</v>
       </c>
       <c r="BW13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY13" s="2">
         <v>0</v>
@@ -4596,19 +4596,19 @@
         <v>0</v>
       </c>
       <c r="CI13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CJ13" s="2">
         <v>1</v>
       </c>
       <c r="CK13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CL13" s="2">
         <v>0</v>
       </c>
       <c r="CM13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CN13" s="2">
         <v>0</v>
@@ -4660,31 +4660,31 @@
         <v>72</v>
       </c>
       <c r="G14" s="1">
-        <v>44707</v>
+        <v>44695</v>
       </c>
       <c r="H14" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J14" s="2">
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="L14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14" s="2">
         <v>0</v>
       </c>
       <c r="O14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P14" s="2">
         <v>0</v>
@@ -4693,7 +4693,7 @@
         <v>0</v>
       </c>
       <c r="R14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S14" s="2">
         <v>0</v>
@@ -4702,7 +4702,7 @@
         <v>0</v>
       </c>
       <c r="U14" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="V14" s="2">
         <v>0</v>
@@ -4753,7 +4753,7 @@
         <v>0</v>
       </c>
       <c r="AV14" s="1">
-        <v>44714</v>
+        <v>44707</v>
       </c>
       <c r="AW14" s="2">
         <v>1</v>
@@ -4762,26 +4762,26 @@
         <v>1</v>
       </c>
       <c r="AY14" s="2">
-        <v>7.630000114440918</v>
+        <v>9.2399997711181641</v>
       </c>
       <c r="AZ14" s="2"/>
       <c r="BA14" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="BB14" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="BC14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG14" s="2">
         <v>0</v>
@@ -4793,10 +4793,10 @@
         <v>0</v>
       </c>
       <c r="BJ14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL14" s="2">
         <v>0</v>
@@ -4805,7 +4805,7 @@
         <v>0</v>
       </c>
       <c r="BN14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO14" s="2">
         <v>0</v>
@@ -4832,10 +4832,10 @@
         <v>0</v>
       </c>
       <c r="BW14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BY14" s="2">
         <v>0</v>
@@ -4868,19 +4868,19 @@
         <v>0</v>
       </c>
       <c r="CI14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ14" s="2">
         <v>1</v>
       </c>
       <c r="CK14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CL14" s="2">
         <v>0</v>
       </c>
       <c r="CM14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CN14" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Thursday and Friday morning results
</commit_message>
<xml_diff>
--- a/datasets/analysis_dataset.xlsx
+++ b/datasets/analysis_dataset.xlsx
@@ -51,10 +51,10 @@
     <t>193</t>
   </si>
   <si>
+    <t>253</t>
+  </si>
+  <si>
     <t>299</t>
-  </si>
-  <si>
-    <t>253</t>
   </si>
   <si>
     <t>644</t>
@@ -4388,31 +4388,31 @@
         <v>72</v>
       </c>
       <c r="G13" s="1">
-        <v>44695</v>
+        <v>44707</v>
       </c>
       <c r="H13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J13" s="2">
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="L13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N13" s="2">
         <v>0</v>
       </c>
       <c r="O13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P13" s="2">
         <v>0</v>
@@ -4421,7 +4421,7 @@
         <v>0</v>
       </c>
       <c r="R13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S13" s="2">
         <v>0</v>
@@ -4430,7 +4430,7 @@
         <v>0</v>
       </c>
       <c r="U13" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="V13" s="2">
         <v>0</v>
@@ -4481,7 +4481,7 @@
         <v>0</v>
       </c>
       <c r="AV13" s="1">
-        <v>44707</v>
+        <v>44714</v>
       </c>
       <c r="AW13" s="2">
         <v>1</v>
@@ -4490,26 +4490,26 @@
         <v>1</v>
       </c>
       <c r="AY13" s="2">
-        <v>9.2399997711181641</v>
+        <v>7.630000114440918</v>
       </c>
       <c r="AZ13" s="2"/>
       <c r="BA13" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="BB13" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BC13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG13" s="2">
         <v>0</v>
@@ -4521,10 +4521,10 @@
         <v>0</v>
       </c>
       <c r="BJ13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL13" s="2">
         <v>0</v>
@@ -4533,7 +4533,7 @@
         <v>0</v>
       </c>
       <c r="BN13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BO13" s="2">
         <v>0</v>
@@ -4560,10 +4560,10 @@
         <v>0</v>
       </c>
       <c r="BW13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY13" s="2">
         <v>0</v>
@@ -4596,19 +4596,19 @@
         <v>0</v>
       </c>
       <c r="CI13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CJ13" s="2">
         <v>1</v>
       </c>
       <c r="CK13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CL13" s="2">
         <v>0</v>
       </c>
       <c r="CM13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CN13" s="2">
         <v>0</v>
@@ -4660,31 +4660,31 @@
         <v>72</v>
       </c>
       <c r="G14" s="1">
-        <v>44707</v>
+        <v>44695</v>
       </c>
       <c r="H14" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J14" s="2">
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="L14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14" s="2">
         <v>0</v>
       </c>
       <c r="O14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P14" s="2">
         <v>0</v>
@@ -4693,7 +4693,7 @@
         <v>0</v>
       </c>
       <c r="R14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S14" s="2">
         <v>0</v>
@@ -4702,7 +4702,7 @@
         <v>0</v>
       </c>
       <c r="U14" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="V14" s="2">
         <v>0</v>
@@ -4753,7 +4753,7 @@
         <v>0</v>
       </c>
       <c r="AV14" s="1">
-        <v>44714</v>
+        <v>44707</v>
       </c>
       <c r="AW14" s="2">
         <v>1</v>
@@ -4762,26 +4762,26 @@
         <v>1</v>
       </c>
       <c r="AY14" s="2">
-        <v>7.630000114440918</v>
+        <v>9.2399997711181641</v>
       </c>
       <c r="AZ14" s="2"/>
       <c r="BA14" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="BB14" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="BC14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG14" s="2">
         <v>0</v>
@@ -4793,10 +4793,10 @@
         <v>0</v>
       </c>
       <c r="BJ14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL14" s="2">
         <v>0</v>
@@ -4805,7 +4805,7 @@
         <v>0</v>
       </c>
       <c r="BN14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO14" s="2">
         <v>0</v>
@@ -4832,10 +4832,10 @@
         <v>0</v>
       </c>
       <c r="BW14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BY14" s="2">
         <v>0</v>
@@ -4868,19 +4868,19 @@
         <v>0</v>
       </c>
       <c r="CI14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ14" s="2">
         <v>1</v>
       </c>
       <c r="CK14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CL14" s="2">
         <v>0</v>
       </c>
       <c r="CM14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CN14" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Monday and Tuesday results
</commit_message>
<xml_diff>
--- a/datasets/analysis_dataset.xlsx
+++ b/datasets/analysis_dataset.xlsx
@@ -33,12 +33,12 @@
     <t>368</t>
   </si>
   <si>
+    <t>424</t>
+  </si>
+  <si>
     <t>280</t>
   </si>
   <si>
-    <t>424</t>
-  </si>
-  <si>
     <t>437</t>
   </si>
   <si>
@@ -51,12 +51,12 @@
     <t>193</t>
   </si>
   <si>
+    <t>253</t>
+  </si>
+  <si>
     <t>299</t>
   </si>
   <si>
-    <t>253</t>
-  </si>
-  <si>
     <t>644</t>
   </si>
   <si>
@@ -258,12 +258,12 @@
     <t>syringe</t>
   </si>
   <si>
+    <t>spatula</t>
+  </si>
+  <si>
     <t>pill</t>
   </si>
   <si>
-    <t>spatula</t>
-  </si>
-  <si>
     <t>swab</t>
   </si>
   <si>
@@ -348,10 +348,10 @@
     <t>tan</t>
   </si>
   <si>
+    <t>white</t>
+  </si>
+  <si>
     <t>blue</t>
-  </si>
-  <si>
-    <t>white</t>
   </si>
   <si>
     <t>brown</t>
@@ -1100,7 +1100,7 @@
         <v>125</v>
       </c>
       <c r="Y1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="Z1" t="s">
         <v>120</v>
@@ -2732,7 +2732,7 @@
         <v>70</v>
       </c>
       <c r="G7" s="1">
-        <v>44701</v>
+        <v>44484</v>
       </c>
       <c r="H7" t="s">
         <v>81</v>
@@ -2744,13 +2744,13 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="L7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7" s="2">
         <v>0</v>
@@ -2771,22 +2771,22 @@
         <v>0</v>
       </c>
       <c r="T7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U7" t="s">
         <v>111</v>
       </c>
       <c r="V7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W7" t="s">
-        <v>81</v>
+        <v>120</v>
       </c>
       <c r="X7" s="2"/>
-      <c r="Y7" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2">
+        <v>1</v>
+      </c>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
@@ -2807,14 +2807,12 @@
         <v>108</v>
       </c>
       <c r="AP7" t="s">
-        <v>155</v>
+        <v>108</v>
       </c>
       <c r="AQ7" t="s">
-        <v>160</v>
-      </c>
-      <c r="AR7" s="2">
-        <v>0</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="AR7" s="2"/>
       <c r="AS7" t="s">
         <v>108</v>
       </c>
@@ -2823,35 +2821,35 @@
         <v>0</v>
       </c>
       <c r="AV7" s="1">
-        <v>44721</v>
+        <v>44603</v>
       </c>
       <c r="AW7" s="2">
         <v>1</v>
       </c>
       <c r="AX7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY7" s="2">
-        <v>6.3899998664855957</v>
+        <v>11.399999618530273</v>
       </c>
       <c r="AZ7" s="2"/>
       <c r="BA7" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="BB7" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="BC7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG7" s="2">
         <v>0</v>
@@ -2860,7 +2858,7 @@
         <v>0</v>
       </c>
       <c r="BI7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ7" s="2">
         <v>0</v>
@@ -2869,7 +2867,7 @@
         <v>0</v>
       </c>
       <c r="BL7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM7" s="2">
         <v>0</v>
@@ -2902,10 +2900,10 @@
         <v>0</v>
       </c>
       <c r="BW7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BY7" s="2">
         <v>0</v>
@@ -2941,7 +2939,7 @@
         <v>0</v>
       </c>
       <c r="CJ7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CK7" s="2">
         <v>0</v>
@@ -2950,13 +2948,13 @@
         <v>0</v>
       </c>
       <c r="CM7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CN7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CO7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CP7" t="s">
         <v>47</v>
@@ -3006,7 +3004,7 @@
         <v>70</v>
       </c>
       <c r="G8" s="1">
-        <v>44484</v>
+        <v>44701</v>
       </c>
       <c r="H8" t="s">
         <v>82</v>
@@ -3018,13 +3016,13 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="L8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8" s="2">
         <v>0</v>
@@ -3045,22 +3043,22 @@
         <v>0</v>
       </c>
       <c r="T8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8" t="s">
         <v>112</v>
       </c>
       <c r="V8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W8" t="s">
-        <v>120</v>
+        <v>82</v>
       </c>
       <c r="X8" s="2"/>
-      <c r="Y8" s="2"/>
-      <c r="Z8" s="2">
-        <v>1</v>
-      </c>
+      <c r="Y8" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
@@ -3081,12 +3079,14 @@
         <v>108</v>
       </c>
       <c r="AP8" t="s">
-        <v>108</v>
+        <v>155</v>
       </c>
       <c r="AQ8" t="s">
-        <v>79</v>
-      </c>
-      <c r="AR8" s="2"/>
+        <v>160</v>
+      </c>
+      <c r="AR8" s="2">
+        <v>0</v>
+      </c>
       <c r="AS8" t="s">
         <v>108</v>
       </c>
@@ -3095,35 +3095,35 @@
         <v>0</v>
       </c>
       <c r="AV8" s="1">
-        <v>44603</v>
+        <v>44721</v>
       </c>
       <c r="AW8" s="2">
         <v>1</v>
       </c>
       <c r="AX8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY8" s="2">
-        <v>11.399999618530273</v>
+        <v>6.3899998664855957</v>
       </c>
       <c r="AZ8" s="2"/>
       <c r="BA8" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="BB8" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="BC8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG8" s="2">
         <v>0</v>
@@ -3132,7 +3132,7 @@
         <v>0</v>
       </c>
       <c r="BI8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ8" s="2">
         <v>0</v>
@@ -3141,7 +3141,7 @@
         <v>0</v>
       </c>
       <c r="BL8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BM8" s="2">
         <v>0</v>
@@ -3174,10 +3174,10 @@
         <v>0</v>
       </c>
       <c r="BW8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY8" s="2">
         <v>0</v>
@@ -3213,7 +3213,7 @@
         <v>0</v>
       </c>
       <c r="CJ8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CK8" s="2">
         <v>0</v>
@@ -3222,13 +3222,13 @@
         <v>0</v>
       </c>
       <c r="CM8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CN8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CO8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CP8" t="s">
         <v>47</v>
@@ -3594,7 +3594,7 @@
         <v>0</v>
       </c>
       <c r="U10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V10" s="2">
         <v>0</v>
@@ -4107,10 +4107,10 @@
         <v>44883</v>
       </c>
       <c r="H12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J12" s="2">
         <v>1</v>
@@ -4146,7 +4146,7 @@
         <v>0</v>
       </c>
       <c r="U12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V12" s="2">
         <v>0</v>
@@ -4388,31 +4388,31 @@
         <v>72</v>
       </c>
       <c r="G13" s="1">
-        <v>44695</v>
+        <v>44707</v>
       </c>
       <c r="H13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J13" s="2">
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="L13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N13" s="2">
         <v>0</v>
       </c>
       <c r="O13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P13" s="2">
         <v>0</v>
@@ -4421,7 +4421,7 @@
         <v>0</v>
       </c>
       <c r="R13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S13" s="2">
         <v>0</v>
@@ -4430,7 +4430,7 @@
         <v>0</v>
       </c>
       <c r="U13" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="V13" s="2">
         <v>0</v>
@@ -4481,7 +4481,7 @@
         <v>0</v>
       </c>
       <c r="AV13" s="1">
-        <v>44707</v>
+        <v>44714</v>
       </c>
       <c r="AW13" s="2">
         <v>1</v>
@@ -4490,26 +4490,26 @@
         <v>1</v>
       </c>
       <c r="AY13" s="2">
-        <v>9.2399997711181641</v>
+        <v>7.630000114440918</v>
       </c>
       <c r="AZ13" s="2"/>
       <c r="BA13" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="BB13" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="BC13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG13" s="2">
         <v>0</v>
@@ -4521,10 +4521,10 @@
         <v>0</v>
       </c>
       <c r="BJ13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL13" s="2">
         <v>0</v>
@@ -4533,7 +4533,7 @@
         <v>0</v>
       </c>
       <c r="BN13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BO13" s="2">
         <v>0</v>
@@ -4560,10 +4560,10 @@
         <v>0</v>
       </c>
       <c r="BW13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY13" s="2">
         <v>0</v>
@@ -4596,19 +4596,19 @@
         <v>0</v>
       </c>
       <c r="CI13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CJ13" s="2">
         <v>1</v>
       </c>
       <c r="CK13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CL13" s="2">
         <v>0</v>
       </c>
       <c r="CM13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CN13" s="2">
         <v>0</v>
@@ -4660,31 +4660,31 @@
         <v>72</v>
       </c>
       <c r="G14" s="1">
-        <v>44707</v>
+        <v>44695</v>
       </c>
       <c r="H14" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J14" s="2">
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="L14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14" s="2">
         <v>0</v>
       </c>
       <c r="O14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P14" s="2">
         <v>0</v>
@@ -4693,7 +4693,7 @@
         <v>0</v>
       </c>
       <c r="R14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S14" s="2">
         <v>0</v>
@@ -4702,7 +4702,7 @@
         <v>0</v>
       </c>
       <c r="U14" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="V14" s="2">
         <v>0</v>
@@ -4753,7 +4753,7 @@
         <v>0</v>
       </c>
       <c r="AV14" s="1">
-        <v>44714</v>
+        <v>44707</v>
       </c>
       <c r="AW14" s="2">
         <v>1</v>
@@ -4762,26 +4762,26 @@
         <v>1</v>
       </c>
       <c r="AY14" s="2">
-        <v>7.630000114440918</v>
+        <v>9.2399997711181641</v>
       </c>
       <c r="AZ14" s="2"/>
       <c r="BA14" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="BB14" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="BC14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG14" s="2">
         <v>0</v>
@@ -4793,10 +4793,10 @@
         <v>0</v>
       </c>
       <c r="BJ14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL14" s="2">
         <v>0</v>
@@ -4805,7 +4805,7 @@
         <v>0</v>
       </c>
       <c r="BN14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO14" s="2">
         <v>0</v>
@@ -4832,10 +4832,10 @@
         <v>0</v>
       </c>
       <c r="BW14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BY14" s="2">
         <v>0</v>
@@ -4868,19 +4868,19 @@
         <v>0</v>
       </c>
       <c r="CI14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ14" s="2">
         <v>1</v>
       </c>
       <c r="CK14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CL14" s="2">
         <v>0</v>
       </c>
       <c r="CM14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CN14" s="2">
         <v>0</v>
@@ -4974,7 +4974,7 @@
         <v>0</v>
       </c>
       <c r="U15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V15" s="2">
         <v>0</v>
@@ -5765,10 +5765,10 @@
         <v>44871</v>
       </c>
       <c r="H18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J18" s="2">
         <v>1</v>
@@ -5804,7 +5804,7 @@
         <v>0</v>
       </c>
       <c r="U18" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V18" s="2">
         <v>1</v>
@@ -6325,10 +6325,10 @@
         <v>44727</v>
       </c>
       <c r="H20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J20" s="2">
         <v>1</v>
@@ -6364,7 +6364,7 @@
         <v>0</v>
       </c>
       <c r="U20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V20" s="2">
         <v>0</v>

</xml_diff>